<commit_message>
Sieve of Eratosthenes (Program to find all prime numbers below given number) Added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519DF654-7717-4163-8D55-725822207383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B215F87-CCBB-427A-8723-39DCF5163E03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="509">
   <si>
     <t>Topic:</t>
   </si>
@@ -1549,6 +1549,9 @@
   </si>
   <si>
     <t>DGN0MATH</t>
+  </si>
+  <si>
+    <t>PAPN0MATH</t>
   </si>
 </sst>
 </file>
@@ -2020,7 +2023,7 @@
   <dimension ref="A1:F501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2268,14 +2271,12 @@
         <v>474</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>472</v>
-      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="9" t="s">

</xml_diff>

<commit_message>
Kth largest element program moved to Searching & Sorting
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0FC137-768A-44EE-9E7F-03462B584564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD2FB50-E0EB-4651-88CF-6C6E23911B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="511">
   <si>
     <t>Topic:</t>
   </si>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2345,28 +2345,30 @@
       <c r="C24" s="11" t="s">
         <v>502</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="4" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>466</v>
+        <v>8</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
@@ -2374,10 +2376,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>3</v>
@@ -2388,10 +2390,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>3</v>
@@ -2402,10 +2404,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>3</v>
@@ -2415,11 +2417,9 @@
       <c r="A30" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>510</v>
-      </c>
+      <c r="B30" s="10"/>
       <c r="C30" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>3</v>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>3</v>
@@ -2443,7 +2443,7 @@
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>3</v>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>3</v>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>3</v>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>3</v>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>3</v>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>3</v>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>3</v>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>3</v>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>3</v>
@@ -2551,7 +2551,7 @@
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>3</v>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>3</v>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>3</v>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>3</v>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>3</v>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>3</v>
@@ -2623,7 +2623,7 @@
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>3</v>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>3</v>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>3</v>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>3</v>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>3</v>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>3</v>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>3</v>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>3</v>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>3</v>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>3</v>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>3</v>
@@ -2755,32 +2755,32 @@
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A59" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="10"/>
-      <c r="C59" s="11" t="s">
-        <v>40</v>
-      </c>
       <c r="D59" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
       <c r="D60" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
+      <c r="A61" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D61" s="8" t="s">
         <v>3</v>
       </c>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>3</v>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>3</v>
@@ -2815,7 +2815,7 @@
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>3</v>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>3</v>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>3</v>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>3</v>
@@ -2863,7 +2863,7 @@
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>3</v>
@@ -2875,7 +2875,7 @@
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>3</v>
@@ -2887,28 +2887,28 @@
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A71" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>3</v>
-      </c>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A73" s="10"/>
+      <c r="A73" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="B73" s="10"/>
-      <c r="D73" s="8"/>
+      <c r="C73" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="10" t="s">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>3</v>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>3</v>
@@ -2939,8 +2939,8 @@
         <v>52</v>
       </c>
       <c r="B76" s="10"/>
-      <c r="C76" s="11" t="s">
-        <v>55</v>
+      <c r="C76" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>3</v>
@@ -2951,8 +2951,8 @@
         <v>52</v>
       </c>
       <c r="B77" s="10"/>
-      <c r="C77" s="6" t="s">
-        <v>56</v>
+      <c r="C77" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>3</v>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>3</v>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>3</v>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>3</v>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>3</v>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>3</v>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>3</v>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>3</v>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>3</v>
@@ -3060,7 +3060,7 @@
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>3</v>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>3</v>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>3</v>
@@ -3096,7 +3096,7 @@
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>3</v>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>3</v>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="B91" s="10"/>
       <c r="C91" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>3</v>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>3</v>
@@ -3144,7 +3144,7 @@
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>3</v>
@@ -3156,7 +3156,7 @@
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>3</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>3</v>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>3</v>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>3</v>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>3</v>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>3</v>
@@ -3228,7 +3228,7 @@
       </c>
       <c r="B100" s="10"/>
       <c r="C100" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>3</v>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>3</v>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="B102" s="10"/>
       <c r="C102" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>3</v>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="B103" s="10"/>
       <c r="C103" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>3</v>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="B104" s="10"/>
       <c r="C104" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>3</v>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>3</v>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="B106" s="10"/>
       <c r="C106" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>3</v>
@@ -3312,7 +3312,7 @@
       </c>
       <c r="B107" s="10"/>
       <c r="C107" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>3</v>
@@ -3324,7 +3324,7 @@
       </c>
       <c r="B108" s="10"/>
       <c r="C108" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>3</v>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="B109" s="10"/>
       <c r="C109" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>3</v>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="B110" s="10"/>
       <c r="C110" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>3</v>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="B111" s="10"/>
       <c r="C111" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>3</v>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="B112" s="10"/>
       <c r="C112" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>3</v>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="B113" s="10"/>
       <c r="C113" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>3</v>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="B114" s="10"/>
       <c r="C114" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>3</v>
@@ -3408,28 +3408,28 @@
       </c>
       <c r="B115" s="10"/>
       <c r="C115" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A116" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B116" s="10"/>
-      <c r="C116" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>3</v>
-      </c>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="D117" s="8"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A118" s="8"/>
-      <c r="B118" s="8"/>
-      <c r="D118" s="8"/>
+      <c r="A118" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B118" s="10"/>
+      <c r="C118" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" s="10" t="s">
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B119" s="10"/>
       <c r="C119" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>3</v>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="B120" s="10"/>
       <c r="C120" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>3</v>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="B121" s="10"/>
       <c r="C121" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>3</v>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="B122" s="10"/>
       <c r="C122" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>3</v>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="B123" s="10"/>
       <c r="C123" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>3</v>
@@ -3497,7 +3497,7 @@
       </c>
       <c r="B124" s="10"/>
       <c r="C124" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>3</v>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="B125" s="10"/>
       <c r="C125" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>3</v>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="B126" s="10"/>
       <c r="C126" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>3</v>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="B127" s="10"/>
       <c r="C127" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D127" s="8" t="s">
         <v>3</v>
@@ -3545,7 +3545,7 @@
       </c>
       <c r="B128" s="10"/>
       <c r="C128" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>3</v>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="B129" s="10"/>
       <c r="C129" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>3</v>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="B130" s="10"/>
       <c r="C130" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>3</v>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B131" s="10"/>
       <c r="C131" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>3</v>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="B132" s="10"/>
       <c r="C132" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>3</v>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="B133" s="10"/>
       <c r="C133" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D133" s="8" t="s">
         <v>3</v>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="B134" s="10"/>
       <c r="C134" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D134" s="8" t="s">
         <v>3</v>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="B135" s="10"/>
       <c r="C135" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D135" s="8" t="s">
         <v>3</v>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B136" s="10"/>
       <c r="C136" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D136" s="8" t="s">
         <v>3</v>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="B137" s="10"/>
       <c r="C137" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D137" s="8" t="s">
         <v>3</v>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="B138" s="10"/>
       <c r="C138" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D138" s="8" t="s">
         <v>3</v>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B139" s="10"/>
       <c r="C139" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D139" s="8" t="s">
         <v>3</v>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="B140" s="10"/>
       <c r="C140" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D140" s="8" t="s">
         <v>3</v>
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B141" s="10"/>
       <c r="C141" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D141" s="8" t="s">
         <v>3</v>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="B142" s="10"/>
       <c r="C142" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>3</v>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="B143" s="10"/>
       <c r="C143" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D143" s="8" t="s">
         <v>3</v>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="B144" s="10"/>
       <c r="C144" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D144" s="8" t="s">
         <v>3</v>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="B145" s="10"/>
       <c r="C145" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D145" s="8" t="s">
         <v>3</v>
@@ -3761,7 +3761,7 @@
       </c>
       <c r="B146" s="10"/>
       <c r="C146" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D146" s="8" t="s">
         <v>3</v>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B147" s="10"/>
       <c r="C147" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D147" s="8" t="s">
         <v>3</v>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="B148" s="10"/>
       <c r="C148" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D148" s="8" t="s">
         <v>3</v>
@@ -3797,7 +3797,7 @@
       </c>
       <c r="B149" s="10"/>
       <c r="C149" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D149" s="8" t="s">
         <v>3</v>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="B150" s="10"/>
       <c r="C150" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D150" s="8" t="s">
         <v>3</v>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B151" s="10"/>
       <c r="C151" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D151" s="8" t="s">
         <v>3</v>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="B152" s="10"/>
       <c r="C152" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D152" s="8" t="s">
         <v>3</v>
@@ -3845,7 +3845,7 @@
       </c>
       <c r="B153" s="10"/>
       <c r="C153" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D153" s="8" t="s">
         <v>3</v>
@@ -3855,12 +3855,14 @@
       <c r="A154" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B154" s="10"/>
+      <c r="B154" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="C154" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D154" s="8" t="s">
-        <v>3</v>
+        <v>490</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.4">
@@ -3868,10 +3870,10 @@
         <v>96</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C155" s="11" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>465</v>
@@ -3882,14 +3884,12 @@
         <v>96</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>487</v>
+        <v>506</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>465</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D156" s="14"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A157" s="10"/>
@@ -7841,128 +7841,128 @@
   <hyperlinks>
     <hyperlink ref="C22" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>
     <hyperlink ref="C23" r:id="rId2" xr:uid="{2D6F1134-3C08-7445-B19A-9B94A18B55C7}"/>
-    <hyperlink ref="C26" r:id="rId3" xr:uid="{E5A98931-37E8-6B4A-90BE-8DC72405341A}"/>
-    <hyperlink ref="C27" r:id="rId4" xr:uid="{02736918-E09F-7A46-90B3-AFCC33AA559B}"/>
-    <hyperlink ref="C28" r:id="rId5" xr:uid="{6E8DD30A-A9F9-4C44-B26C-C9E236F10798}"/>
-    <hyperlink ref="C29" r:id="rId6" xr:uid="{0D55765B-95A7-154F-96F3-B7E4C581021F}"/>
-    <hyperlink ref="C30" r:id="rId7" xr:uid="{6F687ABA-C04B-AF4F-9F11-A038DCB20FB9}"/>
-    <hyperlink ref="C31" r:id="rId8" xr:uid="{11C9D8CC-9F1E-004E-8EC2-C758DC9C8CAB}"/>
-    <hyperlink ref="C32" r:id="rId9" xr:uid="{56E4962F-CB3D-9E48-A26E-19A1F5C800C9}"/>
-    <hyperlink ref="C33" r:id="rId10" xr:uid="{899DDBD9-9ED6-3A4D-8AFE-8FAA6DA88DBC}"/>
-    <hyperlink ref="C34" r:id="rId11" xr:uid="{76D41EAC-A28A-2845-8515-CA3C70D823B7}"/>
-    <hyperlink ref="C35" r:id="rId12" xr:uid="{828948BE-DD97-DE4A-BAD6-B415E29198F0}"/>
-    <hyperlink ref="C36" r:id="rId13" xr:uid="{E98C86AA-12E7-124C-B7D0-BCDFB246040B}"/>
-    <hyperlink ref="C37" r:id="rId14" xr:uid="{192741A9-FF68-DC4A-99FA-69F9968AB4F2}"/>
-    <hyperlink ref="C38" r:id="rId15" xr:uid="{DBD9BA9C-91C6-B144-A800-DCB3BED33DE7}"/>
-    <hyperlink ref="C39" r:id="rId16" xr:uid="{A285BDE8-00E7-A94C-8E43-A0C4829D42FA}"/>
-    <hyperlink ref="C40" r:id="rId17" xr:uid="{B0C21764-2962-1649-8AFA-10FB9420C5FC}"/>
-    <hyperlink ref="C41" r:id="rId18" xr:uid="{9282CC15-9B38-E54B-B64C-557745C9C00A}"/>
-    <hyperlink ref="C42" r:id="rId19" xr:uid="{3BCCEBE2-AC3B-AC4F-8BA9-439ACEA133D4}"/>
-    <hyperlink ref="C43" r:id="rId20" xr:uid="{74F8D761-6EBF-594A-A6C7-40DE4CE96958}"/>
-    <hyperlink ref="C44" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
-    <hyperlink ref="C45" r:id="rId22" xr:uid="{2BF3F606-410B-264D-BF60-191C34D616BB}"/>
-    <hyperlink ref="C46" r:id="rId23" xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
-    <hyperlink ref="C47" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
-    <hyperlink ref="C48" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
-    <hyperlink ref="C49" r:id="rId26" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
-    <hyperlink ref="C50" r:id="rId27" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
-    <hyperlink ref="C51" r:id="rId28" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
-    <hyperlink ref="C52" r:id="rId29" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
-    <hyperlink ref="C53" r:id="rId30" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
-    <hyperlink ref="C54" r:id="rId31" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
-    <hyperlink ref="C55" r:id="rId32" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
-    <hyperlink ref="C56" r:id="rId33" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
-    <hyperlink ref="C57" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
-    <hyperlink ref="C58" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
-    <hyperlink ref="C59" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
-    <hyperlink ref="C62" r:id="rId37" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
-    <hyperlink ref="C63" r:id="rId38" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
-    <hyperlink ref="C64" r:id="rId39" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
-    <hyperlink ref="C65" r:id="rId40" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
-    <hyperlink ref="C66" r:id="rId41" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
-    <hyperlink ref="C67" r:id="rId42" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
-    <hyperlink ref="C68" r:id="rId43" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
-    <hyperlink ref="C69" r:id="rId44" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
-    <hyperlink ref="C70" r:id="rId45" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
-    <hyperlink ref="C71" r:id="rId46" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
-    <hyperlink ref="C74" r:id="rId47" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
-    <hyperlink ref="C75" r:id="rId48" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
-    <hyperlink ref="C76" r:id="rId49" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
-    <hyperlink ref="C78" r:id="rId50" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
-    <hyperlink ref="C79" r:id="rId51" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
-    <hyperlink ref="C80" r:id="rId52" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
-    <hyperlink ref="C81" r:id="rId53" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
-    <hyperlink ref="C82" r:id="rId54" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
-    <hyperlink ref="C83" r:id="rId55" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
-    <hyperlink ref="C84" r:id="rId56" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
-    <hyperlink ref="C85" r:id="rId57" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
-    <hyperlink ref="C86" r:id="rId58" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
-    <hyperlink ref="C87" r:id="rId59" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
-    <hyperlink ref="C88" r:id="rId60" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
-    <hyperlink ref="C89" r:id="rId61" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
-    <hyperlink ref="C90" r:id="rId62" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
-    <hyperlink ref="C91" r:id="rId63" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
-    <hyperlink ref="C92" r:id="rId64" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
-    <hyperlink ref="C93" r:id="rId65" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
-    <hyperlink ref="C94" r:id="rId66" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
-    <hyperlink ref="C95" r:id="rId67" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
-    <hyperlink ref="C96" r:id="rId68" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
-    <hyperlink ref="C97" r:id="rId69" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
-    <hyperlink ref="C98" r:id="rId70" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
-    <hyperlink ref="C99" r:id="rId71" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
-    <hyperlink ref="C100" r:id="rId72" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
-    <hyperlink ref="C101" r:id="rId73" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
-    <hyperlink ref="C102" r:id="rId74" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
-    <hyperlink ref="C103" r:id="rId75" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
-    <hyperlink ref="C104" r:id="rId76" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
-    <hyperlink ref="C105" r:id="rId77" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="C106" r:id="rId78" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="C107" r:id="rId79" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="C108" r:id="rId80" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="C109" r:id="rId81" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="C110" r:id="rId82" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="C111" r:id="rId83" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="C112" r:id="rId84" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="C113" r:id="rId85" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="C114" r:id="rId86" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
-    <hyperlink ref="C115" r:id="rId87" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
-    <hyperlink ref="C116" r:id="rId88" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
-    <hyperlink ref="C119" r:id="rId89" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
-    <hyperlink ref="C120" r:id="rId90" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
-    <hyperlink ref="C121" r:id="rId91" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
-    <hyperlink ref="C122" r:id="rId92" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
-    <hyperlink ref="C124" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
-    <hyperlink ref="C125" r:id="rId94" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
-    <hyperlink ref="C126" r:id="rId95" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
-    <hyperlink ref="C127" r:id="rId96" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
-    <hyperlink ref="C128" r:id="rId97" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
-    <hyperlink ref="C129" r:id="rId98" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
-    <hyperlink ref="C131" r:id="rId99" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
-    <hyperlink ref="C132" r:id="rId100" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
-    <hyperlink ref="C133" r:id="rId101" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
-    <hyperlink ref="C134" r:id="rId102" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
-    <hyperlink ref="C135" r:id="rId103" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
-    <hyperlink ref="C136" r:id="rId104" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
-    <hyperlink ref="C137" r:id="rId105" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
-    <hyperlink ref="C138" r:id="rId106" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
-    <hyperlink ref="C139" r:id="rId107" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
-    <hyperlink ref="C140" r:id="rId108" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
-    <hyperlink ref="C141" r:id="rId109" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
-    <hyperlink ref="C142" r:id="rId110" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
-    <hyperlink ref="C143" r:id="rId111" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
-    <hyperlink ref="C144" r:id="rId112" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
-    <hyperlink ref="C145" r:id="rId113" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
-    <hyperlink ref="C146" r:id="rId114" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
-    <hyperlink ref="C147" r:id="rId115" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
-    <hyperlink ref="C148" r:id="rId116" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
-    <hyperlink ref="C149" r:id="rId117" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
-    <hyperlink ref="C150" r:id="rId118" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
-    <hyperlink ref="C151" r:id="rId119" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
-    <hyperlink ref="C152" r:id="rId120" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
-    <hyperlink ref="C153" r:id="rId121" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
-    <hyperlink ref="C154" r:id="rId122" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
-    <hyperlink ref="C123" r:id="rId123" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
-    <hyperlink ref="C130" r:id="rId124" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
+    <hyperlink ref="C156" r:id="rId3" xr:uid="{E5A98931-37E8-6B4A-90BE-8DC72405341A}"/>
+    <hyperlink ref="C26" r:id="rId4" xr:uid="{02736918-E09F-7A46-90B3-AFCC33AA559B}"/>
+    <hyperlink ref="C27" r:id="rId5" xr:uid="{6E8DD30A-A9F9-4C44-B26C-C9E236F10798}"/>
+    <hyperlink ref="C28" r:id="rId6" xr:uid="{0D55765B-95A7-154F-96F3-B7E4C581021F}"/>
+    <hyperlink ref="C29" r:id="rId7" xr:uid="{6F687ABA-C04B-AF4F-9F11-A038DCB20FB9}"/>
+    <hyperlink ref="C30" r:id="rId8" xr:uid="{11C9D8CC-9F1E-004E-8EC2-C758DC9C8CAB}"/>
+    <hyperlink ref="C31" r:id="rId9" xr:uid="{56E4962F-CB3D-9E48-A26E-19A1F5C800C9}"/>
+    <hyperlink ref="C32" r:id="rId10" xr:uid="{899DDBD9-9ED6-3A4D-8AFE-8FAA6DA88DBC}"/>
+    <hyperlink ref="C33" r:id="rId11" xr:uid="{76D41EAC-A28A-2845-8515-CA3C70D823B7}"/>
+    <hyperlink ref="C34" r:id="rId12" xr:uid="{828948BE-DD97-DE4A-BAD6-B415E29198F0}"/>
+    <hyperlink ref="C35" r:id="rId13" xr:uid="{E98C86AA-12E7-124C-B7D0-BCDFB246040B}"/>
+    <hyperlink ref="C36" r:id="rId14" xr:uid="{192741A9-FF68-DC4A-99FA-69F9968AB4F2}"/>
+    <hyperlink ref="C37" r:id="rId15" xr:uid="{DBD9BA9C-91C6-B144-A800-DCB3BED33DE7}"/>
+    <hyperlink ref="C38" r:id="rId16" xr:uid="{A285BDE8-00E7-A94C-8E43-A0C4829D42FA}"/>
+    <hyperlink ref="C39" r:id="rId17" xr:uid="{B0C21764-2962-1649-8AFA-10FB9420C5FC}"/>
+    <hyperlink ref="C40" r:id="rId18" xr:uid="{9282CC15-9B38-E54B-B64C-557745C9C00A}"/>
+    <hyperlink ref="C41" r:id="rId19" xr:uid="{3BCCEBE2-AC3B-AC4F-8BA9-439ACEA133D4}"/>
+    <hyperlink ref="C42" r:id="rId20" xr:uid="{74F8D761-6EBF-594A-A6C7-40DE4CE96958}"/>
+    <hyperlink ref="C43" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
+    <hyperlink ref="C44" r:id="rId22" xr:uid="{2BF3F606-410B-264D-BF60-191C34D616BB}"/>
+    <hyperlink ref="C45" r:id="rId23" xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
+    <hyperlink ref="C46" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
+    <hyperlink ref="C47" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
+    <hyperlink ref="C48" r:id="rId26" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
+    <hyperlink ref="C49" r:id="rId27" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
+    <hyperlink ref="C50" r:id="rId28" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
+    <hyperlink ref="C51" r:id="rId29" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
+    <hyperlink ref="C52" r:id="rId30" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
+    <hyperlink ref="C53" r:id="rId31" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
+    <hyperlink ref="C54" r:id="rId32" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
+    <hyperlink ref="C55" r:id="rId33" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
+    <hyperlink ref="C56" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
+    <hyperlink ref="C57" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
+    <hyperlink ref="C58" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
+    <hyperlink ref="C61" r:id="rId37" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
+    <hyperlink ref="C62" r:id="rId38" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
+    <hyperlink ref="C63" r:id="rId39" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
+    <hyperlink ref="C64" r:id="rId40" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
+    <hyperlink ref="C65" r:id="rId41" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
+    <hyperlink ref="C66" r:id="rId42" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
+    <hyperlink ref="C67" r:id="rId43" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
+    <hyperlink ref="C68" r:id="rId44" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
+    <hyperlink ref="C69" r:id="rId45" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
+    <hyperlink ref="C70" r:id="rId46" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
+    <hyperlink ref="C73" r:id="rId47" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
+    <hyperlink ref="C74" r:id="rId48" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
+    <hyperlink ref="C75" r:id="rId49" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
+    <hyperlink ref="C77" r:id="rId50" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
+    <hyperlink ref="C78" r:id="rId51" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
+    <hyperlink ref="C79" r:id="rId52" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
+    <hyperlink ref="C80" r:id="rId53" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
+    <hyperlink ref="C81" r:id="rId54" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
+    <hyperlink ref="C82" r:id="rId55" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
+    <hyperlink ref="C83" r:id="rId56" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
+    <hyperlink ref="C84" r:id="rId57" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
+    <hyperlink ref="C85" r:id="rId58" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
+    <hyperlink ref="C86" r:id="rId59" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
+    <hyperlink ref="C87" r:id="rId60" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
+    <hyperlink ref="C88" r:id="rId61" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
+    <hyperlink ref="C89" r:id="rId62" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
+    <hyperlink ref="C90" r:id="rId63" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
+    <hyperlink ref="C91" r:id="rId64" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
+    <hyperlink ref="C92" r:id="rId65" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
+    <hyperlink ref="C93" r:id="rId66" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
+    <hyperlink ref="C94" r:id="rId67" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
+    <hyperlink ref="C95" r:id="rId68" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
+    <hyperlink ref="C96" r:id="rId69" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
+    <hyperlink ref="C97" r:id="rId70" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
+    <hyperlink ref="C98" r:id="rId71" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
+    <hyperlink ref="C99" r:id="rId72" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
+    <hyperlink ref="C100" r:id="rId73" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
+    <hyperlink ref="C101" r:id="rId74" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
+    <hyperlink ref="C102" r:id="rId75" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
+    <hyperlink ref="C103" r:id="rId76" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
+    <hyperlink ref="C104" r:id="rId77" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
+    <hyperlink ref="C105" r:id="rId78" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
+    <hyperlink ref="C106" r:id="rId79" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
+    <hyperlink ref="C107" r:id="rId80" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
+    <hyperlink ref="C108" r:id="rId81" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
+    <hyperlink ref="C109" r:id="rId82" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
+    <hyperlink ref="C110" r:id="rId83" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
+    <hyperlink ref="C111" r:id="rId84" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
+    <hyperlink ref="C112" r:id="rId85" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
+    <hyperlink ref="C113" r:id="rId86" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
+    <hyperlink ref="C114" r:id="rId87" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
+    <hyperlink ref="C115" r:id="rId88" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
+    <hyperlink ref="C118" r:id="rId89" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
+    <hyperlink ref="C119" r:id="rId90" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
+    <hyperlink ref="C120" r:id="rId91" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
+    <hyperlink ref="C121" r:id="rId92" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
+    <hyperlink ref="C123" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
+    <hyperlink ref="C124" r:id="rId94" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
+    <hyperlink ref="C125" r:id="rId95" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
+    <hyperlink ref="C126" r:id="rId96" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
+    <hyperlink ref="C127" r:id="rId97" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
+    <hyperlink ref="C128" r:id="rId98" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
+    <hyperlink ref="C130" r:id="rId99" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
+    <hyperlink ref="C131" r:id="rId100" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
+    <hyperlink ref="C132" r:id="rId101" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
+    <hyperlink ref="C133" r:id="rId102" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
+    <hyperlink ref="C134" r:id="rId103" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
+    <hyperlink ref="C135" r:id="rId104" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
+    <hyperlink ref="C136" r:id="rId105" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
+    <hyperlink ref="C137" r:id="rId106" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
+    <hyperlink ref="C138" r:id="rId107" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
+    <hyperlink ref="C139" r:id="rId108" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
+    <hyperlink ref="C140" r:id="rId109" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
+    <hyperlink ref="C141" r:id="rId110" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
+    <hyperlink ref="C142" r:id="rId111" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
+    <hyperlink ref="C143" r:id="rId112" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
+    <hyperlink ref="C144" r:id="rId113" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
+    <hyperlink ref="C145" r:id="rId114" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
+    <hyperlink ref="C146" r:id="rId115" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
+    <hyperlink ref="C147" r:id="rId116" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
+    <hyperlink ref="C148" r:id="rId117" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
+    <hyperlink ref="C149" r:id="rId118" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
+    <hyperlink ref="C150" r:id="rId119" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
+    <hyperlink ref="C151" r:id="rId120" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
+    <hyperlink ref="C152" r:id="rId121" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
+    <hyperlink ref="C153" r:id="rId122" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
+    <hyperlink ref="C122" r:id="rId123" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
+    <hyperlink ref="C129" r:id="rId124" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
     <hyperlink ref="C158" r:id="rId125" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
     <hyperlink ref="C159" r:id="rId126" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
     <hyperlink ref="C160" r:id="rId127" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
@@ -8284,7 +8284,7 @@
     <hyperlink ref="C498" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
     <hyperlink ref="C499" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="C375" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
-    <hyperlink ref="C156" r:id="rId446" xr:uid="{F0DDC999-C321-4AB4-BA9D-7538150E84D3}"/>
+    <hyperlink ref="C155" r:id="rId446" xr:uid="{F0DDC999-C321-4AB4-BA9D-7538150E84D3}"/>
     <hyperlink ref="C9" r:id="rId447" xr:uid="{310D755F-0FAF-4086-8950-B58917F7CAF8}"/>
     <hyperlink ref="C8" r:id="rId448" xr:uid="{6913685B-862A-49D7-AB28-593B13669931}"/>
     <hyperlink ref="C10" r:id="rId449" xr:uid="{E2555AFC-8C22-4A69-A028-B6C7E7796509}"/>
@@ -8297,7 +8297,7 @@
     <hyperlink ref="C18" r:id="rId456" xr:uid="{D825528B-18AF-463A-AA31-760F76F78A15}"/>
     <hyperlink ref="C12" r:id="rId457" xr:uid="{027E7E1D-0C53-4A77-9662-F495CEC3BAC4}"/>
     <hyperlink ref="C19" r:id="rId458" xr:uid="{B7A6DAE3-6E86-4612-A1FF-539F5C6D3E1D}"/>
-    <hyperlink ref="C155" r:id="rId459" xr:uid="{5221452B-37E3-4315-91B2-6A38CEBB1898}"/>
+    <hyperlink ref="C154" r:id="rId459" xr:uid="{5221452B-37E3-4315-91B2-6A38CEBB1898}"/>
     <hyperlink ref="C24" r:id="rId460" xr:uid="{7C6054B7-B807-4475-B490-126A9686EBA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Program to push negative and positive element aside in a array added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E7A710-9EDC-478C-B655-13AF44680E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C442FE2-366B-4818-AA79-D75AB0EC4B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="3744" yWindow="2016" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="515">
   <si>
     <t>Topic:</t>
   </si>
@@ -1567,6 +1567,9 @@
   </si>
   <si>
     <t>POAE1ARR</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1656,6 +1659,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1673,7 +1682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1706,6 +1715,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2032,7 +2044,7 @@
   <dimension ref="A1:F501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2373,7 +2385,9 @@
       <c r="C26" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="9" t="s">
@@ -2385,8 +2399,8 @@
       <c r="C27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>3</v>
+      <c r="D27" s="14" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -2399,8 +2413,8 @@
       <c r="C28" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>3</v>
+      <c r="D28" s="3" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Program to find frequencies of element in an array is added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C442FE2-366B-4818-AA79-D75AB0EC4B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2B347F-6A6D-434E-AEA4-0CD5CC5EE7B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="2016" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2043,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2427,8 +2427,8 @@
       <c r="C29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>3</v>
+      <c r="D29" s="14" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -2441,8 +2441,8 @@
       <c r="C30" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>3</v>
+      <c r="D30" s="3" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -2453,8 +2453,8 @@
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>3</v>
+      <c r="D31" s="14" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
@@ -2465,8 +2465,8 @@
       <c r="C32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>3</v>
+      <c r="D32" s="14" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
@@ -2477,8 +2477,8 @@
       <c r="C33" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>3</v>
+      <c r="D33" s="14" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
@@ -2621,8 +2621,8 @@
       <c r="C45" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>3</v>
+      <c r="D45" s="3" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
During Revision Minor Changes
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B735BA9A-2AAD-4054-AEFB-6F24F5D51C16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EADEF08-641B-4FCA-8645-D9DDF40692E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="523">
   <si>
     <t>Topic:</t>
   </si>
@@ -1579,6 +1579,21 @@
   </si>
   <si>
     <t>Important</t>
+  </si>
+  <si>
+    <t>Good Question</t>
+  </si>
+  <si>
+    <t>PARTIALLY YES</t>
+  </si>
+  <si>
+    <t>I leave out the portion where we need to preserve the original order</t>
+  </si>
+  <si>
+    <t>Link To Answer</t>
+  </si>
+  <si>
+    <t>Simple Question</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1673,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1677,6 +1692,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1691,7 +1712,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1727,6 +1748,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2052,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="E427" sqref="E427"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2341,6 +2365,9 @@
       <c r="D22" s="3" t="s">
         <v>465</v>
       </c>
+      <c r="E22" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
@@ -2355,6 +2382,9 @@
       <c r="D23" s="3" t="s">
         <v>465</v>
       </c>
+      <c r="E23" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="9" t="s">
@@ -2369,6 +2399,9 @@
       <c r="D24" s="3" t="s">
         <v>465</v>
       </c>
+      <c r="E24" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="9" t="s">
@@ -2383,6 +2416,12 @@
       <c r="D25" s="3" t="s">
         <v>465</v>
       </c>
+      <c r="E25" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="9" t="s">
@@ -2397,6 +2436,12 @@
       <c r="D26" s="3" t="s">
         <v>465</v>
       </c>
+      <c r="E26" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="9" t="s">
@@ -2408,8 +2453,14 @@
       <c r="C27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>514</v>
+      <c r="D27" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -2422,8 +2473,11 @@
       <c r="C28" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>465</v>
+      <c r="D28" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
@@ -2436,8 +2490,11 @@
       <c r="C29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>514</v>
+      <c r="D29" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -2452,6 +2509,12 @@
       </c>
       <c r="D30" s="3" t="s">
         <v>465</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -8362,8 +8425,9 @@
     <hyperlink ref="C75" r:id="rId461" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
     <hyperlink ref="C74" r:id="rId462" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
     <hyperlink ref="C73" r:id="rId463" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
+    <hyperlink ref="F29" r:id="rId464" xr:uid="{03443138-A680-4B72-A76F-ED2F3C418FFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId464"/>
+  <pageSetup orientation="portrait" r:id="rId465"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merging of two sorted array without extra space
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC949CD-96A5-445B-8260-F4D56A4DB1E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EFC990-29DE-4B30-98C4-8C524FC47FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="528">
   <si>
     <t>Topic:</t>
   </si>
@@ -1606,6 +1606,9 @@
   </si>
   <si>
     <t>KD1ARR</t>
+  </si>
+  <si>
+    <t>M2SA1ARR</t>
   </si>
 </sst>
 </file>
@@ -2089,7 +2092,7 @@
   <dimension ref="A1:H503"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2620,7 +2623,9 @@
       <c r="A36" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="9" t="s">
+        <v>527</v>
+      </c>
       <c r="C36" s="10" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Program to find minimum no of jumps
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216AA6A2-5BB1-40B7-BA2F-F816E0CA9D1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32FA80-56C8-4356-B219-F6DCE00FF184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="536">
   <si>
     <t>Topic:</t>
   </si>
@@ -1627,6 +1627,12 @@
   </si>
   <si>
     <t>🗸</t>
+  </si>
+  <si>
+    <t>MNJ1ARR</t>
+  </si>
+  <si>
+    <t>VERY HARD</t>
   </si>
 </sst>
 </file>
@@ -2182,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:K503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2770,7 +2776,9 @@
       <c r="A33" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="9" t="s">
+        <v>534</v>
+      </c>
       <c r="C33" s="10" t="s">
         <v>14</v>
       </c>
@@ -2782,7 +2790,9 @@
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="21"/>
+      <c r="H33" s="24" t="s">
+        <v>535</v>
+      </c>
       <c r="I33" s="5" t="s">
         <v>522</v>
       </c>
@@ -2807,7 +2817,7 @@
         <v>465</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="21"/>
@@ -2830,7 +2840,7 @@
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="23" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H35" s="21"/>
       <c r="K35" s="10" t="s">
@@ -2856,7 +2866,7 @@
       <c r="F36" s="22"/>
       <c r="G36" s="20"/>
       <c r="H36" s="24" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>528</v>
@@ -2883,7 +2893,7 @@
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="23" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H37" s="21"/>
     </row>

</xml_diff>

<commit_message>
Minimize the heights program added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32FA80-56C8-4356-B219-F6DCE00FF184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD91467-27D4-4CB9-BC0A-2E86495F1432}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="527">
   <si>
     <t>Topic:</t>
   </si>
@@ -1521,15 +1521,6 @@
     <t>PAPN0MATH</t>
   </si>
   <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Sieve Of Erasthothenus</t>
-  </si>
-  <si>
-    <t>Eucledian Algorithm</t>
-  </si>
-  <si>
     <t>Find second largest element in array</t>
   </si>
   <si>
@@ -1575,45 +1566,21 @@
     <t>Frequency of all elements in an sorted array</t>
   </si>
   <si>
-    <t>Important</t>
-  </si>
-  <si>
-    <t>Good Question</t>
-  </si>
-  <si>
     <t>PARTIALLY YES</t>
   </si>
   <si>
     <t>Link To Answer</t>
   </si>
   <si>
-    <t>Simple Question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It's usage is Kadan's Algorithm </t>
-  </si>
-  <si>
-    <t>Vey Important</t>
-  </si>
-  <si>
     <t>Answer Link</t>
   </si>
   <si>
-    <t>Very Important</t>
-  </si>
-  <si>
-    <t>I left out that portion where we need to preserve the original order</t>
-  </si>
-  <si>
     <t>KD1ARR</t>
   </si>
   <si>
     <t>M2SA1ARR</t>
   </si>
   <si>
-    <t>Most Important</t>
-  </si>
-  <si>
     <t>DIA1ARR</t>
   </si>
   <si>
@@ -1626,13 +1593,19 @@
     <t>HARD</t>
   </si>
   <si>
-    <t>🗸</t>
-  </si>
-  <si>
     <t>MNJ1ARR</t>
   </si>
   <si>
     <t>VERY HARD</t>
+  </si>
+  <si>
+    <t>☒</t>
+  </si>
+  <si>
+    <t>MMD1ARR</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1823,9 +1796,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2188,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:K503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2203,31 +2173,31 @@
     <col min="10" max="16384" width="11.19921875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C1" s="12" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C2" s="12" t="s">
         <v>494</v>
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C3" s="12" t="s">
         <v>495</v>
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2244,26 +2214,26 @@
         <v>492</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>532</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+        <v>521</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>466</v>
       </c>
@@ -2273,19 +2243,19 @@
       <c r="C8" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>533</v>
-      </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F8" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>466</v>
       </c>
@@ -2295,17 +2265,17 @@
       <c r="C9" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F9" s="21"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
         <v>466</v>
       </c>
@@ -2315,17 +2285,17 @@
       <c r="C10" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F10" s="21"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>466</v>
       </c>
@@ -2335,17 +2305,17 @@
       <c r="C11" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F11" s="21"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
         <v>466</v>
       </c>
@@ -2355,17 +2325,17 @@
       <c r="C12" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F12" s="21"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>466</v>
       </c>
@@ -2375,17 +2345,17 @@
       <c r="C13" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F13" s="21"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
         <v>466</v>
       </c>
@@ -2395,20 +2365,17 @@
       <c r="C14" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="5" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F14" s="21"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>466</v>
       </c>
@@ -2418,17 +2385,17 @@
       <c r="C15" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F15" s="21"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
         <v>466</v>
       </c>
@@ -2438,15 +2405,15 @@
       <c r="C16" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
@@ -2458,15 +2425,15 @@
       <c r="C17" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
@@ -2478,15 +2445,15 @@
       <c r="C18" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
@@ -2498,210 +2465,186 @@
       <c r="C19" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="5" t="s">
-        <v>499</v>
-      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="12"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4"/>
       <c r="D20" s="13"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="D21" s="7"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="D24" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="D25" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="5" t="s">
-        <v>517</v>
-      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>512</v>
-      </c>
-      <c r="D26" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="5" t="s">
-        <v>517</v>
-      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="5" t="s">
-        <v>517</v>
-      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="16" t="s">
-        <v>518</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="5" t="s">
-        <v>525</v>
-      </c>
+      <c r="D28" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A29" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="K29" s="10" t="s">
         <v>514</v>
-      </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.4">
@@ -2709,67 +2652,80 @@
         <v>4</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="5" t="s">
+      <c r="F30" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G30" s="22" t="s">
         <v>520</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="9" t="s">
+        <v>516</v>
+      </c>
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="5" t="s">
-        <v>521</v>
+      <c r="D31" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>519</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="9"/>
+      <c r="B32" s="9" t="s">
+        <v>525</v>
+      </c>
       <c r="C32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="5" t="s">
-        <v>522</v>
+      <c r="D32" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>521</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
@@ -2777,27 +2733,28 @@
         <v>4</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="24" t="s">
-        <v>535</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>522</v>
+      <c r="D33" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>523</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
@@ -2808,43 +2765,51 @@
         <v>490</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>515</v>
-      </c>
-      <c r="D34" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F34" s="19" t="s">
-        <v>530</v>
-      </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="21"/>
+      <c r="F34" s="18" t="s">
+        <v>519</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="23" t="s">
-        <v>531</v>
-      </c>
-      <c r="H35" s="21"/>
+      <c r="F35" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>524</v>
+      </c>
       <c r="K35" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
@@ -2852,27 +2817,28 @@
         <v>4</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="24" t="s">
-        <v>532</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>528</v>
+      <c r="F36" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>521</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
@@ -2880,22 +2846,26 @@
         <v>4</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="F37" s="22"/>
-      <c r="G37" s="23" t="s">
-        <v>531</v>
-      </c>
-      <c r="H37" s="21"/>
+      <c r="F37" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" s="9" t="s">
@@ -2905,12 +2875,12 @@
       <c r="C38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="21"/>
+      <c r="D38" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F38" s="21"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" s="9" t="s">
@@ -2920,12 +2890,12 @@
       <c r="C39" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="21"/>
+      <c r="D39" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F39" s="21"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" s="9" t="s">
@@ -2935,12 +2905,12 @@
       <c r="C40" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="21"/>
+      <c r="D40" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="20"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" s="9" t="s">
@@ -2950,15 +2920,12 @@
       <c r="C41" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="F41" s="22"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="5" t="s">
-        <v>516</v>
-      </c>
+      <c r="F41" s="21"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" s="9" t="s">
@@ -2968,12 +2935,12 @@
       <c r="C42" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="21"/>
+      <c r="D42" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F42" s="21"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="20"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43" s="9" t="s">
@@ -2983,12 +2950,12 @@
       <c r="C43" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F43" s="22"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="21"/>
+      <c r="D43" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F43" s="21"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" s="9" t="s">
@@ -2998,12 +2965,12 @@
       <c r="C44" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="21"/>
+      <c r="D44" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F44" s="21"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="20"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" s="9" t="s">
@@ -3013,12 +2980,12 @@
       <c r="C45" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="21"/>
+      <c r="D45" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F45" s="21"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="20"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" s="9" t="s">
@@ -3028,12 +2995,12 @@
       <c r="C46" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="F46" s="22"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="20"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" s="9" t="s">
@@ -3043,12 +3010,12 @@
       <c r="C47" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D47" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F47" s="22"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="21"/>
+      <c r="D47" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F47" s="21"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="20"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" s="9" t="s">
@@ -3058,12 +3025,12 @@
       <c r="C48" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F48" s="22"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="21"/>
+      <c r="D48" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F48" s="21"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="20"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="9" t="s">
@@ -3073,12 +3040,12 @@
       <c r="C49" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F49" s="22"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="21"/>
+      <c r="D49" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F49" s="21"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="20"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="9" t="s">
@@ -3088,12 +3055,12 @@
       <c r="C50" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F50" s="22"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="21"/>
+      <c r="D50" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F50" s="21"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="20"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="9" t="s">
@@ -3103,12 +3070,12 @@
       <c r="C51" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F51" s="22"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="21"/>
+      <c r="D51" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F51" s="21"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="20"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="9" t="s">
@@ -3118,12 +3085,12 @@
       <c r="C52" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="21"/>
+      <c r="D52" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F52" s="21"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="20"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="9" t="s">
@@ -3136,9 +3103,9 @@
       <c r="D53" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="20"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="9" t="s">
@@ -3148,12 +3115,12 @@
       <c r="C54" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F54" s="22"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="21"/>
+      <c r="D54" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F54" s="21"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="20"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="9" t="s">
@@ -3163,12 +3130,12 @@
       <c r="C55" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F55" s="22"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="21"/>
+      <c r="D55" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="20"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="9" t="s">
@@ -3178,12 +3145,12 @@
       <c r="C56" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D56" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F56" s="22"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="21"/>
+      <c r="D56" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F56" s="21"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="20"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="9" t="s">
@@ -3193,12 +3160,12 @@
       <c r="C57" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F57" s="22"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="21"/>
+      <c r="D57" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F57" s="21"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="20"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="9" t="s">
@@ -3208,12 +3175,12 @@
       <c r="C58" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D58" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F58" s="22"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="21"/>
+      <c r="D58" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F58" s="21"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="20"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" s="9" t="s">
@@ -3223,12 +3190,12 @@
       <c r="C59" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D59" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F59" s="22"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="21"/>
+      <c r="D59" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F59" s="21"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="20"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="9" t="s">
@@ -3238,12 +3205,12 @@
       <c r="C60" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D60" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F60" s="22"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="21"/>
+      <c r="D60" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F60" s="21"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="20"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D61" s="13"/>
@@ -4143,7 +4110,7 @@
         <v>96</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C122" s="10" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Program to find next permutation added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD91467-27D4-4CB9-BC0A-2E86495F1432}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C243BF-FC90-4044-89F0-10E57E4B9C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="528">
   <si>
     <t>Topic:</t>
   </si>
@@ -1606,6 +1606,9 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>NP1ARR</t>
   </si>
 </sst>
 </file>
@@ -2158,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:K503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2871,16 +2874,27 @@
       <c r="A38" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="9"/>
+      <c r="B38" s="9" t="s">
+        <v>527</v>
+      </c>
       <c r="C38" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>511</v>
-      </c>
-      <c r="F38" s="21"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="20"/>
+        <v>19</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" s="9" t="s">
@@ -2888,7 +2902,7 @@
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>511</v>
@@ -2903,10 +2917,10 @@
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>511</v>
+        <v>21</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>465</v>
       </c>
       <c r="F40" s="21"/>
       <c r="G40" s="19"/>
@@ -2918,10 +2932,10 @@
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>465</v>
+        <v>22</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>511</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="19"/>
@@ -2933,7 +2947,7 @@
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>511</v>
@@ -2948,7 +2962,7 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>511</v>
@@ -2963,7 +2977,7 @@
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>511</v>
@@ -2978,10 +2992,10 @@
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>511</v>
+        <v>26</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>465</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="19"/>
@@ -2993,10 +3007,10 @@
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>465</v>
+        <v>27</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>511</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="19"/>
@@ -3008,7 +3022,7 @@
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>511</v>
@@ -3023,7 +3037,7 @@
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>511</v>
@@ -3038,7 +3052,7 @@
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>511</v>
@@ -3053,7 +3067,7 @@
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>511</v>
@@ -3068,7 +3082,7 @@
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>511</v>
@@ -3083,10 +3097,10 @@
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>511</v>
+        <v>33</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>465</v>
       </c>
       <c r="F52" s="21"/>
       <c r="G52" s="19"/>
@@ -3098,10 +3112,10 @@
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>465</v>
+        <v>34</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>511</v>
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="19"/>
@@ -3113,7 +3127,7 @@
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>511</v>
@@ -3128,7 +3142,7 @@
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>511</v>
@@ -3143,7 +3157,7 @@
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>511</v>
@@ -3158,7 +3172,7 @@
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>511</v>
@@ -3173,7 +3187,7 @@
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>511</v>
@@ -3188,7 +3202,7 @@
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>511</v>
@@ -3198,22 +3212,22 @@
       <c r="H59" s="20"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A60" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>511</v>
-      </c>
-      <c r="F60" s="21"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="20"/>
+      <c r="D60" s="13"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D61" s="13"/>
+      <c r="A61" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
@@ -3224,7 +3238,7 @@
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="10" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>3</v>
@@ -3239,7 +3253,7 @@
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>3</v>
@@ -3254,7 +3268,7 @@
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="10" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>3</v>
@@ -3269,7 +3283,7 @@
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="10" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>3</v>
@@ -3284,7 +3298,7 @@
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="10" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>3</v>
@@ -3299,7 +3313,7 @@
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="10" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>3</v>
@@ -3314,7 +3328,7 @@
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>3</v>
@@ -3329,7 +3343,7 @@
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="10" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>3</v>
@@ -3344,7 +3358,7 @@
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="10" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>3</v>
@@ -3354,24 +3368,24 @@
       <c r="H70" s="12"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A71" s="9" t="s">
-        <v>452</v>
-      </c>
+      <c r="A71" s="9"/>
       <c r="B71" s="9"/>
-      <c r="C71" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D71" s="7"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="D72" s="7"/>
+      <c r="A72" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" s="7"/>
+      <c r="C72" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
       <c r="H72" s="12"/>
@@ -3382,7 +3396,7 @@
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>3</v>
@@ -3397,7 +3411,7 @@
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>3</v>
@@ -3412,7 +3426,7 @@
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>3</v>
@@ -3427,7 +3441,7 @@
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>3</v>
@@ -3442,7 +3456,7 @@
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>3</v>
@@ -3457,7 +3471,7 @@
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>3</v>
@@ -3472,7 +3486,7 @@
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>3</v>
@@ -3487,7 +3501,7 @@
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>3</v>
@@ -3502,7 +3516,7 @@
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>3</v>
@@ -3512,24 +3526,19 @@
       <c r="H81" s="12"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B82" s="7"/>
+      <c r="B82" s="9"/>
       <c r="C82" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="F82" s="21"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="20"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84" s="9" t="s">
@@ -9222,29 +9231,29 @@
     <hyperlink ref="C35" r:id="rId11" xr:uid="{76D41EAC-A28A-2845-8515-CA3C70D823B7}"/>
     <hyperlink ref="C36" r:id="rId12" xr:uid="{828948BE-DD97-DE4A-BAD6-B415E29198F0}"/>
     <hyperlink ref="C37" r:id="rId13" xr:uid="{E98C86AA-12E7-124C-B7D0-BCDFB246040B}"/>
-    <hyperlink ref="C38" r:id="rId14" xr:uid="{192741A9-FF68-DC4A-99FA-69F9968AB4F2}"/>
-    <hyperlink ref="C39" r:id="rId15" xr:uid="{DBD9BA9C-91C6-B144-A800-DCB3BED33DE7}"/>
-    <hyperlink ref="C40" r:id="rId16" xr:uid="{A285BDE8-00E7-A94C-8E43-A0C4829D42FA}"/>
-    <hyperlink ref="C41" r:id="rId17" xr:uid="{B0C21764-2962-1649-8AFA-10FB9420C5FC}"/>
-    <hyperlink ref="C42" r:id="rId18" xr:uid="{9282CC15-9B38-E54B-B64C-557745C9C00A}"/>
-    <hyperlink ref="C43" r:id="rId19" xr:uid="{3BCCEBE2-AC3B-AC4F-8BA9-439ACEA133D4}"/>
-    <hyperlink ref="C44" r:id="rId20" xr:uid="{74F8D761-6EBF-594A-A6C7-40DE4CE96958}"/>
-    <hyperlink ref="C45" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
-    <hyperlink ref="C46" r:id="rId22" xr:uid="{2BF3F606-410B-264D-BF60-191C34D616BB}"/>
-    <hyperlink ref="C47" r:id="rId23" xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
-    <hyperlink ref="C48" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
-    <hyperlink ref="C49" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
-    <hyperlink ref="C50" r:id="rId26" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
-    <hyperlink ref="C51" r:id="rId27" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
-    <hyperlink ref="C52" r:id="rId28" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
-    <hyperlink ref="C53" r:id="rId29" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
-    <hyperlink ref="C54" r:id="rId30" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
-    <hyperlink ref="C55" r:id="rId31" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
-    <hyperlink ref="C56" r:id="rId32" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
-    <hyperlink ref="C57" r:id="rId33" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
-    <hyperlink ref="C58" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
-    <hyperlink ref="C59" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
-    <hyperlink ref="C60" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
+    <hyperlink ref="C82" r:id="rId14" xr:uid="{192741A9-FF68-DC4A-99FA-69F9968AB4F2}"/>
+    <hyperlink ref="C38" r:id="rId15" xr:uid="{DBD9BA9C-91C6-B144-A800-DCB3BED33DE7}"/>
+    <hyperlink ref="C39" r:id="rId16" xr:uid="{A285BDE8-00E7-A94C-8E43-A0C4829D42FA}"/>
+    <hyperlink ref="C40" r:id="rId17" xr:uid="{B0C21764-2962-1649-8AFA-10FB9420C5FC}"/>
+    <hyperlink ref="C41" r:id="rId18" xr:uid="{9282CC15-9B38-E54B-B64C-557745C9C00A}"/>
+    <hyperlink ref="C42" r:id="rId19" xr:uid="{3BCCEBE2-AC3B-AC4F-8BA9-439ACEA133D4}"/>
+    <hyperlink ref="C43" r:id="rId20" xr:uid="{74F8D761-6EBF-594A-A6C7-40DE4CE96958}"/>
+    <hyperlink ref="C44" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
+    <hyperlink ref="C45" r:id="rId22" xr:uid="{2BF3F606-410B-264D-BF60-191C34D616BB}"/>
+    <hyperlink ref="C46" r:id="rId23" xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
+    <hyperlink ref="C47" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
+    <hyperlink ref="C48" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
+    <hyperlink ref="C49" r:id="rId26" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
+    <hyperlink ref="C50" r:id="rId27" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
+    <hyperlink ref="C51" r:id="rId28" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
+    <hyperlink ref="C52" r:id="rId29" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
+    <hyperlink ref="C53" r:id="rId30" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
+    <hyperlink ref="C54" r:id="rId31" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
+    <hyperlink ref="C55" r:id="rId32" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
+    <hyperlink ref="C56" r:id="rId33" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
+    <hyperlink ref="C57" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
+    <hyperlink ref="C58" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
+    <hyperlink ref="C59" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
     <hyperlink ref="C161" r:id="rId37" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
     <hyperlink ref="C162" r:id="rId38" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
     <hyperlink ref="C163" r:id="rId39" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
@@ -9597,16 +9606,16 @@
     <hyperlink ref="C482" r:id="rId386" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
     <hyperlink ref="C481" r:id="rId387" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
     <hyperlink ref="C480" r:id="rId388" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="C62" r:id="rId389" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="C63" r:id="rId390" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="C64" r:id="rId391" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="C65" r:id="rId392" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="C66" r:id="rId393" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="C67" r:id="rId394" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="C68" r:id="rId395" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="C71" r:id="rId396" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="C69" r:id="rId397" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="C70" r:id="rId398" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="C61" r:id="rId389" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="C62" r:id="rId390" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="C63" r:id="rId391" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="C64" r:id="rId392" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="C65" r:id="rId393" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="C66" r:id="rId394" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="C67" r:id="rId395" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="C70" r:id="rId396" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="C68" r:id="rId397" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="C69" r:id="rId398" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="C325" r:id="rId399" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="C121" r:id="rId400" xr:uid="{F0DDC999-C321-4AB4-BA9D-7538150E84D3}"/>
     <hyperlink ref="C9" r:id="rId401" xr:uid="{310D755F-0FAF-4086-8950-B58917F7CAF8}"/>
@@ -9662,16 +9671,16 @@
     <hyperlink ref="C126" r:id="rId451" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
     <hyperlink ref="C125" r:id="rId452" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
     <hyperlink ref="C124" r:id="rId453" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
-    <hyperlink ref="C82" r:id="rId454" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
-    <hyperlink ref="C81" r:id="rId455" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
-    <hyperlink ref="C80" r:id="rId456" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
-    <hyperlink ref="C79" r:id="rId457" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
-    <hyperlink ref="C78" r:id="rId458" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
-    <hyperlink ref="C77" r:id="rId459" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
-    <hyperlink ref="C76" r:id="rId460" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
-    <hyperlink ref="C75" r:id="rId461" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
-    <hyperlink ref="C74" r:id="rId462" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
-    <hyperlink ref="C73" r:id="rId463" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
+    <hyperlink ref="C81" r:id="rId454" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
+    <hyperlink ref="C80" r:id="rId455" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
+    <hyperlink ref="C79" r:id="rId456" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
+    <hyperlink ref="C78" r:id="rId457" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
+    <hyperlink ref="C77" r:id="rId458" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
+    <hyperlink ref="C76" r:id="rId459" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
+    <hyperlink ref="C75" r:id="rId460" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
+    <hyperlink ref="C74" r:id="rId461" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
+    <hyperlink ref="C73" r:id="rId462" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
+    <hyperlink ref="C72" r:id="rId463" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
     <hyperlink ref="K29" r:id="rId464" xr:uid="{03443138-A680-4B72-A76F-ED2F3C418FFF}"/>
     <hyperlink ref="K32" r:id="rId465" xr:uid="{E2846214-1318-4E7F-B406-DB8B8C109F51}"/>
     <hyperlink ref="K33" r:id="rId466" xr:uid="{654A45B7-1C43-48E0-B7BB-03647CB459F1}"/>

</xml_diff>

<commit_message>
Program to find triplet added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27AD1DA-5036-41C4-B3E3-C9A0E73D626F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D2D386-8DFF-4026-AAF4-11D73D697963}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="537">
   <si>
     <t>Topic:</t>
   </si>
@@ -1629,10 +1629,13 @@
     <t>find maximum product subarray (DP)</t>
   </si>
   <si>
-    <t>MPSA4HASH</t>
-  </si>
-  <si>
     <t>MPSA15DP</t>
+  </si>
+  <si>
+    <t>WASON4HASH</t>
+  </si>
+  <si>
+    <t>TSGV1ARR</t>
   </si>
 </sst>
 </file>
@@ -2185,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:K504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2644,6 +2647,9 @@
       <c r="D28" s="15" t="s">
         <v>510</v>
       </c>
+      <c r="E28" s="17" t="s">
+        <v>508</v>
+      </c>
       <c r="F28" s="21"/>
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
@@ -3051,16 +3057,27 @@
       <c r="A44" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="9"/>
+      <c r="B44" s="9" t="s">
+        <v>536</v>
+      </c>
       <c r="C44" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D44" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="E44" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="20"/>
+      <c r="F44" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" s="9" t="s">
@@ -3068,10 +3085,10 @@
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>508</v>
+        <v>30</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>462</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="19"/>
@@ -3083,10 +3100,10 @@
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>462</v>
+        <v>31</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>508</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="19"/>
@@ -3098,7 +3115,7 @@
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>508</v>
@@ -3113,7 +3130,7 @@
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>508</v>
@@ -3128,7 +3145,7 @@
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>508</v>
@@ -3143,7 +3160,7 @@
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>508</v>
@@ -3158,7 +3175,7 @@
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>508</v>
@@ -3173,7 +3190,7 @@
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>508</v>
@@ -3183,22 +3200,22 @@
       <c r="H52" s="20"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A53" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="F53" s="21"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="20"/>
+      <c r="D53" s="13"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D54" s="13"/>
+      <c r="A54" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
@@ -3209,7 +3226,7 @@
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="10" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>3</v>
@@ -3224,7 +3241,7 @@
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="10" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>3</v>
@@ -3239,7 +3256,7 @@
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="10" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>3</v>
@@ -3254,7 +3271,7 @@
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="10" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>3</v>
@@ -3269,7 +3286,7 @@
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>3</v>
@@ -3284,7 +3301,7 @@
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="10" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>3</v>
@@ -3299,7 +3316,7 @@
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="10" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>3</v>
@@ -3314,7 +3331,7 @@
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="10" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>3</v>
@@ -3329,7 +3346,7 @@
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="10" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>3</v>
@@ -3339,24 +3356,24 @@
       <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A64" s="9" t="s">
-        <v>449</v>
-      </c>
+      <c r="A64" s="9"/>
       <c r="B64" s="9"/>
-      <c r="C64" s="10" t="s">
-        <v>459</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D64" s="7"/>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9"/>
-      <c r="D65" s="7"/>
+      <c r="A65" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="7"/>
+      <c r="C65" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
@@ -3367,7 +3384,7 @@
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>3</v>
@@ -3382,7 +3399,7 @@
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>3</v>
@@ -3397,7 +3414,7 @@
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>3</v>
@@ -3412,7 +3429,7 @@
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>3</v>
@@ -3427,7 +3444,7 @@
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>3</v>
@@ -3442,7 +3459,7 @@
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>3</v>
@@ -3457,7 +3474,7 @@
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>3</v>
@@ -3472,7 +3489,7 @@
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>3</v>
@@ -3487,7 +3504,7 @@
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>3</v>
@@ -3497,52 +3514,54 @@
       <c r="H74" s="12"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="7"/>
+      <c r="B75" s="9"/>
       <c r="C75" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="F75" s="21"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="20"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A76" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="A76" s="9"/>
       <c r="B76" s="9"/>
-      <c r="C76" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76" s="17" t="s">
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A77" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="B77" s="9"/>
+      <c r="C77" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="F76" s="21"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="20"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="20"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A78" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B78" s="9"/>
+      <c r="B78" s="9" t="s">
+        <v>530</v>
+      </c>
       <c r="C78" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D78" s="17" t="s">
         <v>508</v>
@@ -3555,11 +3574,9 @@
       <c r="A79" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>530</v>
-      </c>
+      <c r="B79" s="9"/>
       <c r="C79" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D79" s="17" t="s">
         <v>508</v>
@@ -3567,16 +3584,17 @@
       <c r="F79" s="21"/>
       <c r="G79" s="19"/>
       <c r="H79" s="20"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
+      <c r="K79" s="10"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A80" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B80" s="9" t="s">
-        <v>534</v>
-      </c>
+      <c r="B80" s="9"/>
       <c r="C80" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D80" s="17" t="s">
         <v>508</v>
@@ -3584,17 +3602,16 @@
       <c r="F80" s="21"/>
       <c r="G80" s="19"/>
       <c r="H80" s="20"/>
-      <c r="I80" s="10"/>
-      <c r="J80" s="10"/>
-      <c r="K80" s="10"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B81" s="9"/>
+      <c r="B81" s="9" t="s">
+        <v>535</v>
+      </c>
       <c r="C81" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D81" s="17" t="s">
         <v>508</v>
@@ -4223,10 +4240,11 @@
       <c r="A123" s="9"/>
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
-      <c r="D123" s="17"/>
-      <c r="F123" s="21"/>
-      <c r="G123" s="19"/>
-      <c r="H123" s="20"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A124" s="9" t="s">
@@ -9202,7 +9220,7 @@
         <v>389</v>
       </c>
       <c r="B487" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C487" s="10" t="s">
         <v>533</v>
@@ -9354,29 +9372,29 @@
     <hyperlink ref="C35" r:id="rId11" xr:uid="{76D41EAC-A28A-2845-8515-CA3C70D823B7}"/>
     <hyperlink ref="C36" r:id="rId12" xr:uid="{828948BE-DD97-DE4A-BAD6-B415E29198F0}"/>
     <hyperlink ref="C37" r:id="rId13" xr:uid="{E98C86AA-12E7-124C-B7D0-BCDFB246040B}"/>
-    <hyperlink ref="C76" r:id="rId14" xr:uid="{192741A9-FF68-DC4A-99FA-69F9968AB4F2}"/>
+    <hyperlink ref="C75" r:id="rId14" xr:uid="{192741A9-FF68-DC4A-99FA-69F9968AB4F2}"/>
     <hyperlink ref="C38" r:id="rId15" xr:uid="{DBD9BA9C-91C6-B144-A800-DCB3BED33DE7}"/>
     <hyperlink ref="C122" r:id="rId16" xr:uid="{A285BDE8-00E7-A94C-8E43-A0C4829D42FA}"/>
     <hyperlink ref="C39" r:id="rId17" xr:uid="{B0C21764-2962-1649-8AFA-10FB9420C5FC}"/>
-    <hyperlink ref="C78" r:id="rId18" xr:uid="{9282CC15-9B38-E54B-B64C-557745C9C00A}"/>
+    <hyperlink ref="C77" r:id="rId18" xr:uid="{9282CC15-9B38-E54B-B64C-557745C9C00A}"/>
     <hyperlink ref="C40" r:id="rId19" display="find common elements In 3 sorted arrays" xr:uid="{3BCCEBE2-AC3B-AC4F-8BA9-439ACEA133D4}"/>
     <hyperlink ref="C41" r:id="rId20" xr:uid="{74F8D761-6EBF-594A-A6C7-40DE4CE96958}"/>
-    <hyperlink ref="C79" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
+    <hyperlink ref="C78" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
     <hyperlink ref="C42" r:id="rId22" display="Find factorial of a large number" xr:uid="{2BF3F606-410B-264D-BF60-191C34D616BB}"/>
     <hyperlink ref="C487" r:id="rId23" display="find maximum product subarray " xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
-    <hyperlink ref="C80" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
-    <hyperlink ref="C81" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
+    <hyperlink ref="C79" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
+    <hyperlink ref="C80" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
     <hyperlink ref="C43" r:id="rId26" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
-    <hyperlink ref="C44" r:id="rId27" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
-    <hyperlink ref="C45" r:id="rId28" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
-    <hyperlink ref="C46" r:id="rId29" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
-    <hyperlink ref="C47" r:id="rId30" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
-    <hyperlink ref="C48" r:id="rId31" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
-    <hyperlink ref="C49" r:id="rId32" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
-    <hyperlink ref="C50" r:id="rId33" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
-    <hyperlink ref="C51" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
-    <hyperlink ref="C52" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
-    <hyperlink ref="C53" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
+    <hyperlink ref="C81" r:id="rId27" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
+    <hyperlink ref="C44" r:id="rId28" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
+    <hyperlink ref="C45" r:id="rId29" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
+    <hyperlink ref="C46" r:id="rId30" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
+    <hyperlink ref="C47" r:id="rId31" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
+    <hyperlink ref="C48" r:id="rId32" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
+    <hyperlink ref="C49" r:id="rId33" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
+    <hyperlink ref="C50" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
+    <hyperlink ref="C51" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
+    <hyperlink ref="C52" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
     <hyperlink ref="C161" r:id="rId37" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
     <hyperlink ref="C162" r:id="rId38" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
     <hyperlink ref="C163" r:id="rId39" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
@@ -9729,16 +9747,16 @@
     <hyperlink ref="C482" r:id="rId386" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
     <hyperlink ref="C481" r:id="rId387" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
     <hyperlink ref="C480" r:id="rId388" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="C55" r:id="rId389" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="C56" r:id="rId390" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="C57" r:id="rId391" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="C58" r:id="rId392" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="C59" r:id="rId393" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="C60" r:id="rId394" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="C61" r:id="rId395" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="C64" r:id="rId396" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="C62" r:id="rId397" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="C63" r:id="rId398" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="C54" r:id="rId389" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="C55" r:id="rId390" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="C56" r:id="rId391" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="C57" r:id="rId392" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="C58" r:id="rId393" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="C59" r:id="rId394" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="C60" r:id="rId395" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="C63" r:id="rId396" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="C61" r:id="rId397" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="C62" r:id="rId398" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="C325" r:id="rId399" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="C120" r:id="rId400" xr:uid="{F0DDC999-C321-4AB4-BA9D-7538150E84D3}"/>
     <hyperlink ref="C9" r:id="rId401" xr:uid="{310D755F-0FAF-4086-8950-B58917F7CAF8}"/>
@@ -9794,16 +9812,16 @@
     <hyperlink ref="C126" r:id="rId451" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
     <hyperlink ref="C125" r:id="rId452" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
     <hyperlink ref="C124" r:id="rId453" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
-    <hyperlink ref="C75" r:id="rId454" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
-    <hyperlink ref="C74" r:id="rId455" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
-    <hyperlink ref="C73" r:id="rId456" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
-    <hyperlink ref="C72" r:id="rId457" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
-    <hyperlink ref="C71" r:id="rId458" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
-    <hyperlink ref="C70" r:id="rId459" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
-    <hyperlink ref="C69" r:id="rId460" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
-    <hyperlink ref="C68" r:id="rId461" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
-    <hyperlink ref="C67" r:id="rId462" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
-    <hyperlink ref="C66" r:id="rId463" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
+    <hyperlink ref="C74" r:id="rId454" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
+    <hyperlink ref="C73" r:id="rId455" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
+    <hyperlink ref="C72" r:id="rId456" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
+    <hyperlink ref="C71" r:id="rId457" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
+    <hyperlink ref="C70" r:id="rId458" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
+    <hyperlink ref="C69" r:id="rId459" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
+    <hyperlink ref="C68" r:id="rId460" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
+    <hyperlink ref="C67" r:id="rId461" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
+    <hyperlink ref="C66" r:id="rId462" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
+    <hyperlink ref="C65" r:id="rId463" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
     <hyperlink ref="K29" r:id="rId464" xr:uid="{03443138-A680-4B72-A76F-ED2F3C418FFF}"/>
     <hyperlink ref="K32" r:id="rId465" xr:uid="{E2846214-1318-4E7F-B406-DB8B8C109F51}"/>
     <hyperlink ref="K33" r:id="rId466" xr:uid="{654A45B7-1C43-48E0-B7BB-03647CB459F1}"/>

</xml_diff>

<commit_message>
Program to Find smallest subarray have greater sum added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D2D386-8DFF-4026-AAF4-11D73D697963}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E16647-E039-42B9-91E1-536DE0D23E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="541">
   <si>
     <t>Topic:</t>
   </si>
@@ -1636,6 +1636,18 @@
   </si>
   <si>
     <t>TSGV1ARR</t>
+  </si>
+  <si>
+    <t>UNDERSTAND</t>
+  </si>
+  <si>
+    <t>PP=Done in GFG Practice Only</t>
+  </si>
+  <si>
+    <t>UNDERSTAND=ONLY UNDERSTANDED LOGIC</t>
+  </si>
+  <si>
+    <t>SSA1ARR</t>
   </si>
 </sst>
 </file>
@@ -1792,7 +1804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1855,6 +1867,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2188,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:K504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2207,12 +2223,21 @@
       <c r="C1" s="12" t="s">
         <v>460</v>
       </c>
+      <c r="D1" s="25" t="s">
+        <v>538</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C2" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="25" t="s">
+        <v>539</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C3" s="12" t="s">
@@ -3083,46 +3108,82 @@
       <c r="A45" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="9"/>
+      <c r="B45" s="9" t="s">
+        <v>487</v>
+      </c>
       <c r="C45" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>462</v>
       </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="20"/>
+      <c r="E45" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="9"/>
+      <c r="B46" s="9" t="s">
+        <v>537</v>
+      </c>
       <c r="C46" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="20"/>
+      <c r="D46" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>521</v>
+      </c>
+      <c r="K46" s="24" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="9"/>
+      <c r="B47" s="9" t="s">
+        <v>540</v>
+      </c>
       <c r="C47" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="E47" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="F47" s="21"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="20"/>
+      <c r="F47" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="H47" s="23" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" s="9" t="s">
@@ -9357,6 +9418,10 @@
       <c r="D504" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C22" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>
@@ -9827,8 +9892,9 @@
     <hyperlink ref="K33" r:id="rId466" xr:uid="{654A45B7-1C43-48E0-B7BB-03647CB459F1}"/>
     <hyperlink ref="K35" r:id="rId467" xr:uid="{BDF59F61-A334-4583-8D5C-080958A57655}"/>
     <hyperlink ref="K36" r:id="rId468" xr:uid="{69563388-281D-4E78-9CB7-84F164525B40}"/>
+    <hyperlink ref="K46" r:id="rId469" xr:uid="{0FFAE0D5-B9D2-4673-9AFA-6C8D93507F0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId469"/>
+  <pageSetup orientation="portrait" r:id="rId470"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Program to count total set bits is added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A12A20-3D89-4001-ABDA-72AA0DFDB5ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911EB541-588B-4BCB-AA6F-968C2182E68A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="546">
   <si>
     <t>Topic:</t>
   </si>
@@ -1656,10 +1656,13 @@
     <t>FSB2BITS</t>
   </si>
   <si>
-    <t>Check Kth Bit is Set or Not</t>
-  </si>
-  <si>
-    <t>KBSON2BITS</t>
+    <t>RDB2BITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Rightmost Difference Bit </t>
+  </si>
+  <si>
+    <t>CTSB2BITS</t>
   </si>
 </sst>
 </file>
@@ -1816,7 +1819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1882,17 +1885,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2225,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:K506"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2244,21 +2244,21 @@
       <c r="C1" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>538</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C2" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>539</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C3" s="12" t="s">
@@ -3243,6 +3243,9 @@
       <c r="D49" s="17" t="s">
         <v>508</v>
       </c>
+      <c r="E49" s="17" t="s">
+        <v>508</v>
+      </c>
       <c r="F49" s="21"/>
       <c r="G49" s="19"/>
       <c r="H49" s="20"/>
@@ -3258,6 +3261,9 @@
       <c r="D50" s="17" t="s">
         <v>508</v>
       </c>
+      <c r="E50" s="17" t="s">
+        <v>508</v>
+      </c>
       <c r="F50" s="21"/>
       <c r="G50" s="19"/>
       <c r="H50" s="20"/>
@@ -3273,6 +3279,9 @@
       <c r="D51" s="17" t="s">
         <v>508</v>
       </c>
+      <c r="E51" s="17" t="s">
+        <v>508</v>
+      </c>
       <c r="F51" s="21"/>
       <c r="G51" s="19"/>
       <c r="H51" s="20"/>
@@ -3286,6 +3295,9 @@
         <v>37</v>
       </c>
       <c r="D52" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="E52" s="17" t="s">
         <v>508</v>
       </c>
       <c r="F52" s="21"/>
@@ -3306,7 +3318,7 @@
       <c r="A54" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="26" t="s">
         <v>542</v>
       </c>
       <c r="C54" s="10" t="s">
@@ -3332,42 +3344,67 @@
       <c r="A55" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="26" t="s">
+        <v>543</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>543</v>
-      </c>
-      <c r="D55" s="13"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
+      <c r="D55" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="G55" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B56" s="27"/>
+      <c r="B56" s="25" t="s">
+        <v>487</v>
+      </c>
       <c r="C56" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
+      <c r="D56" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B57" s="27"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="10" t="s">
         <v>451</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>3</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>508</v>
       </c>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
@@ -3377,12 +3414,15 @@
       <c r="A58" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B58" s="27"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="10" t="s">
         <v>452</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>3</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>508</v>
       </c>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
@@ -3392,22 +3432,33 @@
       <c r="A59" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B59" s="27"/>
+      <c r="B59" s="25" t="s">
+        <v>545</v>
+      </c>
       <c r="C59" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
+      <c r="D59" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B60" s="27"/>
+      <c r="B60" s="25"/>
       <c r="C60" s="10" t="s">
         <v>454</v>
       </c>
@@ -3422,7 +3473,7 @@
       <c r="A61" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B61" s="27"/>
+      <c r="B61" s="25"/>
       <c r="C61" s="10" t="s">
         <v>455</v>
       </c>
@@ -3437,7 +3488,7 @@
       <c r="A62" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B62" s="27"/>
+      <c r="B62" s="25"/>
       <c r="C62" s="10" t="s">
         <v>456</v>
       </c>
@@ -3452,7 +3503,7 @@
       <c r="A63" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B63" s="27"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="10" t="s">
         <v>457</v>
       </c>
@@ -3467,7 +3518,7 @@
       <c r="A64" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B64" s="27"/>
+      <c r="B64" s="25"/>
       <c r="C64" s="10" t="s">
         <v>458</v>
       </c>
@@ -3482,7 +3533,7 @@
       <c r="A65" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B65" s="27"/>
+      <c r="B65" s="25"/>
       <c r="C65" s="10" t="s">
         <v>459</v>
       </c>
@@ -3495,7 +3546,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="9"/>
-      <c r="B66" s="27"/>
+      <c r="B66" s="25"/>
       <c r="D66" s="7"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
@@ -3505,7 +3556,7 @@
       <c r="A67" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="28"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="10" t="s">
         <v>39</v>
       </c>
@@ -3520,7 +3571,7 @@
       <c r="A68" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="28"/>
+      <c r="B68" s="26"/>
       <c r="C68" s="10" t="s">
         <v>40</v>
       </c>
@@ -3535,7 +3586,7 @@
       <c r="A69" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="28"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="10" t="s">
         <v>41</v>
       </c>
@@ -3550,7 +3601,7 @@
       <c r="A70" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="28"/>
+      <c r="B70" s="26"/>
       <c r="C70" s="10" t="s">
         <v>42</v>
       </c>
@@ -3565,7 +3616,7 @@
       <c r="A71" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B71" s="28"/>
+      <c r="B71" s="26"/>
       <c r="C71" s="10" t="s">
         <v>43</v>
       </c>
@@ -3580,7 +3631,7 @@
       <c r="A72" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B72" s="28"/>
+      <c r="B72" s="26"/>
       <c r="C72" s="10" t="s">
         <v>44</v>
       </c>
@@ -3595,7 +3646,7 @@
       <c r="A73" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="28"/>
+      <c r="B73" s="26"/>
       <c r="C73" s="10" t="s">
         <v>45</v>
       </c>
@@ -3610,7 +3661,7 @@
       <c r="A74" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B74" s="28"/>
+      <c r="B74" s="26"/>
       <c r="C74" s="10" t="s">
         <v>46</v>
       </c>
@@ -3625,7 +3676,7 @@
       <c r="A75" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="28"/>
+      <c r="B75" s="26"/>
       <c r="C75" s="10" t="s">
         <v>47</v>
       </c>
@@ -3640,7 +3691,7 @@
       <c r="A76" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="28"/>
+      <c r="B76" s="26"/>
       <c r="C76" s="10" t="s">
         <v>48</v>
       </c>
@@ -3655,7 +3706,7 @@
       <c r="A77" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B77" s="27"/>
+      <c r="B77" s="25"/>
       <c r="C77" s="10" t="s">
         <v>18</v>
       </c>
@@ -3668,7 +3719,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="9"/>
-      <c r="B78" s="27"/>
+      <c r="B78" s="25"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
       <c r="E78" s="10"/>
@@ -3680,7 +3731,7 @@
       <c r="A79" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B79" s="27"/>
+      <c r="B79" s="25"/>
       <c r="C79" s="10" t="s">
         <v>22</v>
       </c>
@@ -3695,7 +3746,7 @@
       <c r="A80" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B80" s="27" t="s">
+      <c r="B80" s="25" t="s">
         <v>530</v>
       </c>
       <c r="C80" s="10" t="s">
@@ -3712,7 +3763,7 @@
       <c r="A81" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B81" s="27"/>
+      <c r="B81" s="25"/>
       <c r="C81" s="10" t="s">
         <v>25</v>
       </c>
@@ -3730,7 +3781,7 @@
       <c r="A82" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B82" s="27"/>
+      <c r="B82" s="25"/>
       <c r="C82" s="10" t="s">
         <v>26</v>
       </c>
@@ -3745,7 +3796,7 @@
       <c r="A83" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B83" s="27" t="s">
+      <c r="B83" s="25" t="s">
         <v>535</v>
       </c>
       <c r="C83" s="10" t="s">
@@ -3760,7 +3811,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A84" s="9"/>
-      <c r="B84" s="27"/>
+      <c r="B84" s="25"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
@@ -3772,7 +3823,7 @@
       <c r="A85" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B85" s="27"/>
+      <c r="B85" s="25"/>
       <c r="C85" s="10" t="s">
         <v>94</v>
       </c>
@@ -3787,7 +3838,7 @@
       <c r="A86" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B86" s="27"/>
+      <c r="B86" s="25"/>
       <c r="C86" s="10" t="s">
         <v>95</v>
       </c>
@@ -3802,7 +3853,7 @@
       <c r="A87" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="27"/>
+      <c r="B87" s="25"/>
       <c r="C87" s="10" t="s">
         <v>96</v>
       </c>
@@ -3817,7 +3868,7 @@
       <c r="A88" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="27"/>
+      <c r="B88" s="25"/>
       <c r="C88" s="10" t="s">
         <v>97</v>
       </c>
@@ -3832,7 +3883,7 @@
       <c r="A89" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B89" s="27"/>
+      <c r="B89" s="25"/>
       <c r="C89" s="10" t="s">
         <v>98</v>
       </c>
@@ -3847,7 +3898,7 @@
       <c r="A90" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="27"/>
+      <c r="B90" s="25"/>
       <c r="C90" s="10" t="s">
         <v>99</v>
       </c>
@@ -3862,7 +3913,7 @@
       <c r="A91" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="27"/>
+      <c r="B91" s="25"/>
       <c r="C91" s="10" t="s">
         <v>100</v>
       </c>
@@ -3877,7 +3928,7 @@
       <c r="A92" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="27"/>
+      <c r="B92" s="25"/>
       <c r="C92" s="10" t="s">
         <v>101</v>
       </c>
@@ -3892,7 +3943,7 @@
       <c r="A93" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="27"/>
+      <c r="B93" s="25"/>
       <c r="C93" s="10" t="s">
         <v>102</v>
       </c>
@@ -3907,7 +3958,7 @@
       <c r="A94" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="27"/>
+      <c r="B94" s="25"/>
       <c r="C94" s="10" t="s">
         <v>103</v>
       </c>
@@ -3922,7 +3973,7 @@
       <c r="A95" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="27"/>
+      <c r="B95" s="25"/>
       <c r="C95" s="10" t="s">
         <v>104</v>
       </c>
@@ -3937,7 +3988,7 @@
       <c r="A96" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B96" s="27"/>
+      <c r="B96" s="25"/>
       <c r="C96" s="10" t="s">
         <v>105</v>
       </c>
@@ -3952,7 +4003,7 @@
       <c r="A97" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B97" s="27"/>
+      <c r="B97" s="25"/>
       <c r="C97" s="10" t="s">
         <v>106</v>
       </c>
@@ -3967,7 +4018,7 @@
       <c r="A98" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B98" s="27"/>
+      <c r="B98" s="25"/>
       <c r="C98" s="10" t="s">
         <v>107</v>
       </c>
@@ -3982,7 +4033,7 @@
       <c r="A99" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B99" s="27"/>
+      <c r="B99" s="25"/>
       <c r="C99" s="10" t="s">
         <v>108</v>
       </c>
@@ -3997,7 +4048,7 @@
       <c r="A100" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B100" s="27"/>
+      <c r="B100" s="25"/>
       <c r="C100" s="10" t="s">
         <v>109</v>
       </c>
@@ -4012,7 +4063,7 @@
       <c r="A101" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B101" s="27"/>
+      <c r="B101" s="25"/>
       <c r="C101" s="10" t="s">
         <v>110</v>
       </c>
@@ -4027,7 +4078,7 @@
       <c r="A102" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B102" s="27"/>
+      <c r="B102" s="25"/>
       <c r="C102" s="10" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Program to Find Whether Number is power of 2 or not Added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911EB541-588B-4BCB-AA6F-968C2182E68A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA96AE3E-DA4C-4ABB-8DDB-952D9083FEBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="547">
   <si>
     <t>Topic:</t>
   </si>
@@ -1404,9 +1404,6 @@
     <t>Calculate square of a number without using *, / and pow()</t>
   </si>
   <si>
-    <t>Power Set</t>
-  </si>
-  <si>
     <t>DSA CheatSheet</t>
   </si>
   <si>
@@ -1663,6 +1660,12 @@
   </si>
   <si>
     <t>CTSB2BITS</t>
+  </si>
+  <si>
+    <t>Power Set (THIS QUESTION CAN ONLY BE DONE IN C++), BECAUSE IN JAVA STRINGS ARE IMMUTABLR</t>
+  </si>
+  <si>
+    <t>POT2BITS</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2229,7 @@
   <dimension ref="A1:K506"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2242,27 +2245,27 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C1" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C2" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C3" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -2278,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -2287,19 +2290,19 @@
         <v>2</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F6" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>516</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>517</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>518</v>
-      </c>
       <c r="K6" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -2311,41 +2314,41 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>464</v>
-      </c>
       <c r="D8" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="19"/>
@@ -2353,19 +2356,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="19"/>
@@ -2373,19 +2376,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="19"/>
@@ -2393,19 +2396,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="19"/>
@@ -2413,19 +2416,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="19"/>
@@ -2433,19 +2436,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>474</v>
-      </c>
       <c r="D14" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="19"/>
@@ -2453,19 +2456,19 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>476</v>
-      </c>
       <c r="D15" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="19"/>
@@ -2473,19 +2476,19 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="19"/>
@@ -2493,19 +2496,19 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="19"/>
@@ -2513,19 +2516,19 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="19"/>
@@ -2533,19 +2536,19 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="19"/>
@@ -2565,16 +2568,16 @@
         <v>4</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="19"/>
@@ -2585,16 +2588,16 @@
         <v>4</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="19"/>
@@ -2605,16 +2608,16 @@
         <v>4</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="19"/>
@@ -2625,16 +2628,16 @@
         <v>4</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="19"/>
@@ -2645,16 +2648,16 @@
         <v>4</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="19"/>
@@ -2665,16 +2668,16 @@
         <v>4</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="19"/>
@@ -2685,16 +2688,16 @@
         <v>4</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="19"/>
@@ -2705,22 +2708,22 @@
         <v>4</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="19"/>
       <c r="H29" s="20"/>
       <c r="K29" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.4">
@@ -2728,25 +2731,25 @@
         <v>4</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H30" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
@@ -2754,25 +2757,25 @@
         <v>4</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H31" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.4">
@@ -2780,28 +2783,28 @@
         <v>4</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H32" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
@@ -2809,28 +2812,28 @@
         <v>4</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H33" s="23" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
@@ -2838,25 +2841,25 @@
         <v>4</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H34" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
@@ -2864,28 +2867,28 @@
         <v>4</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H35" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
@@ -2893,28 +2896,28 @@
         <v>4</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H36" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
@@ -2922,25 +2925,25 @@
         <v>4</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H37" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
@@ -2948,25 +2951,25 @@
         <v>4</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H38" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
@@ -2974,25 +2977,25 @@
         <v>4</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H39" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
@@ -3000,25 +3003,25 @@
         <v>4</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>527</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>528</v>
-      </c>
       <c r="D40" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H40" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
@@ -3026,25 +3029,25 @@
         <v>4</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
@@ -3052,25 +3055,25 @@
         <v>4</v>
       </c>
       <c r="B42" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>532</v>
-      </c>
       <c r="D42" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
@@ -3078,25 +3081,25 @@
         <v>4</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H43" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
@@ -3104,25 +3107,25 @@
         <v>4</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H44" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
@@ -3130,25 +3133,25 @@
         <v>4</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H45" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
@@ -3156,28 +3159,28 @@
         <v>4</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K46" s="24" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
@@ -3185,25 +3188,25 @@
         <v>4</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
@@ -3211,28 +3214,28 @@
         <v>4</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" s="9" t="s">
         <v>4</v>
       </c>
@@ -3241,16 +3244,16 @@
         <v>34</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="19"/>
       <c r="H49" s="20"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" s="9" t="s">
         <v>4</v>
       </c>
@@ -3259,16 +3262,16 @@
         <v>35</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="19"/>
       <c r="H50" s="20"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" s="9" t="s">
         <v>4</v>
       </c>
@@ -3277,16 +3280,16 @@
         <v>36</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="19"/>
       <c r="H51" s="20"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A52" s="9" t="s">
         <v>4</v>
       </c>
@@ -3295,16 +3298,16 @@
         <v>37</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F52" s="21"/>
       <c r="G52" s="19"/>
       <c r="H52" s="20"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="10"/>
@@ -3314,103 +3317,111 @@
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" s="9" t="s">
         <v>449</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A55" s="9" t="s">
         <v>449</v>
       </c>
       <c r="B55" s="26" t="s">
+        <v>542</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>544</v>
-      </c>
       <c r="D55" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H55" s="23" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A56" s="9" t="s">
         <v>449</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>450</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H56" s="23" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A57" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="25" t="s">
+        <v>486</v>
+      </c>
       <c r="C57" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>3</v>
+      <c r="D57" s="15" t="s">
+        <v>461</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+        <v>507</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A58" s="9" t="s">
         <v>449</v>
       </c>
@@ -3422,54 +3433,68 @@
         <v>3</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A59" s="9" t="s">
         <v>449</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>453</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E59" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H59" s="23" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+        <v>517</v>
+      </c>
+      <c r="K59" s="10" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A60" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B60" s="25"/>
+      <c r="B60" s="25" t="s">
+        <v>546</v>
+      </c>
       <c r="C60" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D60" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A61" s="9" t="s">
         <v>449</v>
       </c>
@@ -3484,7 +3509,7 @@
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A62" s="9" t="s">
         <v>449</v>
       </c>
@@ -3499,7 +3524,7 @@
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A63" s="9" t="s">
         <v>449</v>
       </c>
@@ -3514,7 +3539,7 @@
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A64" s="9" t="s">
         <v>449</v>
       </c>
@@ -3533,16 +3558,27 @@
       <c r="A65" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B65" s="25"/>
+      <c r="B65" s="25" t="s">
+        <v>536</v>
+      </c>
       <c r="C65" s="10" t="s">
-        <v>459</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
+        <v>545</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="G65" s="22" t="s">
+        <v>516</v>
+      </c>
+      <c r="H65" s="23" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="9"/>
@@ -3711,7 +3747,7 @@
         <v>18</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F77" s="21"/>
       <c r="G77" s="19"/>
@@ -3729,14 +3765,14 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B79" s="25"/>
       <c r="C79" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F79" s="21"/>
       <c r="G79" s="19"/>
@@ -3744,16 +3780,16 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A80" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F80" s="21"/>
       <c r="G80" s="19"/>
@@ -3761,14 +3797,14 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B81" s="25"/>
       <c r="C81" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F81" s="21"/>
       <c r="G81" s="19"/>
@@ -3779,14 +3815,14 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A82" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B82" s="25"/>
       <c r="C82" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F82" s="21"/>
       <c r="G82" s="19"/>
@@ -3794,16 +3830,16 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A83" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F83" s="21"/>
       <c r="G83" s="19"/>
@@ -4364,13 +4400,13 @@
         <v>93</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F121" s="12"/>
       <c r="G121" s="12"/>
@@ -4381,13 +4417,13 @@
         <v>93</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F122" s="12"/>
       <c r="G122" s="12"/>
@@ -4398,7 +4434,7 @@
         <v>93</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>7</v>
@@ -4419,7 +4455,7 @@
         <v>20</v>
       </c>
       <c r="D124" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F124" s="21"/>
       <c r="G124" s="19"/>
@@ -9409,25 +9445,25 @@
         <v>389</v>
       </c>
       <c r="B489" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C489" s="10" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D489" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E489" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F489" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G489" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H489" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="490" spans="1:9" x14ac:dyDescent="0.4">
@@ -9947,7 +9983,7 @@
     <hyperlink ref="C60" r:id="rId393" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
     <hyperlink ref="C61" r:id="rId394" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
     <hyperlink ref="C62" r:id="rId395" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="C65" r:id="rId396" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="C65" r:id="rId396" display="Power Set" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
     <hyperlink ref="C63" r:id="rId397" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
     <hyperlink ref="C64" r:id="rId398" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="C327" r:id="rId399" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
@@ -10023,8 +10059,9 @@
     <hyperlink ref="K46" r:id="rId469" xr:uid="{0FFAE0D5-B9D2-4673-9AFA-6C8D93507F0D}"/>
     <hyperlink ref="C54" r:id="rId470" xr:uid="{398562CF-08D2-49BF-9B88-E010B2218981}"/>
     <hyperlink ref="C55" r:id="rId471" xr:uid="{7C1954A5-BE1A-4C08-8F55-696C8CA140C2}"/>
+    <hyperlink ref="K59" r:id="rId472" xr:uid="{A369B69D-75A6-46BE-A60D-5CF05EDC7715}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId472"/>
+  <pageSetup orientation="portrait" r:id="rId473"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Program to count how may bits need to flip to make a as b Added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA96AE3E-DA4C-4ABB-8DDB-952D9083FEBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914E6315-1E13-402F-A2A2-E9DC3356E95C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="548">
   <si>
     <t>Topic:</t>
   </si>
@@ -1666,6 +1666,9 @@
   </si>
   <si>
     <t>POT2BITS</t>
+  </si>
+  <si>
+    <t>NOBTF2BITS</t>
   </si>
 </sst>
 </file>
@@ -2229,7 +2232,7 @@
   <dimension ref="A1:K506"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -3425,19 +3428,27 @@
       <c r="A58" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="25" t="s">
+        <v>547</v>
+      </c>
       <c r="C58" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>3</v>
+      <c r="D58" s="15" t="s">
+        <v>461</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
+      <c r="F58" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A59" s="9" t="s">
@@ -3498,16 +3509,27 @@
       <c r="A61" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B61" s="25"/>
+      <c r="B61" s="25" t="s">
+        <v>536</v>
+      </c>
       <c r="C61" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
+      <c r="D61" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A62" s="9" t="s">

</xml_diff>

<commit_message>
Program to find element in matrix
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914E6315-1E13-402F-A2A2-E9DC3356E95C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656D0660-24B5-4425-B3C5-3C868A6E15F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="549">
   <si>
     <t>Topic:</t>
   </si>
@@ -1669,6 +1669,9 @@
   </si>
   <si>
     <t>NOBTF2BITS</t>
+  </si>
+  <si>
+    <t>SEIM3MAT</t>
   </si>
 </sst>
 </file>
@@ -1756,7 +1759,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1801,12 +1804,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF990099"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF33CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1825,7 +1822,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1867,9 +1864,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2231,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:K506"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2250,21 +2244,21 @@
       <c r="C1" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>537</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C2" s="12" t="s">
         <v>490</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>538</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C3" s="12" t="s">
@@ -2328,14 +2322,14 @@
       <c r="D8" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
@@ -2350,12 +2344,12 @@
       <c r="D9" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
@@ -2370,12 +2364,12 @@
       <c r="D10" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
@@ -2390,12 +2384,12 @@
       <c r="D11" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
@@ -2410,12 +2404,12 @@
       <c r="D12" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
@@ -2430,12 +2424,12 @@
       <c r="D13" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
@@ -2450,12 +2444,12 @@
       <c r="D14" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
@@ -2470,12 +2464,12 @@
       <c r="D15" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
@@ -2490,12 +2484,12 @@
       <c r="D16" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
@@ -2510,12 +2504,12 @@
       <c r="D17" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
@@ -2530,12 +2524,12 @@
       <c r="D18" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
@@ -2550,12 +2544,12 @@
       <c r="D19" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="12"/>
@@ -2582,9 +2576,9 @@
       <c r="E22" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
@@ -2602,9 +2596,9 @@
       <c r="E23" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="9" t="s">
@@ -2622,9 +2616,9 @@
       <c r="E24" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" s="9" t="s">
@@ -2642,9 +2636,9 @@
       <c r="E25" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="9" t="s">
@@ -2662,9 +2656,9 @@
       <c r="E26" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="9" t="s">
@@ -2682,9 +2676,9 @@
       <c r="E27" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
@@ -2699,12 +2693,12 @@
       <c r="D28" s="15" t="s">
         <v>509</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A29" s="9" t="s">
@@ -2719,12 +2713,12 @@
       <c r="D29" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
       <c r="K29" s="10" t="s">
         <v>510</v>
       </c>
@@ -2745,13 +2739,13 @@
       <c r="E30" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -2771,13 +2765,13 @@
       <c r="E31" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H31" s="23" t="s">
+      <c r="H31" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -2797,13 +2791,13 @@
       <c r="E32" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H32" s="23" t="s">
+      <c r="H32" s="22" t="s">
         <v>517</v>
       </c>
       <c r="K32" s="10" t="s">
@@ -2820,19 +2814,19 @@
       <c r="C33" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H33" s="23" t="s">
+      <c r="H33" s="22" t="s">
         <v>519</v>
       </c>
       <c r="K33" s="10" t="s">
@@ -2855,13 +2849,13 @@
       <c r="E34" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H34" s="23" t="s">
+      <c r="H34" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -2881,13 +2875,13 @@
       <c r="E35" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G35" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="H35" s="22" t="s">
         <v>520</v>
       </c>
       <c r="K35" s="10" t="s">
@@ -2910,13 +2904,13 @@
       <c r="E36" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H36" s="23" t="s">
+      <c r="H36" s="22" t="s">
         <v>517</v>
       </c>
       <c r="K36" s="10" t="s">
@@ -2939,13 +2933,13 @@
       <c r="E37" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="H37" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -2965,13 +2959,13 @@
       <c r="E38" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="F38" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H38" s="23" t="s">
+      <c r="H38" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -2991,13 +2985,13 @@
       <c r="E39" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="G39" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H39" s="23" t="s">
+      <c r="H39" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3017,13 +3011,13 @@
       <c r="E40" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G40" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H40" s="23" t="s">
+      <c r="H40" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3043,13 +3037,13 @@
       <c r="E41" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H41" s="23" t="s">
+      <c r="H41" s="22" t="s">
         <v>517</v>
       </c>
     </row>
@@ -3066,16 +3060,16 @@
       <c r="D42" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="F42" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H42" s="23" t="s">
+      <c r="H42" s="22" t="s">
         <v>517</v>
       </c>
     </row>
@@ -3092,16 +3086,16 @@
       <c r="D43" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="G43" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H43" s="23" t="s">
+      <c r="H43" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3118,16 +3112,16 @@
       <c r="D44" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F44" s="21" t="s">
+      <c r="F44" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="G44" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H44" s="23" t="s">
+      <c r="H44" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3144,16 +3138,16 @@
       <c r="D45" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F45" s="21" t="s">
+      <c r="F45" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="G45" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>517</v>
       </c>
     </row>
@@ -3170,19 +3164,19 @@
       <c r="D46" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="G46" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>520</v>
       </c>
-      <c r="K46" s="24" t="s">
+      <c r="K46" s="23" t="s">
         <v>511</v>
       </c>
     </row>
@@ -3199,16 +3193,16 @@
       <c r="D47" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="E47" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G47" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H47" s="23" t="s">
+      <c r="H47" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3225,16 +3219,16 @@
       <c r="D48" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F48" s="18" t="s">
+      <c r="F48" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G48" s="19" t="s">
+      <c r="G48" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H48" s="23" t="s">
+      <c r="H48" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3246,15 +3240,15 @@
       <c r="C49" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="19"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" s="9" t="s">
@@ -3264,15 +3258,15 @@
       <c r="C50" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E50" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F50" s="21"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="19"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" s="9" t="s">
@@ -3282,15 +3276,15 @@
       <c r="C51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E51" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F51" s="21"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A52" s="9" t="s">
@@ -3300,15 +3294,15 @@
       <c r="C52" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F52" s="21"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="19"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" s="9"/>
@@ -3324,7 +3318,7 @@
       <c r="A54" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="25" t="s">
         <v>541</v>
       </c>
       <c r="C54" s="10" t="s">
@@ -3333,16 +3327,16 @@
       <c r="D54" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F54" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H54" s="23" t="s">
+      <c r="H54" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3350,7 +3344,7 @@
       <c r="A55" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="25" t="s">
         <v>542</v>
       </c>
       <c r="C55" s="10" t="s">
@@ -3359,16 +3353,16 @@
       <c r="D55" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="F55" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G55" s="19" t="s">
+      <c r="G55" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H55" s="23" t="s">
+      <c r="H55" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3376,7 +3370,7 @@
       <c r="A56" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="24" t="s">
         <v>486</v>
       </c>
       <c r="C56" s="10" t="s">
@@ -3385,16 +3379,16 @@
       <c r="D56" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F56" s="18" t="s">
+      <c r="F56" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G56" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H56" s="23" t="s">
+      <c r="H56" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3402,7 +3396,7 @@
       <c r="A57" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B57" s="25" t="s">
+      <c r="B57" s="24" t="s">
         <v>486</v>
       </c>
       <c r="C57" s="10" t="s">
@@ -3411,16 +3405,16 @@
       <c r="D57" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E57" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F57" s="21" t="s">
+      <c r="F57" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="G57" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H57" s="23" t="s">
+      <c r="H57" s="22" t="s">
         <v>517</v>
       </c>
     </row>
@@ -3428,7 +3422,7 @@
       <c r="A58" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="24" t="s">
         <v>547</v>
       </c>
       <c r="C58" s="10" t="s">
@@ -3437,16 +3431,16 @@
       <c r="D58" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E58" s="17" t="s">
+      <c r="E58" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F58" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="G58" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H58" s="23" t="s">
+      <c r="H58" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3454,7 +3448,7 @@
       <c r="A59" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="B59" s="24" t="s">
         <v>544</v>
       </c>
       <c r="C59" s="10" t="s">
@@ -3463,16 +3457,16 @@
       <c r="D59" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E59" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F59" s="21" t="s">
+      <c r="F59" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="G59" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H59" s="23" t="s">
+      <c r="H59" s="22" t="s">
         <v>517</v>
       </c>
       <c r="K59" s="10" t="s">
@@ -3483,7 +3477,7 @@
       <c r="A60" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B60" s="25" t="s">
+      <c r="B60" s="24" t="s">
         <v>546</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -3492,16 +3486,16 @@
       <c r="D60" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F60" s="18" t="s">
+      <c r="F60" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H60" s="23" t="s">
+      <c r="H60" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3509,7 +3503,7 @@
       <c r="A61" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="24" t="s">
         <v>536</v>
       </c>
       <c r="C61" s="10" t="s">
@@ -3518,16 +3512,16 @@
       <c r="D61" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E61" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F61" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H61" s="23" t="s">
+      <c r="H61" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -3535,7 +3529,7 @@
       <c r="A62" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B62" s="25"/>
+      <c r="B62" s="24"/>
       <c r="C62" s="10" t="s">
         <v>456</v>
       </c>
@@ -3550,7 +3544,7 @@
       <c r="A63" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B63" s="25"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="10" t="s">
         <v>457</v>
       </c>
@@ -3565,7 +3559,7 @@
       <c r="A64" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B64" s="25"/>
+      <c r="B64" s="24"/>
       <c r="C64" s="10" t="s">
         <v>458</v>
       </c>
@@ -3580,31 +3574,31 @@
       <c r="A65" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="24" t="s">
         <v>536</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>545</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="E65" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F65" s="21" t="s">
+      <c r="F65" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G65" s="22" t="s">
+      <c r="G65" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="H65" s="23" t="s">
+      <c r="H65" s="22" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="9"/>
-      <c r="B66" s="25"/>
+      <c r="B66" s="24"/>
       <c r="D66" s="7"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
@@ -3614,7 +3608,7 @@
       <c r="A67" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="26"/>
+      <c r="B67" s="25"/>
       <c r="C67" s="10" t="s">
         <v>39</v>
       </c>
@@ -3629,22 +3623,33 @@
       <c r="A68" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="26"/>
+      <c r="B68" s="25" t="s">
+        <v>548</v>
+      </c>
       <c r="C68" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
+      <c r="D68" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>520</v>
+      </c>
+      <c r="G68" s="21" t="s">
+        <v>516</v>
+      </c>
+      <c r="H68" s="22" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="26"/>
+      <c r="B69" s="25"/>
       <c r="C69" s="10" t="s">
         <v>41</v>
       </c>
@@ -3659,7 +3664,7 @@
       <c r="A70" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="26"/>
+      <c r="B70" s="25"/>
       <c r="C70" s="10" t="s">
         <v>42</v>
       </c>
@@ -3674,7 +3679,7 @@
       <c r="A71" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B71" s="26"/>
+      <c r="B71" s="25"/>
       <c r="C71" s="10" t="s">
         <v>43</v>
       </c>
@@ -3689,7 +3694,7 @@
       <c r="A72" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B72" s="26"/>
+      <c r="B72" s="25"/>
       <c r="C72" s="10" t="s">
         <v>44</v>
       </c>
@@ -3704,7 +3709,7 @@
       <c r="A73" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="26"/>
+      <c r="B73" s="25"/>
       <c r="C73" s="10" t="s">
         <v>45</v>
       </c>
@@ -3719,7 +3724,7 @@
       <c r="A74" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B74" s="26"/>
+      <c r="B74" s="25"/>
       <c r="C74" s="10" t="s">
         <v>46</v>
       </c>
@@ -3734,7 +3739,7 @@
       <c r="A75" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="26"/>
+      <c r="B75" s="25"/>
       <c r="C75" s="10" t="s">
         <v>47</v>
       </c>
@@ -3749,7 +3754,7 @@
       <c r="A76" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="26"/>
+      <c r="B76" s="25"/>
       <c r="C76" s="10" t="s">
         <v>48</v>
       </c>
@@ -3764,20 +3769,20 @@
       <c r="A77" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B77" s="25"/>
+      <c r="B77" s="24"/>
       <c r="C77" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D77" s="17" t="s">
+      <c r="D77" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F77" s="21"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="19"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="9"/>
-      <c r="B78" s="25"/>
+      <c r="B78" s="24"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
       <c r="E78" s="10"/>
@@ -3789,48 +3794,48 @@
       <c r="A79" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B79" s="25"/>
+      <c r="B79" s="24"/>
       <c r="C79" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D79" s="17" t="s">
+      <c r="D79" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F79" s="21"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="19"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A80" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B80" s="25" t="s">
+      <c r="B80" s="24" t="s">
         <v>529</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D80" s="17" t="s">
+      <c r="D80" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F80" s="21"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="19"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B81" s="25"/>
+      <c r="B81" s="24"/>
       <c r="C81" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D81" s="17" t="s">
+      <c r="D81" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F81" s="21"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="19"/>
       <c r="I81" s="10"/>
       <c r="J81" s="10"/>
       <c r="K81" s="10"/>
@@ -3839,37 +3844,37 @@
       <c r="A82" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B82" s="25"/>
+      <c r="B82" s="24"/>
       <c r="C82" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D82" s="17" t="s">
+      <c r="D82" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F82" s="21"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="19"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A83" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B83" s="25" t="s">
+      <c r="B83" s="24" t="s">
         <v>534</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D83" s="17" t="s">
+      <c r="D83" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F83" s="21"/>
-      <c r="G83" s="19"/>
-      <c r="H83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="19"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A84" s="9"/>
-      <c r="B84" s="25"/>
+      <c r="B84" s="24"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
@@ -3881,7 +3886,7 @@
       <c r="A85" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B85" s="25"/>
+      <c r="B85" s="24"/>
       <c r="C85" s="10" t="s">
         <v>94</v>
       </c>
@@ -3896,7 +3901,7 @@
       <c r="A86" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B86" s="25"/>
+      <c r="B86" s="24"/>
       <c r="C86" s="10" t="s">
         <v>95</v>
       </c>
@@ -3911,7 +3916,7 @@
       <c r="A87" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="25"/>
+      <c r="B87" s="24"/>
       <c r="C87" s="10" t="s">
         <v>96</v>
       </c>
@@ -3926,7 +3931,7 @@
       <c r="A88" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="25"/>
+      <c r="B88" s="24"/>
       <c r="C88" s="10" t="s">
         <v>97</v>
       </c>
@@ -3941,7 +3946,7 @@
       <c r="A89" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B89" s="25"/>
+      <c r="B89" s="24"/>
       <c r="C89" s="10" t="s">
         <v>98</v>
       </c>
@@ -3956,7 +3961,7 @@
       <c r="A90" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="25"/>
+      <c r="B90" s="24"/>
       <c r="C90" s="10" t="s">
         <v>99</v>
       </c>
@@ -3971,7 +3976,7 @@
       <c r="A91" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="25"/>
+      <c r="B91" s="24"/>
       <c r="C91" s="10" t="s">
         <v>100</v>
       </c>
@@ -3986,7 +3991,7 @@
       <c r="A92" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="25"/>
+      <c r="B92" s="24"/>
       <c r="C92" s="10" t="s">
         <v>101</v>
       </c>
@@ -4001,7 +4006,7 @@
       <c r="A93" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="25"/>
+      <c r="B93" s="24"/>
       <c r="C93" s="10" t="s">
         <v>102</v>
       </c>
@@ -4016,7 +4021,7 @@
       <c r="A94" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="25"/>
+      <c r="B94" s="24"/>
       <c r="C94" s="10" t="s">
         <v>103</v>
       </c>
@@ -4031,7 +4036,7 @@
       <c r="A95" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="25"/>
+      <c r="B95" s="24"/>
       <c r="C95" s="10" t="s">
         <v>104</v>
       </c>
@@ -4046,7 +4051,7 @@
       <c r="A96" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B96" s="25"/>
+      <c r="B96" s="24"/>
       <c r="C96" s="10" t="s">
         <v>105</v>
       </c>
@@ -4061,7 +4066,7 @@
       <c r="A97" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B97" s="25"/>
+      <c r="B97" s="24"/>
       <c r="C97" s="10" t="s">
         <v>106</v>
       </c>
@@ -4076,7 +4081,7 @@
       <c r="A98" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B98" s="25"/>
+      <c r="B98" s="24"/>
       <c r="C98" s="10" t="s">
         <v>107</v>
       </c>
@@ -4091,7 +4096,7 @@
       <c r="A99" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B99" s="25"/>
+      <c r="B99" s="24"/>
       <c r="C99" s="10" t="s">
         <v>108</v>
       </c>
@@ -4106,7 +4111,7 @@
       <c r="A100" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B100" s="25"/>
+      <c r="B100" s="24"/>
       <c r="C100" s="10" t="s">
         <v>109</v>
       </c>
@@ -4121,7 +4126,7 @@
       <c r="A101" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B101" s="25"/>
+      <c r="B101" s="24"/>
       <c r="C101" s="10" t="s">
         <v>110</v>
       </c>
@@ -4136,7 +4141,7 @@
       <c r="A102" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B102" s="25"/>
+      <c r="B102" s="24"/>
       <c r="C102" s="10" t="s">
         <v>111</v>
       </c>
@@ -4476,12 +4481,12 @@
       <c r="C124" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D124" s="17" t="s">
+      <c r="D124" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F124" s="21"/>
-      <c r="G124" s="19"/>
-      <c r="H124" s="20"/>
+      <c r="F124" s="20"/>
+      <c r="G124" s="18"/>
+      <c r="H124" s="19"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A125" s="9"/>
@@ -9472,19 +9477,19 @@
       <c r="C489" s="10" t="s">
         <v>532</v>
       </c>
-      <c r="D489" s="17" t="s">
+      <c r="D489" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="E489" s="17" t="s">
+      <c r="E489" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="F489" s="21" t="s">
+      <c r="F489" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="G489" s="19" t="s">
+      <c r="G489" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H489" s="23" t="s">
+      <c r="H489" s="22" t="s">
         <v>517</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Program to find one string is subsequence of another or not added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AF6C99-DA7B-4FEE-9FDF-2527369D5F36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277B750F-2618-4300-A434-5A1CECB5E451}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="571">
   <si>
     <t>Topic:</t>
   </si>
@@ -2300,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:M511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116:H116"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -5111,7 +5111,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A129" s="9"/>
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
@@ -5121,97 +5121,166 @@
       <c r="G129" s="10"/>
       <c r="H129" s="10"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A130" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B130" s="9"/>
+      <c r="B130" s="9" t="s">
+        <v>479</v>
+      </c>
       <c r="C130" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D130" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F130" s="12"/>
-      <c r="G130" s="12"/>
-      <c r="H130" s="12"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D130" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E130" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F130" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G130" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H130" s="22" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A131" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B131" s="9"/>
+      <c r="B131" s="9" t="s">
+        <v>479</v>
+      </c>
       <c r="C131" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D131" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F131" s="12"/>
-      <c r="G131" s="12"/>
-      <c r="H131" s="12"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D131" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E131" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F131" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G131" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H131" s="22" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A132" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B132" s="9"/>
+      <c r="B132" s="9" t="s">
+        <v>528</v>
+      </c>
       <c r="C132" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D132" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F132" s="12"/>
-      <c r="G132" s="12"/>
-      <c r="H132" s="12"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D132" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E132" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F132" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G132" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H132" s="22" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A133" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B133" s="9"/>
+      <c r="B133" s="9" t="s">
+        <v>528</v>
+      </c>
       <c r="C133" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D133" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F133" s="12"/>
-      <c r="G133" s="12"/>
-      <c r="H133" s="12"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D133" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E133" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F133" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G133" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H133" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="K133" s="10" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A134" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B134" s="9"/>
+      <c r="B134" s="9" t="s">
+        <v>528</v>
+      </c>
       <c r="C134" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D134" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F134" s="12"/>
-      <c r="G134" s="12"/>
-      <c r="H134" s="12"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D134" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E134" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F134" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G134" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H134" s="22" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A135" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B135" s="9"/>
+      <c r="B135" s="9" t="s">
+        <v>528</v>
+      </c>
       <c r="C135" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D135" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F135" s="12"/>
-      <c r="G135" s="12"/>
-      <c r="H135" s="12"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D135" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E135" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F135" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G135" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H135" s="22" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A136" s="9" t="s">
         <v>49</v>
       </c>
@@ -5226,7 +5295,7 @@
       <c r="G136" s="12"/>
       <c r="H136" s="12"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A137" s="9" t="s">
         <v>49</v>
       </c>
@@ -5241,7 +5310,7 @@
       <c r="G137" s="12"/>
       <c r="H137" s="12"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A138" s="9" t="s">
         <v>49</v>
       </c>
@@ -5256,7 +5325,7 @@
       <c r="G138" s="12"/>
       <c r="H138" s="12"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A139" s="9" t="s">
         <v>49</v>
       </c>
@@ -5271,7 +5340,7 @@
       <c r="G139" s="12"/>
       <c r="H139" s="12"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A140" s="9" t="s">
         <v>49</v>
       </c>
@@ -5286,7 +5355,7 @@
       <c r="G140" s="12"/>
       <c r="H140" s="12"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A141" s="9" t="s">
         <v>49</v>
       </c>
@@ -5301,7 +5370,7 @@
       <c r="G141" s="12"/>
       <c r="H141" s="12"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A142" s="9" t="s">
         <v>49</v>
       </c>
@@ -5316,7 +5385,7 @@
       <c r="G142" s="12"/>
       <c r="H142" s="12"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A143" s="9" t="s">
         <v>49</v>
       </c>
@@ -5331,7 +5400,7 @@
       <c r="G143" s="12"/>
       <c r="H143" s="12"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A144" s="9" t="s">
         <v>49</v>
       </c>
@@ -10735,8 +10804,9 @@
     <hyperlink ref="C95" r:id="rId480" xr:uid="{B3BDB9E7-86C2-425B-9403-FE742A8BB665}"/>
     <hyperlink ref="K113" r:id="rId481" xr:uid="{4ABCF4E2-1F23-4DEC-B83E-6F25022FECD7}"/>
     <hyperlink ref="K112" r:id="rId482" xr:uid="{A2E21C54-125D-4835-97AC-B66CAC68024E}"/>
+    <hyperlink ref="K133" r:id="rId483" xr:uid="{A2CD53AF-BF86-4A7D-9093-4B270E99140E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId483"/>
+  <pageSetup orientation="portrait" r:id="rId484"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
String class methods file added
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBECC2E-84CB-4DC6-8989-F61D3071E97D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF08BC3B-D274-4512-8FE7-8D4828E14FB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="574">
   <si>
     <t>Topic:</t>
   </si>
@@ -1741,6 +1741,12 @@
   </si>
   <si>
     <t>STK8SAQ</t>
+  </si>
+  <si>
+    <t>NPS6STR</t>
+  </si>
+  <si>
+    <t>Write a program to find if a string is present in another string</t>
   </si>
 </sst>
 </file>
@@ -2301,10 +2307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:M511"/>
+  <dimension ref="A1:M512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -5310,19 +5316,18 @@
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A137" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B137" s="9"/>
+      <c r="A137" s="9"/>
+      <c r="B137" s="9" t="s">
+        <v>572</v>
+      </c>
       <c r="C137" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D137" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F137" s="12"/>
-      <c r="G137" s="12"/>
-      <c r="H137" s="12"/>
+        <v>573</v>
+      </c>
+      <c r="D137" s="15"/>
+      <c r="E137" s="16"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="18"/>
+      <c r="H137" s="22"/>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A138" s="9" t="s">
@@ -5330,7 +5335,7 @@
       </c>
       <c r="B138" s="9"/>
       <c r="C138" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D138" s="7" t="s">
         <v>3</v>
@@ -5345,7 +5350,7 @@
       </c>
       <c r="B139" s="9"/>
       <c r="C139" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D139" s="7" t="s">
         <v>3</v>
@@ -5360,7 +5365,7 @@
       </c>
       <c r="B140" s="9"/>
       <c r="C140" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D140" s="7" t="s">
         <v>3</v>
@@ -5375,7 +5380,7 @@
       </c>
       <c r="B141" s="9"/>
       <c r="C141" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D141" s="7" t="s">
         <v>3</v>
@@ -5390,7 +5395,7 @@
       </c>
       <c r="B142" s="9"/>
       <c r="C142" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D142" s="7" t="s">
         <v>3</v>
@@ -5405,7 +5410,7 @@
       </c>
       <c r="B143" s="9"/>
       <c r="C143" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D143" s="7" t="s">
         <v>3</v>
@@ -5420,7 +5425,7 @@
       </c>
       <c r="B144" s="9"/>
       <c r="C144" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D144" s="7" t="s">
         <v>3</v>
@@ -5435,7 +5440,7 @@
       </c>
       <c r="B145" s="9"/>
       <c r="C145" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D145" s="7" t="s">
         <v>3</v>
@@ -5450,7 +5455,7 @@
       </c>
       <c r="B146" s="9"/>
       <c r="C146" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D146" s="7" t="s">
         <v>3</v>
@@ -5465,7 +5470,7 @@
       </c>
       <c r="B147" s="9"/>
       <c r="C147" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D147" s="7" t="s">
         <v>3</v>
@@ -5480,7 +5485,7 @@
       </c>
       <c r="B148" s="9"/>
       <c r="C148" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D148" s="7" t="s">
         <v>3</v>
@@ -5495,7 +5500,7 @@
       </c>
       <c r="B149" s="9"/>
       <c r="C149" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D149" s="7" t="s">
         <v>3</v>
@@ -5510,7 +5515,7 @@
       </c>
       <c r="B150" s="9"/>
       <c r="C150" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D150" s="7" t="s">
         <v>3</v>
@@ -5525,7 +5530,7 @@
       </c>
       <c r="B151" s="9"/>
       <c r="C151" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D151" s="7" t="s">
         <v>3</v>
@@ -5540,7 +5545,7 @@
       </c>
       <c r="B152" s="9"/>
       <c r="C152" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D152" s="7" t="s">
         <v>3</v>
@@ -5555,7 +5560,7 @@
       </c>
       <c r="B153" s="9"/>
       <c r="C153" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D153" s="7" t="s">
         <v>3</v>
@@ -5570,7 +5575,7 @@
       </c>
       <c r="B154" s="9"/>
       <c r="C154" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D154" s="7" t="s">
         <v>3</v>
@@ -5585,7 +5590,7 @@
       </c>
       <c r="B155" s="9"/>
       <c r="C155" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D155" s="7" t="s">
         <v>3</v>
@@ -5600,7 +5605,7 @@
       </c>
       <c r="B156" s="9"/>
       <c r="C156" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D156" s="7" t="s">
         <v>3</v>
@@ -5615,7 +5620,7 @@
       </c>
       <c r="B157" s="9"/>
       <c r="C157" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D157" s="7" t="s">
         <v>3</v>
@@ -5630,7 +5635,7 @@
       </c>
       <c r="B158" s="9"/>
       <c r="C158" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D158" s="7" t="s">
         <v>3</v>
@@ -5645,7 +5650,7 @@
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D159" s="7" t="s">
         <v>3</v>
@@ -5660,7 +5665,7 @@
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D160" s="7" t="s">
         <v>3</v>
@@ -5675,7 +5680,7 @@
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D161" s="7" t="s">
         <v>3</v>
@@ -5690,7 +5695,7 @@
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D162" s="7" t="s">
         <v>3</v>
@@ -5705,7 +5710,7 @@
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D163" s="7" t="s">
         <v>3</v>
@@ -5720,7 +5725,7 @@
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D164" s="7" t="s">
         <v>3</v>
@@ -5735,7 +5740,7 @@
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D165" s="7" t="s">
         <v>3</v>
@@ -5750,7 +5755,7 @@
       </c>
       <c r="B166" s="9"/>
       <c r="C166" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D166" s="7" t="s">
         <v>3</v>
@@ -5765,7 +5770,7 @@
       </c>
       <c r="B167" s="9"/>
       <c r="C167" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D167" s="7" t="s">
         <v>3</v>
@@ -5780,7 +5785,7 @@
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D168" s="7" t="s">
         <v>3</v>
@@ -5795,7 +5800,7 @@
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D169" s="7" t="s">
         <v>3</v>
@@ -5810,7 +5815,7 @@
       </c>
       <c r="B170" s="9"/>
       <c r="C170" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D170" s="7" t="s">
         <v>3</v>
@@ -5825,7 +5830,7 @@
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D171" s="7" t="s">
         <v>3</v>
@@ -5840,7 +5845,7 @@
       </c>
       <c r="B172" s="9"/>
       <c r="C172" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D172" s="7" t="s">
         <v>3</v>
@@ -5850,50 +5855,41 @@
       <c r="H172" s="12"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A173" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B173" s="9"/>
+      <c r="C173" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F173" s="12"/>
       <c r="G173" s="12"/>
       <c r="H173" s="12"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
-      <c r="D174" s="7"/>
       <c r="F174" s="12"/>
       <c r="G174" s="12"/>
       <c r="H174" s="12"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A175" s="9"/>
-      <c r="B175" s="9"/>
-      <c r="C175" s="10"/>
-      <c r="D175" s="13"/>
+      <c r="A175" s="7"/>
+      <c r="B175" s="7"/>
+      <c r="D175" s="7"/>
       <c r="F175" s="12"/>
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A176" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B176" s="7"/>
-      <c r="C176" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D176" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="E176" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="F176" s="17" t="s">
-        <v>507</v>
-      </c>
-      <c r="G176" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="H176" s="22" t="s">
-        <v>512</v>
-      </c>
+      <c r="A176" s="9"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="10"/>
+      <c r="D176" s="13"/>
+      <c r="F176" s="12"/>
+      <c r="G176" s="12"/>
+      <c r="H176" s="12"/>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A177" s="7" t="s">
@@ -5901,7 +5897,7 @@
       </c>
       <c r="B177" s="7"/>
       <c r="C177" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D177" s="15" t="s">
         <v>454</v>
@@ -5917,9 +5913,6 @@
       </c>
       <c r="H177" s="22" t="s">
         <v>512</v>
-      </c>
-      <c r="K177" s="10" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.4">
@@ -5928,7 +5921,7 @@
       </c>
       <c r="B178" s="7"/>
       <c r="C178" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D178" s="15" t="s">
         <v>454</v>
@@ -5944,6 +5937,9 @@
       </c>
       <c r="H178" s="22" t="s">
         <v>512</v>
+      </c>
+      <c r="K178" s="10" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.4">
@@ -5952,14 +5948,23 @@
       </c>
       <c r="B179" s="7"/>
       <c r="C179" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D179" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F179" s="12"/>
-      <c r="G179" s="12"/>
-      <c r="H179" s="12"/>
+        <v>126</v>
+      </c>
+      <c r="D179" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E179" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F179" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G179" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H179" s="22" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A180" s="7" t="s">
@@ -5967,7 +5972,7 @@
       </c>
       <c r="B180" s="7"/>
       <c r="C180" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D180" s="7" t="s">
         <v>3</v>
@@ -5982,7 +5987,7 @@
       </c>
       <c r="B181" s="7"/>
       <c r="C181" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D181" s="7" t="s">
         <v>3</v>
@@ -5997,7 +6002,7 @@
       </c>
       <c r="B182" s="7"/>
       <c r="C182" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D182" s="7" t="s">
         <v>3</v>
@@ -6012,7 +6017,7 @@
       </c>
       <c r="B183" s="7"/>
       <c r="C183" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D183" s="7" t="s">
         <v>3</v>
@@ -6027,7 +6032,7 @@
       </c>
       <c r="B184" s="7"/>
       <c r="C184" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D184" s="7" t="s">
         <v>3</v>
@@ -6042,7 +6047,7 @@
       </c>
       <c r="B185" s="7"/>
       <c r="C185" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D185" s="7" t="s">
         <v>3</v>
@@ -6057,7 +6062,7 @@
       </c>
       <c r="B186" s="7"/>
       <c r="C186" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D186" s="7" t="s">
         <v>3</v>
@@ -6072,7 +6077,7 @@
       </c>
       <c r="B187" s="7"/>
       <c r="C187" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D187" s="7" t="s">
         <v>3</v>
@@ -6087,7 +6092,7 @@
       </c>
       <c r="B188" s="7"/>
       <c r="C188" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D188" s="7" t="s">
         <v>3</v>
@@ -6102,7 +6107,7 @@
       </c>
       <c r="B189" s="7"/>
       <c r="C189" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D189" s="7" t="s">
         <v>3</v>
@@ -6117,7 +6122,7 @@
       </c>
       <c r="B190" s="7"/>
       <c r="C190" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D190" s="7" t="s">
         <v>3</v>
@@ -6132,7 +6137,7 @@
       </c>
       <c r="B191" s="7"/>
       <c r="C191" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D191" s="7" t="s">
         <v>3</v>
@@ -6147,7 +6152,7 @@
       </c>
       <c r="B192" s="7"/>
       <c r="C192" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D192" s="7" t="s">
         <v>3</v>
@@ -6162,7 +6167,7 @@
       </c>
       <c r="B193" s="7"/>
       <c r="C193" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D193" s="7" t="s">
         <v>3</v>
@@ -6177,7 +6182,7 @@
       </c>
       <c r="B194" s="7"/>
       <c r="C194" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D194" s="7" t="s">
         <v>3</v>
@@ -6192,7 +6197,7 @@
       </c>
       <c r="B195" s="7"/>
       <c r="C195" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D195" s="7" t="s">
         <v>3</v>
@@ -6207,7 +6212,7 @@
       </c>
       <c r="B196" s="7"/>
       <c r="C196" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D196" s="7" t="s">
         <v>3</v>
@@ -6222,7 +6227,7 @@
       </c>
       <c r="B197" s="7"/>
       <c r="C197" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D197" s="7" t="s">
         <v>3</v>
@@ -6237,7 +6242,7 @@
       </c>
       <c r="B198" s="7"/>
       <c r="C198" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D198" s="7" t="s">
         <v>3</v>
@@ -6252,7 +6257,7 @@
       </c>
       <c r="B199" s="7"/>
       <c r="C199" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D199" s="7" t="s">
         <v>3</v>
@@ -6267,7 +6272,7 @@
       </c>
       <c r="B200" s="7"/>
       <c r="C200" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D200" s="7" t="s">
         <v>3</v>
@@ -6281,8 +6286,8 @@
         <v>123</v>
       </c>
       <c r="B201" s="7"/>
-      <c r="C201" s="5" t="s">
-        <v>149</v>
+      <c r="C201" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="D201" s="7" t="s">
         <v>3</v>
@@ -6297,7 +6302,7 @@
       </c>
       <c r="B202" s="7"/>
       <c r="C202" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D202" s="7" t="s">
         <v>3</v>
@@ -6311,8 +6316,8 @@
         <v>123</v>
       </c>
       <c r="B203" s="7"/>
-      <c r="C203" s="10" t="s">
-        <v>151</v>
+      <c r="C203" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="D203" s="7" t="s">
         <v>3</v>
@@ -6327,7 +6332,7 @@
       </c>
       <c r="B204" s="7"/>
       <c r="C204" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D204" s="7" t="s">
         <v>3</v>
@@ -6342,7 +6347,7 @@
       </c>
       <c r="B205" s="7"/>
       <c r="C205" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D205" s="7" t="s">
         <v>3</v>
@@ -6357,7 +6362,7 @@
       </c>
       <c r="B206" s="7"/>
       <c r="C206" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D206" s="7" t="s">
         <v>3</v>
@@ -6372,7 +6377,7 @@
       </c>
       <c r="B207" s="7"/>
       <c r="C207" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D207" s="7" t="s">
         <v>3</v>
@@ -6387,7 +6392,7 @@
       </c>
       <c r="B208" s="7"/>
       <c r="C208" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D208" s="7" t="s">
         <v>3</v>
@@ -6402,7 +6407,7 @@
       </c>
       <c r="B209" s="7"/>
       <c r="C209" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D209" s="7" t="s">
         <v>3</v>
@@ -6417,7 +6422,7 @@
       </c>
       <c r="B210" s="7"/>
       <c r="C210" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D210" s="7" t="s">
         <v>3</v>
@@ -6432,7 +6437,7 @@
       </c>
       <c r="B211" s="7"/>
       <c r="C211" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D211" s="7" t="s">
         <v>3</v>
@@ -6442,43 +6447,34 @@
       <c r="H211" s="12"/>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A212" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B212" s="7"/>
+      <c r="C212" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D212" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F212" s="12"/>
       <c r="G212" s="12"/>
       <c r="H212" s="12"/>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A213" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="B213" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="C213" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="D213" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="E213" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="F213" s="17" t="s">
-        <v>507</v>
-      </c>
-      <c r="G213" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="H213" s="22" t="s">
-        <v>512</v>
-      </c>
+      <c r="F213" s="12"/>
+      <c r="G213" s="12"/>
+      <c r="H213" s="12"/>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A214" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B214" s="9"/>
+      <c r="B214" s="9" t="s">
+        <v>571</v>
+      </c>
       <c r="C214" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D214" s="15" t="s">
         <v>454</v>
@@ -6502,14 +6498,23 @@
       </c>
       <c r="B215" s="9"/>
       <c r="C215" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="D215" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F215" s="12"/>
-      <c r="G215" s="12"/>
-      <c r="H215" s="12"/>
+        <v>276</v>
+      </c>
+      <c r="D215" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E215" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F215" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G215" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H215" s="22" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A216" s="9" t="s">
@@ -6517,7 +6522,7 @@
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D216" s="7" t="s">
         <v>3</v>
@@ -6532,7 +6537,7 @@
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D217" s="7" t="s">
         <v>3</v>
@@ -6547,7 +6552,7 @@
       </c>
       <c r="B218" s="9"/>
       <c r="C218" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D218" s="7" t="s">
         <v>3</v>
@@ -6562,7 +6567,7 @@
       </c>
       <c r="B219" s="9"/>
       <c r="C219" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D219" s="7" t="s">
         <v>3</v>
@@ -6577,7 +6582,7 @@
       </c>
       <c r="B220" s="9"/>
       <c r="C220" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D220" s="7" t="s">
         <v>3</v>
@@ -6592,7 +6597,7 @@
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D221" s="7" t="s">
         <v>3</v>
@@ -6607,7 +6612,7 @@
       </c>
       <c r="B222" s="9"/>
       <c r="C222" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D222" s="7" t="s">
         <v>3</v>
@@ -6622,7 +6627,7 @@
       </c>
       <c r="B223" s="9"/>
       <c r="C223" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D223" s="7" t="s">
         <v>3</v>
@@ -6637,7 +6642,7 @@
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D224" s="7" t="s">
         <v>3</v>
@@ -6652,7 +6657,7 @@
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D225" s="7" t="s">
         <v>3</v>
@@ -6666,8 +6671,8 @@
         <v>274</v>
       </c>
       <c r="B226" s="9"/>
-      <c r="C226" s="4" t="s">
-        <v>288</v>
+      <c r="C226" s="10" t="s">
+        <v>287</v>
       </c>
       <c r="D226" s="7" t="s">
         <v>3</v>
@@ -6681,8 +6686,8 @@
         <v>274</v>
       </c>
       <c r="B227" s="9"/>
-      <c r="C227" s="10" t="s">
-        <v>289</v>
+      <c r="C227" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="D227" s="7" t="s">
         <v>3</v>
@@ -6697,7 +6702,7 @@
       </c>
       <c r="B228" s="9"/>
       <c r="C228" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D228" s="7" t="s">
         <v>3</v>
@@ -6712,7 +6717,7 @@
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D229" s="7" t="s">
         <v>3</v>
@@ -6727,7 +6732,7 @@
       </c>
       <c r="B230" s="9"/>
       <c r="C230" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D230" s="7" t="s">
         <v>3</v>
@@ -6742,7 +6747,7 @@
       </c>
       <c r="B231" s="9"/>
       <c r="C231" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D231" s="7" t="s">
         <v>3</v>
@@ -6757,7 +6762,7 @@
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D232" s="7" t="s">
         <v>3</v>
@@ -6772,7 +6777,7 @@
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D233" s="7" t="s">
         <v>3</v>
@@ -6787,7 +6792,7 @@
       </c>
       <c r="B234" s="9"/>
       <c r="C234" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D234" s="7" t="s">
         <v>3</v>
@@ -6802,7 +6807,7 @@
       </c>
       <c r="B235" s="9"/>
       <c r="C235" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D235" s="7" t="s">
         <v>3</v>
@@ -6817,7 +6822,7 @@
       </c>
       <c r="B236" s="9"/>
       <c r="C236" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D236" s="7" t="s">
         <v>3</v>
@@ -6832,7 +6837,7 @@
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D237" s="7" t="s">
         <v>3</v>
@@ -6847,7 +6852,7 @@
       </c>
       <c r="B238" s="9"/>
       <c r="C238" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D238" s="7" t="s">
         <v>3</v>
@@ -6862,7 +6867,7 @@
       </c>
       <c r="B239" s="9"/>
       <c r="C239" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D239" s="7" t="s">
         <v>3</v>
@@ -6877,7 +6882,7 @@
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D240" s="7" t="s">
         <v>3</v>
@@ -6892,7 +6897,7 @@
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D241" s="7" t="s">
         <v>3</v>
@@ -6907,7 +6912,7 @@
       </c>
       <c r="B242" s="9"/>
       <c r="C242" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D242" s="7" t="s">
         <v>3</v>
@@ -6922,7 +6927,7 @@
       </c>
       <c r="B243" s="9"/>
       <c r="C243" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D243" s="7" t="s">
         <v>3</v>
@@ -6937,7 +6942,7 @@
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D244" s="7" t="s">
         <v>3</v>
@@ -6952,7 +6957,7 @@
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D245" s="7" t="s">
         <v>3</v>
@@ -6967,7 +6972,7 @@
       </c>
       <c r="B246" s="9"/>
       <c r="C246" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D246" s="7" t="s">
         <v>3</v>
@@ -6982,7 +6987,7 @@
       </c>
       <c r="B247" s="9"/>
       <c r="C247" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D247" s="7" t="s">
         <v>3</v>
@@ -6997,7 +7002,7 @@
       </c>
       <c r="B248" s="9"/>
       <c r="C248" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D248" s="7" t="s">
         <v>3</v>
@@ -7012,7 +7017,7 @@
       </c>
       <c r="B249" s="9"/>
       <c r="C249" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D249" s="7" t="s">
         <v>3</v>
@@ -7027,7 +7032,7 @@
       </c>
       <c r="B250" s="9"/>
       <c r="C250" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D250" s="7" t="s">
         <v>3</v>
@@ -7037,22 +7042,22 @@
       <c r="H250" s="12"/>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D251" s="7"/>
+      <c r="A251" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B251" s="9"/>
+      <c r="C251" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="D251" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F251" s="12"/>
       <c r="G251" s="12"/>
       <c r="H251" s="12"/>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A252" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B252" s="9"/>
-      <c r="C252" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D252" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D252" s="7"/>
       <c r="F252" s="12"/>
       <c r="G252" s="12"/>
       <c r="H252" s="12"/>
@@ -7063,7 +7068,7 @@
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D253" s="7" t="s">
         <v>3</v>
@@ -7078,7 +7083,7 @@
       </c>
       <c r="B254" s="9"/>
       <c r="C254" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D254" s="7" t="s">
         <v>3</v>
@@ -7093,7 +7098,7 @@
       </c>
       <c r="B255" s="9"/>
       <c r="C255" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D255" s="7" t="s">
         <v>3</v>
@@ -7108,7 +7113,7 @@
       </c>
       <c r="B256" s="9"/>
       <c r="C256" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D256" s="7" t="s">
         <v>3</v>
@@ -7123,7 +7128,7 @@
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D257" s="7" t="s">
         <v>3</v>
@@ -7138,7 +7143,7 @@
       </c>
       <c r="B258" s="9"/>
       <c r="C258" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D258" s="7" t="s">
         <v>3</v>
@@ -7153,7 +7158,7 @@
       </c>
       <c r="B259" s="9"/>
       <c r="C259" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D259" s="7" t="s">
         <v>3</v>
@@ -7168,7 +7173,7 @@
       </c>
       <c r="B260" s="9"/>
       <c r="C260" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D260" s="7" t="s">
         <v>3</v>
@@ -7183,7 +7188,7 @@
       </c>
       <c r="B261" s="9"/>
       <c r="C261" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D261" s="7" t="s">
         <v>3</v>
@@ -7198,7 +7203,7 @@
       </c>
       <c r="B262" s="9"/>
       <c r="C262" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D262" s="7" t="s">
         <v>3</v>
@@ -7213,7 +7218,7 @@
       </c>
       <c r="B263" s="9"/>
       <c r="C263" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D263" s="7" t="s">
         <v>3</v>
@@ -7228,7 +7233,7 @@
       </c>
       <c r="B264" s="9"/>
       <c r="C264" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D264" s="7" t="s">
         <v>3</v>
@@ -7243,7 +7248,7 @@
       </c>
       <c r="B265" s="9"/>
       <c r="C265" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D265" s="7" t="s">
         <v>3</v>
@@ -7258,7 +7263,7 @@
       </c>
       <c r="B266" s="9"/>
       <c r="C266" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D266" s="7" t="s">
         <v>3</v>
@@ -7273,7 +7278,7 @@
       </c>
       <c r="B267" s="9"/>
       <c r="C267" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D267" s="7" t="s">
         <v>3</v>
@@ -7288,7 +7293,7 @@
       </c>
       <c r="B268" s="9"/>
       <c r="C268" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D268" s="7" t="s">
         <v>3</v>
@@ -7303,7 +7308,7 @@
       </c>
       <c r="B269" s="9"/>
       <c r="C269" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D269" s="7" t="s">
         <v>3</v>
@@ -7318,7 +7323,7 @@
       </c>
       <c r="B270" s="9"/>
       <c r="C270" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D270" s="7" t="s">
         <v>3</v>
@@ -7333,7 +7338,7 @@
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D271" s="7" t="s">
         <v>3</v>
@@ -7348,7 +7353,7 @@
       </c>
       <c r="B272" s="9"/>
       <c r="C272" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D272" s="7" t="s">
         <v>3</v>
@@ -7363,7 +7368,7 @@
       </c>
       <c r="B273" s="9"/>
       <c r="C273" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D273" s="7" t="s">
         <v>3</v>
@@ -7378,7 +7383,7 @@
       </c>
       <c r="B274" s="9"/>
       <c r="C274" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D274" s="7" t="s">
         <v>3</v>
@@ -7393,7 +7398,7 @@
       </c>
       <c r="B275" s="9"/>
       <c r="C275" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D275" s="7" t="s">
         <v>3</v>
@@ -7408,7 +7413,7 @@
       </c>
       <c r="B276" s="9"/>
       <c r="C276" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D276" s="7" t="s">
         <v>3</v>
@@ -7423,7 +7428,7 @@
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D277" s="7" t="s">
         <v>3</v>
@@ -7438,7 +7443,7 @@
       </c>
       <c r="B278" s="9"/>
       <c r="C278" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D278" s="7" t="s">
         <v>3</v>
@@ -7453,7 +7458,7 @@
       </c>
       <c r="B279" s="9"/>
       <c r="C279" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D279" s="7" t="s">
         <v>3</v>
@@ -7468,7 +7473,7 @@
       </c>
       <c r="B280" s="9"/>
       <c r="C280" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D280" s="7" t="s">
         <v>3</v>
@@ -7483,7 +7488,7 @@
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D281" s="7" t="s">
         <v>3</v>
@@ -7498,7 +7503,7 @@
       </c>
       <c r="B282" s="9"/>
       <c r="C282" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D282" s="7" t="s">
         <v>3</v>
@@ -7513,7 +7518,7 @@
       </c>
       <c r="B283" s="9"/>
       <c r="C283" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D283" s="7" t="s">
         <v>3</v>
@@ -7528,7 +7533,7 @@
       </c>
       <c r="B284" s="9"/>
       <c r="C284" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D284" s="7" t="s">
         <v>3</v>
@@ -7543,7 +7548,7 @@
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D285" s="7" t="s">
         <v>3</v>
@@ -7558,7 +7563,7 @@
       </c>
       <c r="B286" s="9"/>
       <c r="C286" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D286" s="7" t="s">
         <v>3</v>
@@ -7568,9 +7573,16 @@
       <c r="H286" s="12"/>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A287" s="7"/>
-      <c r="B287" s="7"/>
-      <c r="D287" s="7"/>
+      <c r="A287" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B287" s="9"/>
+      <c r="C287" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D287" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F287" s="12"/>
       <c r="G287" s="12"/>
       <c r="H287" s="12"/>
@@ -7584,16 +7596,9 @@
       <c r="H288" s="12"/>
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A289" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="B289" s="9"/>
-      <c r="C289" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D289" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="A289" s="7"/>
+      <c r="B289" s="7"/>
+      <c r="D289" s="7"/>
       <c r="F289" s="12"/>
       <c r="G289" s="12"/>
       <c r="H289" s="12"/>
@@ -7604,7 +7609,7 @@
       </c>
       <c r="B290" s="9"/>
       <c r="C290" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D290" s="7" t="s">
         <v>3</v>
@@ -7619,7 +7624,7 @@
       </c>
       <c r="B291" s="9"/>
       <c r="C291" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D291" s="7" t="s">
         <v>3</v>
@@ -7634,7 +7639,7 @@
       </c>
       <c r="B292" s="9"/>
       <c r="C292" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D292" s="7" t="s">
         <v>3</v>
@@ -7649,7 +7654,7 @@
       </c>
       <c r="B293" s="9"/>
       <c r="C293" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D293" s="7" t="s">
         <v>3</v>
@@ -7664,7 +7669,7 @@
       </c>
       <c r="B294" s="9"/>
       <c r="C294" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D294" s="7" t="s">
         <v>3</v>
@@ -7678,8 +7683,8 @@
         <v>196</v>
       </c>
       <c r="B295" s="9"/>
-      <c r="C295" s="4" t="s">
-        <v>203</v>
+      <c r="C295" s="10" t="s">
+        <v>202</v>
       </c>
       <c r="D295" s="7" t="s">
         <v>3</v>
@@ -7693,8 +7698,8 @@
         <v>196</v>
       </c>
       <c r="B296" s="9"/>
-      <c r="C296" s="10" t="s">
-        <v>204</v>
+      <c r="C296" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="D296" s="7" t="s">
         <v>3</v>
@@ -7709,7 +7714,7 @@
       </c>
       <c r="B297" s="9"/>
       <c r="C297" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D297" s="7" t="s">
         <v>3</v>
@@ -7724,7 +7729,7 @@
       </c>
       <c r="B298" s="9"/>
       <c r="C298" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D298" s="7" t="s">
         <v>3</v>
@@ -7739,7 +7744,7 @@
       </c>
       <c r="B299" s="9"/>
       <c r="C299" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D299" s="7" t="s">
         <v>3</v>
@@ -7754,7 +7759,7 @@
       </c>
       <c r="B300" s="9"/>
       <c r="C300" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D300" s="7" t="s">
         <v>3</v>
@@ -7769,7 +7774,7 @@
       </c>
       <c r="B301" s="9"/>
       <c r="C301" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D301" s="7" t="s">
         <v>3</v>
@@ -7784,7 +7789,7 @@
       </c>
       <c r="B302" s="9"/>
       <c r="C302" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D302" s="7" t="s">
         <v>3</v>
@@ -7799,7 +7804,7 @@
       </c>
       <c r="B303" s="9"/>
       <c r="C303" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D303" s="7" t="s">
         <v>3</v>
@@ -7814,7 +7819,7 @@
       </c>
       <c r="B304" s="9"/>
       <c r="C304" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D304" s="7" t="s">
         <v>3</v>
@@ -7829,7 +7834,7 @@
       </c>
       <c r="B305" s="9"/>
       <c r="C305" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D305" s="7" t="s">
         <v>3</v>
@@ -7844,7 +7849,7 @@
       </c>
       <c r="B306" s="9"/>
       <c r="C306" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D306" s="7" t="s">
         <v>3</v>
@@ -7859,7 +7864,7 @@
       </c>
       <c r="B307" s="9"/>
       <c r="C307" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D307" s="7" t="s">
         <v>3</v>
@@ -7874,7 +7879,7 @@
       </c>
       <c r="B308" s="9"/>
       <c r="C308" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D308" s="7" t="s">
         <v>3</v>
@@ -7889,7 +7894,7 @@
       </c>
       <c r="B309" s="9"/>
       <c r="C309" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D309" s="7" t="s">
         <v>3</v>
@@ -7904,7 +7909,7 @@
       </c>
       <c r="B310" s="9"/>
       <c r="C310" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D310" s="7" t="s">
         <v>3</v>
@@ -7914,22 +7919,22 @@
       <c r="H310" s="12"/>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D311" s="7"/>
+      <c r="A311" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B311" s="9"/>
+      <c r="C311" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D311" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F311" s="12"/>
       <c r="G311" s="12"/>
       <c r="H311" s="12"/>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A312" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="B312" s="7"/>
-      <c r="C312" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="D312" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D312" s="7"/>
       <c r="F312" s="12"/>
       <c r="G312" s="12"/>
       <c r="H312" s="12"/>
@@ -7940,7 +7945,7 @@
       </c>
       <c r="B313" s="7"/>
       <c r="C313" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D313" s="7" t="s">
         <v>3</v>
@@ -7955,7 +7960,7 @@
       </c>
       <c r="B314" s="7"/>
       <c r="C314" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D314" s="7" t="s">
         <v>3</v>
@@ -7970,7 +7975,7 @@
       </c>
       <c r="B315" s="7"/>
       <c r="C315" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D315" s="7" t="s">
         <v>3</v>
@@ -7985,7 +7990,7 @@
       </c>
       <c r="B316" s="7"/>
       <c r="C316" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D316" s="7" t="s">
         <v>3</v>
@@ -8000,7 +8005,7 @@
       </c>
       <c r="B317" s="7"/>
       <c r="C317" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D317" s="7" t="s">
         <v>3</v>
@@ -8015,7 +8020,7 @@
       </c>
       <c r="B318" s="7"/>
       <c r="C318" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D318" s="7" t="s">
         <v>3</v>
@@ -8030,7 +8035,7 @@
       </c>
       <c r="B319" s="7"/>
       <c r="C319" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D319" s="7" t="s">
         <v>3</v>
@@ -8044,8 +8049,8 @@
         <v>313</v>
       </c>
       <c r="B320" s="7"/>
-      <c r="C320" s="4" t="s">
-        <v>322</v>
+      <c r="C320" s="10" t="s">
+        <v>321</v>
       </c>
       <c r="D320" s="7" t="s">
         <v>3</v>
@@ -8059,8 +8064,8 @@
         <v>313</v>
       </c>
       <c r="B321" s="7"/>
-      <c r="C321" s="10" t="s">
-        <v>323</v>
+      <c r="C321" s="4" t="s">
+        <v>322</v>
       </c>
       <c r="D321" s="7" t="s">
         <v>3</v>
@@ -8075,7 +8080,7 @@
       </c>
       <c r="B322" s="7"/>
       <c r="C322" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D322" s="7" t="s">
         <v>3</v>
@@ -8090,7 +8095,7 @@
       </c>
       <c r="B323" s="7"/>
       <c r="C323" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D323" s="7" t="s">
         <v>3</v>
@@ -8105,7 +8110,7 @@
       </c>
       <c r="B324" s="7"/>
       <c r="C324" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D324" s="7" t="s">
         <v>3</v>
@@ -8120,7 +8125,7 @@
       </c>
       <c r="B325" s="7"/>
       <c r="C325" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D325" s="7" t="s">
         <v>3</v>
@@ -8135,7 +8140,7 @@
       </c>
       <c r="B326" s="7"/>
       <c r="C326" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D326" s="7" t="s">
         <v>3</v>
@@ -8150,7 +8155,7 @@
       </c>
       <c r="B327" s="7"/>
       <c r="C327" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D327" s="7" t="s">
         <v>3</v>
@@ -8165,7 +8170,7 @@
       </c>
       <c r="B328" s="7"/>
       <c r="C328" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D328" s="7" t="s">
         <v>3</v>
@@ -8180,7 +8185,7 @@
       </c>
       <c r="B329" s="7"/>
       <c r="C329" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D329" s="7" t="s">
         <v>3</v>
@@ -8190,25 +8195,25 @@
       <c r="H329" s="12"/>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A330" s="12"/>
-      <c r="B330" s="12"/>
-      <c r="C330" s="10"/>
-      <c r="D330" s="12"/>
+      <c r="A330" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B330" s="7"/>
+      <c r="C330" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="D330" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F330" s="12"/>
       <c r="G330" s="12"/>
       <c r="H330" s="12"/>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A331" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="B331" s="7"/>
-      <c r="C331" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D331" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="A331" s="12"/>
+      <c r="B331" s="12"/>
+      <c r="C331" s="10"/>
+      <c r="D331" s="12"/>
       <c r="F331" s="12"/>
       <c r="G331" s="12"/>
       <c r="H331" s="12"/>
@@ -8219,7 +8224,7 @@
       </c>
       <c r="B332" s="7"/>
       <c r="C332" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D332" s="7" t="s">
         <v>3</v>
@@ -8234,7 +8239,7 @@
       </c>
       <c r="B333" s="7"/>
       <c r="C333" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D333" s="7" t="s">
         <v>3</v>
@@ -8249,7 +8254,7 @@
       </c>
       <c r="B334" s="7"/>
       <c r="C334" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D334" s="7" t="s">
         <v>3</v>
@@ -8264,7 +8269,7 @@
       </c>
       <c r="B335" s="7"/>
       <c r="C335" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D335" s="7" t="s">
         <v>3</v>
@@ -8279,7 +8284,7 @@
       </c>
       <c r="B336" s="7"/>
       <c r="C336" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D336" s="7" t="s">
         <v>3</v>
@@ -8294,7 +8299,7 @@
       </c>
       <c r="B337" s="7"/>
       <c r="C337" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D337" s="7" t="s">
         <v>3</v>
@@ -8309,7 +8314,7 @@
       </c>
       <c r="B338" s="7"/>
       <c r="C338" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D338" s="7" t="s">
         <v>3</v>
@@ -8324,7 +8329,7 @@
       </c>
       <c r="B339" s="7"/>
       <c r="C339" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D339" s="7" t="s">
         <v>3</v>
@@ -8339,7 +8344,7 @@
       </c>
       <c r="B340" s="7"/>
       <c r="C340" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D340" s="7" t="s">
         <v>3</v>
@@ -8354,7 +8359,7 @@
       </c>
       <c r="B341" s="7"/>
       <c r="C341" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D341" s="7" t="s">
         <v>3</v>
@@ -8369,7 +8374,7 @@
       </c>
       <c r="B342" s="7"/>
       <c r="C342" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D342" s="7" t="s">
         <v>3</v>
@@ -8384,7 +8389,7 @@
       </c>
       <c r="B343" s="7"/>
       <c r="C343" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D343" s="7" t="s">
         <v>3</v>
@@ -8399,7 +8404,7 @@
       </c>
       <c r="B344" s="7"/>
       <c r="C344" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D344" s="7" t="s">
         <v>3</v>
@@ -8414,7 +8419,7 @@
       </c>
       <c r="B345" s="7"/>
       <c r="C345" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D345" s="7" t="s">
         <v>3</v>
@@ -8429,7 +8434,7 @@
       </c>
       <c r="B346" s="7"/>
       <c r="C346" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D346" s="7" t="s">
         <v>3</v>
@@ -8444,7 +8449,7 @@
       </c>
       <c r="B347" s="7"/>
       <c r="C347" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D347" s="7" t="s">
         <v>3</v>
@@ -8459,7 +8464,7 @@
       </c>
       <c r="B348" s="7"/>
       <c r="C348" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D348" s="7" t="s">
         <v>3</v>
@@ -8474,7 +8479,7 @@
       </c>
       <c r="B349" s="7"/>
       <c r="C349" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D349" s="7" t="s">
         <v>3</v>
@@ -8489,7 +8494,7 @@
       </c>
       <c r="B350" s="7"/>
       <c r="C350" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D350" s="7" t="s">
         <v>3</v>
@@ -8504,7 +8509,7 @@
       </c>
       <c r="B351" s="7"/>
       <c r="C351" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D351" s="7" t="s">
         <v>3</v>
@@ -8519,7 +8524,7 @@
       </c>
       <c r="B352" s="7"/>
       <c r="C352" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D352" s="7" t="s">
         <v>3</v>
@@ -8534,7 +8539,7 @@
       </c>
       <c r="B353" s="7"/>
       <c r="C353" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D353" s="7" t="s">
         <v>3</v>
@@ -8549,7 +8554,7 @@
       </c>
       <c r="B354" s="7"/>
       <c r="C354" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D354" s="7" t="s">
         <v>3</v>
@@ -8564,7 +8569,7 @@
       </c>
       <c r="B355" s="7"/>
       <c r="C355" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D355" s="7" t="s">
         <v>3</v>
@@ -8579,7 +8584,7 @@
       </c>
       <c r="B356" s="7"/>
       <c r="C356" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D356" s="7" t="s">
         <v>3</v>
@@ -8594,7 +8599,7 @@
       </c>
       <c r="B357" s="7"/>
       <c r="C357" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D357" s="7" t="s">
         <v>3</v>
@@ -8609,7 +8614,7 @@
       </c>
       <c r="B358" s="7"/>
       <c r="C358" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D358" s="7" t="s">
         <v>3</v>
@@ -8624,7 +8629,7 @@
       </c>
       <c r="B359" s="7"/>
       <c r="C359" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D359" s="7" t="s">
         <v>3</v>
@@ -8639,7 +8644,7 @@
       </c>
       <c r="B360" s="7"/>
       <c r="C360" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D360" s="7" t="s">
         <v>3</v>
@@ -8654,7 +8659,7 @@
       </c>
       <c r="B361" s="7"/>
       <c r="C361" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D361" s="7" t="s">
         <v>3</v>
@@ -8669,7 +8674,7 @@
       </c>
       <c r="B362" s="7"/>
       <c r="C362" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D362" s="7" t="s">
         <v>3</v>
@@ -8684,7 +8689,7 @@
       </c>
       <c r="B363" s="7"/>
       <c r="C363" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D363" s="7" t="s">
         <v>3</v>
@@ -8699,7 +8704,7 @@
       </c>
       <c r="B364" s="7"/>
       <c r="C364" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D364" s="7" t="s">
         <v>3</v>
@@ -8729,7 +8734,7 @@
       </c>
       <c r="B366" s="7"/>
       <c r="C366" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D366" s="7" t="s">
         <v>3</v>
@@ -8744,7 +8749,7 @@
       </c>
       <c r="B367" s="7"/>
       <c r="C367" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D367" s="7" t="s">
         <v>3</v>
@@ -8759,7 +8764,7 @@
       </c>
       <c r="B368" s="7"/>
       <c r="C368" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D368" s="7" t="s">
         <v>3</v>
@@ -8774,7 +8779,7 @@
       </c>
       <c r="B369" s="7"/>
       <c r="C369" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D369" s="7" t="s">
         <v>3</v>
@@ -8789,11 +8794,14 @@
       </c>
       <c r="B370" s="7"/>
       <c r="C370" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D370" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="F370" s="12"/>
+      <c r="G370" s="12"/>
+      <c r="H370" s="12"/>
     </row>
     <row r="371" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A371" s="7" t="s">
@@ -8801,7 +8809,7 @@
       </c>
       <c r="B371" s="7"/>
       <c r="C371" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D371" s="7" t="s">
         <v>3</v>
@@ -8813,7 +8821,7 @@
       </c>
       <c r="B372" s="7"/>
       <c r="C372" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D372" s="7" t="s">
         <v>3</v>
@@ -8825,7 +8833,7 @@
       </c>
       <c r="B373" s="7"/>
       <c r="C373" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D373" s="7" t="s">
         <v>3</v>
@@ -8837,41 +8845,41 @@
       </c>
       <c r="B374" s="7"/>
       <c r="C374" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="D374" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A375" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B375" s="7"/>
+      <c r="C375" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="D374" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A375" s="9" t="s">
+      <c r="D375" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A376" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="B375" s="23"/>
-      <c r="C375" s="10" t="s">
+      <c r="B376" s="23"/>
+      <c r="C376" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="D375" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F375" s="12"/>
-      <c r="G375" s="12"/>
-      <c r="H375" s="12"/>
-    </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D376" s="7"/>
+      <c r="D376" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F376" s="12"/>
+      <c r="G376" s="12"/>
+      <c r="H376" s="12"/>
     </row>
     <row r="377" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A377" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B377" s="9"/>
-      <c r="C377" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="D377" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D377" s="7"/>
     </row>
     <row r="378" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A378" s="9" t="s">
@@ -8879,7 +8887,7 @@
       </c>
       <c r="B378" s="9"/>
       <c r="C378" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D378" s="7" t="s">
         <v>3</v>
@@ -8891,7 +8899,7 @@
       </c>
       <c r="B379" s="9"/>
       <c r="C379" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D379" s="7" t="s">
         <v>3</v>
@@ -8903,7 +8911,7 @@
       </c>
       <c r="B380" s="9"/>
       <c r="C380" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D380" s="7" t="s">
         <v>3</v>
@@ -8915,7 +8923,7 @@
       </c>
       <c r="B381" s="9"/>
       <c r="C381" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D381" s="7" t="s">
         <v>3</v>
@@ -8927,7 +8935,7 @@
       </c>
       <c r="B382" s="9"/>
       <c r="C382" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D382" s="7" t="s">
         <v>3</v>
@@ -8939,7 +8947,7 @@
       </c>
       <c r="B383" s="9"/>
       <c r="C383" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D383" s="7" t="s">
         <v>3</v>
@@ -8951,7 +8959,7 @@
       </c>
       <c r="B384" s="9"/>
       <c r="C384" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D384" s="7" t="s">
         <v>3</v>
@@ -8963,7 +8971,7 @@
       </c>
       <c r="B385" s="9"/>
       <c r="C385" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D385" s="7" t="s">
         <v>3</v>
@@ -8975,7 +8983,7 @@
       </c>
       <c r="B386" s="9"/>
       <c r="C386" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D386" s="7" t="s">
         <v>3</v>
@@ -8987,7 +8995,7 @@
       </c>
       <c r="B387" s="9"/>
       <c r="C387" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D387" s="7" t="s">
         <v>3</v>
@@ -8999,7 +9007,7 @@
       </c>
       <c r="B388" s="9"/>
       <c r="C388" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D388" s="7" t="s">
         <v>3</v>
@@ -9011,7 +9019,7 @@
       </c>
       <c r="B389" s="9"/>
       <c r="C389" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D389" s="7" t="s">
         <v>3</v>
@@ -9023,7 +9031,7 @@
       </c>
       <c r="B390" s="9"/>
       <c r="C390" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D390" s="7" t="s">
         <v>3</v>
@@ -9035,7 +9043,7 @@
       </c>
       <c r="B391" s="9"/>
       <c r="C391" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D391" s="7" t="s">
         <v>3</v>
@@ -9047,7 +9055,7 @@
       </c>
       <c r="B392" s="9"/>
       <c r="C392" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D392" s="7" t="s">
         <v>3</v>
@@ -9059,7 +9067,7 @@
       </c>
       <c r="B393" s="9"/>
       <c r="C393" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D393" s="7" t="s">
         <v>3</v>
@@ -9071,7 +9079,7 @@
       </c>
       <c r="B394" s="9"/>
       <c r="C394" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D394" s="7" t="s">
         <v>3</v>
@@ -9083,7 +9091,7 @@
       </c>
       <c r="B395" s="9"/>
       <c r="C395" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D395" s="7" t="s">
         <v>3</v>
@@ -9095,7 +9103,7 @@
       </c>
       <c r="B396" s="9"/>
       <c r="C396" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D396" s="7" t="s">
         <v>3</v>
@@ -9107,7 +9115,7 @@
       </c>
       <c r="B397" s="9"/>
       <c r="C397" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D397" s="7" t="s">
         <v>3</v>
@@ -9119,7 +9127,7 @@
       </c>
       <c r="B398" s="9"/>
       <c r="C398" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D398" s="7" t="s">
         <v>3</v>
@@ -9131,7 +9139,7 @@
       </c>
       <c r="B399" s="9"/>
       <c r="C399" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D399" s="7" t="s">
         <v>3</v>
@@ -9143,7 +9151,7 @@
       </c>
       <c r="B400" s="9"/>
       <c r="C400" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D400" s="7" t="s">
         <v>3</v>
@@ -9155,7 +9163,7 @@
       </c>
       <c r="B401" s="9"/>
       <c r="C401" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D401" s="7" t="s">
         <v>3</v>
@@ -9167,7 +9175,7 @@
       </c>
       <c r="B402" s="9"/>
       <c r="C402" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D402" s="7" t="s">
         <v>3</v>
@@ -9179,7 +9187,7 @@
       </c>
       <c r="B403" s="9"/>
       <c r="C403" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D403" s="7" t="s">
         <v>3</v>
@@ -9191,7 +9199,7 @@
       </c>
       <c r="B404" s="9"/>
       <c r="C404" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D404" s="7" t="s">
         <v>3</v>
@@ -9203,7 +9211,7 @@
       </c>
       <c r="B405" s="9"/>
       <c r="C405" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D405" s="7" t="s">
         <v>3</v>
@@ -9215,7 +9223,7 @@
       </c>
       <c r="B406" s="9"/>
       <c r="C406" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D406" s="7" t="s">
         <v>3</v>
@@ -9227,7 +9235,7 @@
       </c>
       <c r="B407" s="9"/>
       <c r="C407" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D407" s="7" t="s">
         <v>3</v>
@@ -9239,7 +9247,7 @@
       </c>
       <c r="B408" s="9"/>
       <c r="C408" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D408" s="7" t="s">
         <v>3</v>
@@ -9251,7 +9259,7 @@
       </c>
       <c r="B409" s="9"/>
       <c r="C409" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D409" s="7" t="s">
         <v>3</v>
@@ -9263,7 +9271,7 @@
       </c>
       <c r="B410" s="9"/>
       <c r="C410" s="10" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="D410" s="7" t="s">
         <v>3</v>
@@ -9275,29 +9283,29 @@
       </c>
       <c r="B411" s="9"/>
       <c r="C411" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D411" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A412" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B412" s="9"/>
+      <c r="C412" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="D411" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="D412" s="7"/>
+      <c r="D412" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D413" s="7"/>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A414" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="B414" s="9"/>
-      <c r="C414" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="D414" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D414" s="7"/>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A415" s="9" t="s">
@@ -9305,7 +9313,7 @@
       </c>
       <c r="B415" s="9"/>
       <c r="C415" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D415" s="7" t="s">
         <v>3</v>
@@ -9317,7 +9325,7 @@
       </c>
       <c r="B416" s="9"/>
       <c r="C416" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D416" s="7" t="s">
         <v>3</v>
@@ -9329,7 +9337,7 @@
       </c>
       <c r="B417" s="9"/>
       <c r="C417" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D417" s="7" t="s">
         <v>3</v>
@@ -9341,7 +9349,7 @@
       </c>
       <c r="B418" s="9"/>
       <c r="C418" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D418" s="7" t="s">
         <v>3</v>
@@ -9353,7 +9361,7 @@
       </c>
       <c r="B419" s="9"/>
       <c r="C419" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D419" s="7" t="s">
         <v>3</v>
@@ -9365,7 +9373,7 @@
       </c>
       <c r="B420" s="9"/>
       <c r="C420" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D420" s="7" t="s">
         <v>3</v>
@@ -9377,7 +9385,7 @@
       </c>
       <c r="B421" s="9"/>
       <c r="C421" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D421" s="7" t="s">
         <v>3</v>
@@ -9389,7 +9397,7 @@
       </c>
       <c r="B422" s="9"/>
       <c r="C422" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D422" s="7" t="s">
         <v>3</v>
@@ -9401,7 +9409,7 @@
       </c>
       <c r="B423" s="9"/>
       <c r="C423" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D423" s="7" t="s">
         <v>3</v>
@@ -9413,7 +9421,7 @@
       </c>
       <c r="B424" s="9"/>
       <c r="C424" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D424" s="7" t="s">
         <v>3</v>
@@ -9425,7 +9433,7 @@
       </c>
       <c r="B425" s="9"/>
       <c r="C425" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D425" s="7" t="s">
         <v>3</v>
@@ -9437,7 +9445,7 @@
       </c>
       <c r="B426" s="9"/>
       <c r="C426" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D426" s="7" t="s">
         <v>3</v>
@@ -9449,7 +9457,7 @@
       </c>
       <c r="B427" s="9"/>
       <c r="C427" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D427" s="7" t="s">
         <v>3</v>
@@ -9461,7 +9469,7 @@
       </c>
       <c r="B428" s="9"/>
       <c r="C428" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D428" s="7" t="s">
         <v>3</v>
@@ -9473,7 +9481,7 @@
       </c>
       <c r="B429" s="9"/>
       <c r="C429" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D429" s="7" t="s">
         <v>3</v>
@@ -9485,7 +9493,7 @@
       </c>
       <c r="B430" s="9"/>
       <c r="C430" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D430" s="7" t="s">
         <v>3</v>
@@ -9497,7 +9505,7 @@
       </c>
       <c r="B431" s="9"/>
       <c r="C431" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D431" s="7" t="s">
         <v>3</v>
@@ -9509,26 +9517,26 @@
       </c>
       <c r="B432" s="9"/>
       <c r="C432" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D432" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A433" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B433" s="9"/>
+      <c r="C433" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="D432" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="433" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="D433" s="7"/>
+      <c r="D433" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A434" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="B434" s="9"/>
-      <c r="C434" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="D434" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D434" s="7"/>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A435" s="9" t="s">
@@ -9536,7 +9544,7 @@
       </c>
       <c r="B435" s="9"/>
       <c r="C435" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D435" s="7" t="s">
         <v>3</v>
@@ -9548,7 +9556,7 @@
       </c>
       <c r="B436" s="9"/>
       <c r="C436" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D436" s="7" t="s">
         <v>3</v>
@@ -9560,7 +9568,7 @@
       </c>
       <c r="B437" s="9"/>
       <c r="C437" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D437" s="7" t="s">
         <v>3</v>
@@ -9572,7 +9580,7 @@
       </c>
       <c r="B438" s="9"/>
       <c r="C438" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D438" s="7" t="s">
         <v>3</v>
@@ -9584,7 +9592,7 @@
       </c>
       <c r="B439" s="9"/>
       <c r="C439" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D439" s="7" t="s">
         <v>3</v>
@@ -9596,7 +9604,7 @@
       </c>
       <c r="B440" s="9"/>
       <c r="C440" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D440" s="7" t="s">
         <v>3</v>
@@ -9608,7 +9616,7 @@
       </c>
       <c r="B441" s="9"/>
       <c r="C441" s="10" t="s">
-        <v>262</v>
+        <v>389</v>
       </c>
       <c r="D441" s="7" t="s">
         <v>3</v>
@@ -9620,7 +9628,7 @@
       </c>
       <c r="B442" s="9"/>
       <c r="C442" s="10" t="s">
-        <v>390</v>
+        <v>262</v>
       </c>
       <c r="D442" s="7" t="s">
         <v>3</v>
@@ -9632,7 +9640,7 @@
       </c>
       <c r="B443" s="9"/>
       <c r="C443" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D443" s="7" t="s">
         <v>3</v>
@@ -9644,7 +9652,7 @@
       </c>
       <c r="B444" s="9"/>
       <c r="C444" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D444" s="7" t="s">
         <v>3</v>
@@ -9656,7 +9664,7 @@
       </c>
       <c r="B445" s="9"/>
       <c r="C445" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D445" s="7" t="s">
         <v>3</v>
@@ -9668,7 +9676,7 @@
       </c>
       <c r="B446" s="9"/>
       <c r="C446" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D446" s="7" t="s">
         <v>3</v>
@@ -9680,7 +9688,7 @@
       </c>
       <c r="B447" s="9"/>
       <c r="C447" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D447" s="7" t="s">
         <v>3</v>
@@ -9692,7 +9700,7 @@
       </c>
       <c r="B448" s="9"/>
       <c r="C448" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D448" s="7" t="s">
         <v>3</v>
@@ -9704,7 +9712,7 @@
       </c>
       <c r="B449" s="9"/>
       <c r="C449" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D449" s="7" t="s">
         <v>3</v>
@@ -9716,7 +9724,7 @@
       </c>
       <c r="B450" s="9"/>
       <c r="C450" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D450" s="7" t="s">
         <v>3</v>
@@ -9728,7 +9736,7 @@
       </c>
       <c r="B451" s="9"/>
       <c r="C451" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D451" s="7" t="s">
         <v>3</v>
@@ -9740,7 +9748,7 @@
       </c>
       <c r="B452" s="9"/>
       <c r="C452" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D452" s="7" t="s">
         <v>3</v>
@@ -9752,7 +9760,7 @@
       </c>
       <c r="B453" s="9"/>
       <c r="C453" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D453" s="7" t="s">
         <v>3</v>
@@ -9764,7 +9772,7 @@
       </c>
       <c r="B454" s="9"/>
       <c r="C454" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D454" s="7" t="s">
         <v>3</v>
@@ -9776,7 +9784,7 @@
       </c>
       <c r="B455" s="9"/>
       <c r="C455" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D455" s="7" t="s">
         <v>3</v>
@@ -9788,7 +9796,7 @@
       </c>
       <c r="B456" s="9"/>
       <c r="C456" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D456" s="7" t="s">
         <v>3</v>
@@ -9800,7 +9808,7 @@
       </c>
       <c r="B457" s="9"/>
       <c r="C457" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D457" s="7" t="s">
         <v>3</v>
@@ -9812,7 +9820,7 @@
       </c>
       <c r="B458" s="9"/>
       <c r="C458" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D458" s="7" t="s">
         <v>3</v>
@@ -9824,7 +9832,7 @@
       </c>
       <c r="B459" s="9"/>
       <c r="C459" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D459" s="7" t="s">
         <v>3</v>
@@ -9836,7 +9844,7 @@
       </c>
       <c r="B460" s="9"/>
       <c r="C460" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D460" s="7" t="s">
         <v>3</v>
@@ -9848,7 +9856,7 @@
       </c>
       <c r="B461" s="9"/>
       <c r="C461" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D461" s="7" t="s">
         <v>3</v>
@@ -9860,7 +9868,7 @@
       </c>
       <c r="B462" s="9"/>
       <c r="C462" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D462" s="7" t="s">
         <v>3</v>
@@ -9872,7 +9880,7 @@
       </c>
       <c r="B463" s="9"/>
       <c r="C463" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D463" s="7" t="s">
         <v>3</v>
@@ -9884,7 +9892,7 @@
       </c>
       <c r="B464" s="9"/>
       <c r="C464" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D464" s="7" t="s">
         <v>3</v>
@@ -9896,7 +9904,7 @@
       </c>
       <c r="B465" s="9"/>
       <c r="C465" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D465" s="7" t="s">
         <v>3</v>
@@ -9908,7 +9916,7 @@
       </c>
       <c r="B466" s="9"/>
       <c r="C466" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D466" s="7" t="s">
         <v>3</v>
@@ -9920,7 +9928,7 @@
       </c>
       <c r="B467" s="9"/>
       <c r="C467" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D467" s="7" t="s">
         <v>3</v>
@@ -9932,7 +9940,7 @@
       </c>
       <c r="B468" s="9"/>
       <c r="C468" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D468" s="7" t="s">
         <v>3</v>
@@ -9944,7 +9952,7 @@
       </c>
       <c r="B469" s="9"/>
       <c r="C469" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D469" s="7" t="s">
         <v>3</v>
@@ -9956,7 +9964,7 @@
       </c>
       <c r="B470" s="9"/>
       <c r="C470" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D470" s="7" t="s">
         <v>3</v>
@@ -9968,7 +9976,7 @@
       </c>
       <c r="B471" s="9"/>
       <c r="C471" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D471" s="7" t="s">
         <v>3</v>
@@ -9980,7 +9988,7 @@
       </c>
       <c r="B472" s="9"/>
       <c r="C472" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D472" s="7" t="s">
         <v>3</v>
@@ -9992,7 +10000,7 @@
       </c>
       <c r="B473" s="9"/>
       <c r="C473" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D473" s="7" t="s">
         <v>3</v>
@@ -10004,7 +10012,7 @@
       </c>
       <c r="B474" s="9"/>
       <c r="C474" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D474" s="7" t="s">
         <v>3</v>
@@ -10016,7 +10024,7 @@
       </c>
       <c r="B475" s="9"/>
       <c r="C475" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D475" s="7" t="s">
         <v>3</v>
@@ -10028,7 +10036,7 @@
       </c>
       <c r="B476" s="9"/>
       <c r="C476" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D476" s="7" t="s">
         <v>3</v>
@@ -10040,7 +10048,7 @@
       </c>
       <c r="B477" s="9"/>
       <c r="C477" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D477" s="7" t="s">
         <v>3</v>
@@ -10052,7 +10060,7 @@
       </c>
       <c r="B478" s="9"/>
       <c r="C478" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D478" s="7" t="s">
         <v>3</v>
@@ -10064,7 +10072,7 @@
       </c>
       <c r="B479" s="9"/>
       <c r="C479" s="10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D479" s="7" t="s">
         <v>3</v>
@@ -10076,7 +10084,7 @@
       </c>
       <c r="B480" s="9"/>
       <c r="C480" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D480" s="7" t="s">
         <v>3</v>
@@ -10088,7 +10096,7 @@
       </c>
       <c r="B481" s="9"/>
       <c r="C481" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D481" s="7" t="s">
         <v>3</v>
@@ -10100,7 +10108,7 @@
       </c>
       <c r="B482" s="9"/>
       <c r="C482" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D482" s="7" t="s">
         <v>3</v>
@@ -10112,7 +10120,7 @@
       </c>
       <c r="B483" s="9"/>
       <c r="C483" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D483" s="7" t="s">
         <v>3</v>
@@ -10124,7 +10132,7 @@
       </c>
       <c r="B484" s="9"/>
       <c r="C484" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D484" s="7" t="s">
         <v>3</v>
@@ -10136,7 +10144,7 @@
       </c>
       <c r="B485" s="9"/>
       <c r="C485" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D485" s="7" t="s">
         <v>3</v>
@@ -10148,7 +10156,7 @@
       </c>
       <c r="B486" s="9"/>
       <c r="C486" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D486" s="7" t="s">
         <v>3</v>
@@ -10160,7 +10168,7 @@
       </c>
       <c r="B487" s="9"/>
       <c r="C487" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D487" s="7" t="s">
         <v>3</v>
@@ -10172,7 +10180,7 @@
       </c>
       <c r="B488" s="9"/>
       <c r="C488" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D488" s="7" t="s">
         <v>3</v>
@@ -10184,7 +10192,7 @@
       </c>
       <c r="B489" s="9"/>
       <c r="C489" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D489" s="7" t="s">
         <v>3</v>
@@ -10196,7 +10204,7 @@
       </c>
       <c r="B490" s="9"/>
       <c r="C490" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D490" s="7" t="s">
         <v>3</v>
@@ -10208,7 +10216,7 @@
       </c>
       <c r="B491" s="9"/>
       <c r="C491" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D491" s="7" t="s">
         <v>3</v>
@@ -10220,7 +10228,7 @@
       </c>
       <c r="B492" s="9"/>
       <c r="C492" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D492" s="7" t="s">
         <v>3</v>
@@ -10232,7 +10240,7 @@
       </c>
       <c r="B493" s="9"/>
       <c r="C493" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D493" s="7" t="s">
         <v>3</v>
@@ -10242,50 +10250,50 @@
       <c r="A494" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="B494" s="9" t="s">
+      <c r="B494" s="9"/>
+      <c r="C494" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="D494" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="495" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A495" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="B495" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="C494" s="10" t="s">
+      <c r="C495" s="10" t="s">
         <v>524</v>
       </c>
-      <c r="D494" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="E494" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="F494" s="20" t="s">
-        <v>512</v>
-      </c>
-      <c r="G494" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="H494" s="22" t="s">
+      <c r="D495" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="E495" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F495" s="20" t="s">
+        <v>512</v>
+      </c>
+      <c r="G495" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H495" s="22" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A495" s="9"/>
-      <c r="B495" s="9"/>
-      <c r="C495" s="10"/>
-      <c r="D495" s="10"/>
-      <c r="E495" s="10"/>
-      <c r="F495" s="10"/>
-      <c r="G495" s="10"/>
-      <c r="H495" s="10"/>
-      <c r="I495" s="10"/>
-    </row>
     <row r="496" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A496" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="B496" s="7"/>
-      <c r="C496" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="D496" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="A496" s="9"/>
+      <c r="B496" s="9"/>
+      <c r="C496" s="10"/>
+      <c r="D496" s="10"/>
+      <c r="E496" s="10"/>
+      <c r="F496" s="10"/>
+      <c r="G496" s="10"/>
+      <c r="H496" s="10"/>
+      <c r="I496" s="10"/>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A497" s="7" t="s">
@@ -10293,7 +10301,7 @@
       </c>
       <c r="B497" s="7"/>
       <c r="C497" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D497" s="7" t="s">
         <v>3</v>
@@ -10305,7 +10313,7 @@
       </c>
       <c r="B498" s="7"/>
       <c r="C498" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D498" s="7" t="s">
         <v>3</v>
@@ -10317,7 +10325,7 @@
       </c>
       <c r="B499" s="7"/>
       <c r="C499" s="10" t="s">
-        <v>85</v>
+        <v>379</v>
       </c>
       <c r="D499" s="7" t="s">
         <v>3</v>
@@ -10329,7 +10337,7 @@
       </c>
       <c r="B500" s="7"/>
       <c r="C500" s="10" t="s">
-        <v>380</v>
+        <v>85</v>
       </c>
       <c r="D500" s="7" t="s">
         <v>3</v>
@@ -10341,14 +10349,23 @@
       </c>
       <c r="B501" s="7"/>
       <c r="C501" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="D501" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A502" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="B502" s="7"/>
+      <c r="C502" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="D501" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="502" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="D502" s="7"/>
+      <c r="D502" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D503" s="7"/>
@@ -10375,9 +10392,12 @@
       <c r="D510" s="7"/>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A511" s="7"/>
-      <c r="B511" s="7"/>
       <c r="D511" s="7"/>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A512" s="7"/>
+      <c r="B512" s="7"/>
+      <c r="D512" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10408,7 +10428,7 @@
     <hyperlink ref="C41" r:id="rId20" xr:uid="{74F8D761-6EBF-594A-A6C7-40DE4CE96958}"/>
     <hyperlink ref="C81" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
     <hyperlink ref="C42" r:id="rId22" display="Find factorial of a large number" xr:uid="{2BF3F606-410B-264D-BF60-191C34D616BB}"/>
-    <hyperlink ref="C494" r:id="rId23" display="find maximum product subarray " xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
+    <hyperlink ref="C495" r:id="rId23" display="find maximum product subarray " xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
     <hyperlink ref="C82" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
     <hyperlink ref="C83" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
     <hyperlink ref="C43" r:id="rId26" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
@@ -10422,12 +10442,12 @@
     <hyperlink ref="C50" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
     <hyperlink ref="C51" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
     <hyperlink ref="C52" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
-    <hyperlink ref="C167" r:id="rId37" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="C168" r:id="rId38" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="C169" r:id="rId39" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="C170" r:id="rId40" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
-    <hyperlink ref="C171" r:id="rId41" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
-    <hyperlink ref="C172" r:id="rId42" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
+    <hyperlink ref="C168" r:id="rId37" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
+    <hyperlink ref="C169" r:id="rId38" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
+    <hyperlink ref="C170" r:id="rId39" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
+    <hyperlink ref="C171" r:id="rId40" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
+    <hyperlink ref="C172" r:id="rId41" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
+    <hyperlink ref="C173" r:id="rId42" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
     <hyperlink ref="C87" r:id="rId43" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
     <hyperlink ref="C88" r:id="rId44" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
     <hyperlink ref="C89" r:id="rId45" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
@@ -10443,7 +10463,7 @@
     <hyperlink ref="C79" r:id="rId55" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
     <hyperlink ref="C105" r:id="rId56" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
     <hyperlink ref="C106" r:id="rId57" display="Sort array according to count of set bits" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
-    <hyperlink ref="C375" r:id="rId58" display="minimum no. of swaps required to sort the array" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
+    <hyperlink ref="C376" r:id="rId58" display="minimum no. of swaps required to sort the array" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
     <hyperlink ref="C107" r:id="rId59" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
     <hyperlink ref="C108" r:id="rId60" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
     <hyperlink ref="C109" r:id="rId61" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
@@ -10464,316 +10484,316 @@
     <hyperlink ref="C124" r:id="rId76" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
     <hyperlink ref="C92" r:id="rId77" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
     <hyperlink ref="C102" r:id="rId78" display="maximum sum such that no 2 elements are adjacent" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
-    <hyperlink ref="C176" r:id="rId79" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
-    <hyperlink ref="C177" r:id="rId80" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
-    <hyperlink ref="C178" r:id="rId81" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
-    <hyperlink ref="C179" r:id="rId82" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
-    <hyperlink ref="C180" r:id="rId83" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
-    <hyperlink ref="C181" r:id="rId84" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
-    <hyperlink ref="C182" r:id="rId85" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
-    <hyperlink ref="C183" r:id="rId86" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
-    <hyperlink ref="C184" r:id="rId87" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
-    <hyperlink ref="C185" r:id="rId88" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
-    <hyperlink ref="C186" r:id="rId89" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
-    <hyperlink ref="C187" r:id="rId90" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
-    <hyperlink ref="C188" r:id="rId91" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
-    <hyperlink ref="C189" r:id="rId92" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
-    <hyperlink ref="C190" r:id="rId93" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
-    <hyperlink ref="C191" r:id="rId94" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
-    <hyperlink ref="C192" r:id="rId95" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
-    <hyperlink ref="C193" r:id="rId96" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
-    <hyperlink ref="C194" r:id="rId97" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
-    <hyperlink ref="C195" r:id="rId98" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
-    <hyperlink ref="C196" r:id="rId99" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
-    <hyperlink ref="C197" r:id="rId100" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
-    <hyperlink ref="C198" r:id="rId101" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
-    <hyperlink ref="C199" r:id="rId102" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
-    <hyperlink ref="C200" r:id="rId103" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
-    <hyperlink ref="C203" r:id="rId104" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
-    <hyperlink ref="C204" r:id="rId105" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
-    <hyperlink ref="C205" r:id="rId106" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
-    <hyperlink ref="C206" r:id="rId107" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
-    <hyperlink ref="C207" r:id="rId108" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
-    <hyperlink ref="C208" r:id="rId109" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
-    <hyperlink ref="C209" r:id="rId110" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
-    <hyperlink ref="C210" r:id="rId111" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
-    <hyperlink ref="C211" r:id="rId112" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="C252" r:id="rId113" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="C253" r:id="rId114" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="C254" r:id="rId115" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="C255" r:id="rId116" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="C256" r:id="rId117" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="C257" r:id="rId118" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="C258" r:id="rId119" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="C259" r:id="rId120" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="C260" r:id="rId121" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="C261" r:id="rId122" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="C262" r:id="rId123" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="C263" r:id="rId124" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="C264" r:id="rId125" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="C265" r:id="rId126" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="C266" r:id="rId127" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="C267" r:id="rId128" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="C268" r:id="rId129" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="C269" r:id="rId130" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="C270" r:id="rId131" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="C271" r:id="rId132" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="C272" r:id="rId133" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="C273" r:id="rId134" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="C274" r:id="rId135" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="C275" r:id="rId136" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="C276" r:id="rId137" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="C277" r:id="rId138" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="C278" r:id="rId139" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="C279" r:id="rId140" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="C280" r:id="rId141" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="C281" r:id="rId142" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="C282" r:id="rId143" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="C283" r:id="rId144" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="C284" r:id="rId145" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="C285" r:id="rId146" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="C286" r:id="rId147" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="C289" r:id="rId148" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="C290" r:id="rId149" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="C291" r:id="rId150" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="C292" r:id="rId151" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="C293" r:id="rId152" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="C294" r:id="rId153" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="C295" r:id="rId154" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="C296" r:id="rId155" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="C297" r:id="rId156" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="C298" r:id="rId157" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="C299" r:id="rId158" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="C300" r:id="rId159" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="C301" r:id="rId160" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="C302" r:id="rId161" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="C303" r:id="rId162" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="C304" r:id="rId163" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="C305" r:id="rId164" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="C306" r:id="rId165" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="C307" r:id="rId166" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="C308" r:id="rId167" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="C309" r:id="rId168" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="C310" r:id="rId169" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="C377" r:id="rId170" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="C378" r:id="rId171" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="C379" r:id="rId172" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="C380" r:id="rId173" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="C381" r:id="rId174" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="C382" r:id="rId175" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="C383" r:id="rId176" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="C384" r:id="rId177" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="C385" r:id="rId178" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="C386" r:id="rId179" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="C387" r:id="rId180" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="C388" r:id="rId181" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="C389" r:id="rId182" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="C390" r:id="rId183" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="C391" r:id="rId184" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="C392" r:id="rId185" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="C393" r:id="rId186" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="C394" r:id="rId187" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="C395" r:id="rId188" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="C396" r:id="rId189" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="C397" r:id="rId190" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="C398" r:id="rId191" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="C399" r:id="rId192" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="C400" r:id="rId193" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="C401" r:id="rId194" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="C402" r:id="rId195" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="C403" r:id="rId196" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="C404" r:id="rId197" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="C405" r:id="rId198" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="C406" r:id="rId199" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="C407" r:id="rId200" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="C408" r:id="rId201" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="C409" r:id="rId202" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="C410" r:id="rId203" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="C411" r:id="rId204" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="C414" r:id="rId205" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="C415" r:id="rId206" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="C416" r:id="rId207" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="C417" r:id="rId208" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="C418" r:id="rId209" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="C419" r:id="rId210" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="C420" r:id="rId211" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="C421" r:id="rId212" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="C422" r:id="rId213" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="C423" r:id="rId214" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="C424" r:id="rId215" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="C425" r:id="rId216" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="C426" r:id="rId217" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="C427" r:id="rId218" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="C428" r:id="rId219" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="C429" r:id="rId220" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="C430" r:id="rId221" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="C431" r:id="rId222" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="C432" r:id="rId223" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="C213" r:id="rId224" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="C214" r:id="rId225" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="C215" r:id="rId226" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="C216" r:id="rId227" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="C217" r:id="rId228" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="C218" r:id="rId229" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="C219" r:id="rId230" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="C220" r:id="rId231" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="C221" r:id="rId232" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="C222" r:id="rId233" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="C223" r:id="rId234" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="C224" r:id="rId235" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="C225" r:id="rId236" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="C226" r:id="rId237" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="C227" r:id="rId238" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="C228" r:id="rId239" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="C229" r:id="rId240" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="C230" r:id="rId241" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="C231" r:id="rId242" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="C232" r:id="rId243" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="C233" r:id="rId244" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="C234" r:id="rId245" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="C235" r:id="rId246" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="C236" r:id="rId247" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="C237" r:id="rId248" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="C238" r:id="rId249" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="C239" r:id="rId250" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="C240" r:id="rId251" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="C241" r:id="rId252" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="C242" r:id="rId253" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="C243" r:id="rId254" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="C244" r:id="rId255" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="C245" r:id="rId256" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="C246" r:id="rId257" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="C247" r:id="rId258" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="C248" r:id="rId259" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="C249" r:id="rId260" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="C250" r:id="rId261" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="C312" r:id="rId262" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="C313" r:id="rId263" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="C314" r:id="rId264" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="C315" r:id="rId265" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="C316" r:id="rId266" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="C317" r:id="rId267" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="C318" r:id="rId268" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="C319" r:id="rId269" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="C320" r:id="rId270" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="C321" r:id="rId271" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="C322" r:id="rId272" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="C323" r:id="rId273" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="C324" r:id="rId274" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="C325" r:id="rId275" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="C326" r:id="rId276" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="C327" r:id="rId277" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="C328" r:id="rId278" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="C329" r:id="rId279" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="C332" r:id="rId280" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="C333" r:id="rId281" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="C334" r:id="rId282" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="C335" r:id="rId283" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="C336" r:id="rId284" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="C337" r:id="rId285" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="C338" r:id="rId286" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="C339" r:id="rId287" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="C340" r:id="rId288" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="C341" r:id="rId289" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="C342" r:id="rId290" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="C343" r:id="rId291" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="C344" r:id="rId292" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="C345" r:id="rId293" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="C346" r:id="rId294" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="C347" r:id="rId295" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="C348" r:id="rId296" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="C349" r:id="rId297" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="C350" r:id="rId298" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="C351" r:id="rId299" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="C352" r:id="rId300" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="C353" r:id="rId301" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="C354" r:id="rId302" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="C355" r:id="rId303" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="C356" r:id="rId304" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="C357" r:id="rId305" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="C358" r:id="rId306" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="C359" r:id="rId307" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="C360" r:id="rId308" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="C361" r:id="rId309" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="C362" r:id="rId310" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="C363" r:id="rId311" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="C364" r:id="rId312" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="C365" r:id="rId313" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="C366" r:id="rId314" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="C367" r:id="rId315" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="C368" r:id="rId316" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="C369" r:id="rId317" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="C371" r:id="rId318" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="C370" r:id="rId319" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="C372" r:id="rId320" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="C373" r:id="rId321" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="C374" r:id="rId322" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="C496" r:id="rId323" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="C497" r:id="rId324" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="C498" r:id="rId325" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="C499" r:id="rId326" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="C500" r:id="rId327" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="C501" r:id="rId328" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="C434" r:id="rId329" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="C435" r:id="rId330" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="C436" r:id="rId331" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="C437" r:id="rId332" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="C438" r:id="rId333" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="C439" r:id="rId334" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="C440" r:id="rId335" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="C441" r:id="rId336" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="C442" r:id="rId337" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="C443" r:id="rId338" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="C444" r:id="rId339" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="C445" r:id="rId340" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="C446" r:id="rId341" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="C447" r:id="rId342" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="C448" r:id="rId343" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="C449" r:id="rId344" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="C450" r:id="rId345" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="C451" r:id="rId346" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="C452" r:id="rId347" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="C453" r:id="rId348" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="C454" r:id="rId349" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="C455" r:id="rId350" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="C456" r:id="rId351" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="C457" r:id="rId352" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="C458" r:id="rId353" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="C459" r:id="rId354" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="C460" r:id="rId355" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="C461" r:id="rId356" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="C462" r:id="rId357" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="C463" r:id="rId358" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="C464" r:id="rId359" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="C465" r:id="rId360" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="C466" r:id="rId361" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="C467" r:id="rId362" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="C468" r:id="rId363" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="C469" r:id="rId364" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="C470" r:id="rId365" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="C471" r:id="rId366" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="C472" r:id="rId367" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="C473" r:id="rId368" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="C475" r:id="rId369" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="C474" r:id="rId370" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="C476" r:id="rId371" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="C477" r:id="rId372" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="C478" r:id="rId373" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="C479" r:id="rId374" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="C480" r:id="rId375" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="C481" r:id="rId376" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="C482" r:id="rId377" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="C483" r:id="rId378" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="C484" r:id="rId379" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="C485" r:id="rId380" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="C486" r:id="rId381" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="C493" r:id="rId382" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="C492" r:id="rId383" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="C491" r:id="rId384" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="C490" r:id="rId385" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="C489" r:id="rId386" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="C488" r:id="rId387" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="C487" r:id="rId388" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="C177" r:id="rId79" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
+    <hyperlink ref="C178" r:id="rId80" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
+    <hyperlink ref="C179" r:id="rId81" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
+    <hyperlink ref="C180" r:id="rId82" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
+    <hyperlink ref="C181" r:id="rId83" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
+    <hyperlink ref="C182" r:id="rId84" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
+    <hyperlink ref="C183" r:id="rId85" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
+    <hyperlink ref="C184" r:id="rId86" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
+    <hyperlink ref="C185" r:id="rId87" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
+    <hyperlink ref="C186" r:id="rId88" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
+    <hyperlink ref="C187" r:id="rId89" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
+    <hyperlink ref="C188" r:id="rId90" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
+    <hyperlink ref="C189" r:id="rId91" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
+    <hyperlink ref="C190" r:id="rId92" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
+    <hyperlink ref="C191" r:id="rId93" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
+    <hyperlink ref="C192" r:id="rId94" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
+    <hyperlink ref="C193" r:id="rId95" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
+    <hyperlink ref="C194" r:id="rId96" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
+    <hyperlink ref="C195" r:id="rId97" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
+    <hyperlink ref="C196" r:id="rId98" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
+    <hyperlink ref="C197" r:id="rId99" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
+    <hyperlink ref="C198" r:id="rId100" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
+    <hyperlink ref="C199" r:id="rId101" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
+    <hyperlink ref="C200" r:id="rId102" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
+    <hyperlink ref="C201" r:id="rId103" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
+    <hyperlink ref="C204" r:id="rId104" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
+    <hyperlink ref="C205" r:id="rId105" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
+    <hyperlink ref="C206" r:id="rId106" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
+    <hyperlink ref="C207" r:id="rId107" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
+    <hyperlink ref="C208" r:id="rId108" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
+    <hyperlink ref="C209" r:id="rId109" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
+    <hyperlink ref="C210" r:id="rId110" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
+    <hyperlink ref="C211" r:id="rId111" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
+    <hyperlink ref="C212" r:id="rId112" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
+    <hyperlink ref="C253" r:id="rId113" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="C254" r:id="rId114" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="C255" r:id="rId115" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="C256" r:id="rId116" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="C257" r:id="rId117" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="C258" r:id="rId118" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="C259" r:id="rId119" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="C260" r:id="rId120" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="C261" r:id="rId121" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="C262" r:id="rId122" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="C263" r:id="rId123" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="C264" r:id="rId124" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="C265" r:id="rId125" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="C266" r:id="rId126" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="C267" r:id="rId127" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="C268" r:id="rId128" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="C269" r:id="rId129" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="C270" r:id="rId130" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="C271" r:id="rId131" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="C272" r:id="rId132" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="C273" r:id="rId133" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="C274" r:id="rId134" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="C275" r:id="rId135" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="C276" r:id="rId136" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="C277" r:id="rId137" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="C278" r:id="rId138" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="C279" r:id="rId139" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="C280" r:id="rId140" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="C281" r:id="rId141" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="C282" r:id="rId142" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="C283" r:id="rId143" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="C284" r:id="rId144" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="C285" r:id="rId145" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="C286" r:id="rId146" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="C287" r:id="rId147" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="C290" r:id="rId148" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="C291" r:id="rId149" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="C292" r:id="rId150" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="C293" r:id="rId151" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="C294" r:id="rId152" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="C295" r:id="rId153" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="C296" r:id="rId154" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="C297" r:id="rId155" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="C298" r:id="rId156" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="C299" r:id="rId157" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="C300" r:id="rId158" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="C301" r:id="rId159" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="C302" r:id="rId160" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="C303" r:id="rId161" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="C304" r:id="rId162" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="C305" r:id="rId163" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="C306" r:id="rId164" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="C307" r:id="rId165" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="C308" r:id="rId166" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="C309" r:id="rId167" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="C310" r:id="rId168" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="C311" r:id="rId169" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="C378" r:id="rId170" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="C379" r:id="rId171" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="C380" r:id="rId172" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="C381" r:id="rId173" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="C382" r:id="rId174" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="C383" r:id="rId175" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="C384" r:id="rId176" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="C385" r:id="rId177" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="C386" r:id="rId178" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="C387" r:id="rId179" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="C388" r:id="rId180" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="C389" r:id="rId181" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="C390" r:id="rId182" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="C391" r:id="rId183" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="C392" r:id="rId184" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="C393" r:id="rId185" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="C394" r:id="rId186" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="C395" r:id="rId187" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="C396" r:id="rId188" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="C397" r:id="rId189" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="C398" r:id="rId190" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="C399" r:id="rId191" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="C400" r:id="rId192" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="C401" r:id="rId193" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="C402" r:id="rId194" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="C403" r:id="rId195" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="C404" r:id="rId196" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="C405" r:id="rId197" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="C406" r:id="rId198" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="C407" r:id="rId199" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="C408" r:id="rId200" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="C409" r:id="rId201" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="C410" r:id="rId202" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="C411" r:id="rId203" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="C412" r:id="rId204" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="C415" r:id="rId205" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="C416" r:id="rId206" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="C417" r:id="rId207" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="C418" r:id="rId208" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="C419" r:id="rId209" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="C420" r:id="rId210" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="C421" r:id="rId211" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="C422" r:id="rId212" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="C423" r:id="rId213" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="C424" r:id="rId214" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="C425" r:id="rId215" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="C426" r:id="rId216" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="C427" r:id="rId217" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="C428" r:id="rId218" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="C429" r:id="rId219" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="C430" r:id="rId220" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="C431" r:id="rId221" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="C432" r:id="rId222" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="C433" r:id="rId223" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="C214" r:id="rId224" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="C215" r:id="rId225" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="C216" r:id="rId226" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="C217" r:id="rId227" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="C218" r:id="rId228" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="C219" r:id="rId229" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="C220" r:id="rId230" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="C221" r:id="rId231" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="C222" r:id="rId232" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="C223" r:id="rId233" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="C224" r:id="rId234" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="C225" r:id="rId235" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="C226" r:id="rId236" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="C227" r:id="rId237" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="C228" r:id="rId238" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="C229" r:id="rId239" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="C230" r:id="rId240" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="C231" r:id="rId241" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="C232" r:id="rId242" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="C233" r:id="rId243" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="C234" r:id="rId244" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="C235" r:id="rId245" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="C236" r:id="rId246" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="C237" r:id="rId247" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="C238" r:id="rId248" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="C239" r:id="rId249" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="C240" r:id="rId250" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="C241" r:id="rId251" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="C242" r:id="rId252" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="C243" r:id="rId253" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="C244" r:id="rId254" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="C245" r:id="rId255" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="C246" r:id="rId256" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="C247" r:id="rId257" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="C248" r:id="rId258" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="C249" r:id="rId259" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="C250" r:id="rId260" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="C251" r:id="rId261" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="C313" r:id="rId262" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="C314" r:id="rId263" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="C315" r:id="rId264" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="C316" r:id="rId265" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="C317" r:id="rId266" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="C318" r:id="rId267" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="C319" r:id="rId268" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="C320" r:id="rId269" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="C321" r:id="rId270" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="C322" r:id="rId271" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="C323" r:id="rId272" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="C324" r:id="rId273" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="C325" r:id="rId274" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="C326" r:id="rId275" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="C327" r:id="rId276" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="C328" r:id="rId277" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="C329" r:id="rId278" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="C330" r:id="rId279" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="C333" r:id="rId280" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="C334" r:id="rId281" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="C335" r:id="rId282" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="C336" r:id="rId283" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="C337" r:id="rId284" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="C338" r:id="rId285" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="C339" r:id="rId286" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="C340" r:id="rId287" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="C341" r:id="rId288" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="C342" r:id="rId289" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="C343" r:id="rId290" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="C344" r:id="rId291" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="C345" r:id="rId292" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="C346" r:id="rId293" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="C347" r:id="rId294" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="C348" r:id="rId295" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="C349" r:id="rId296" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="C350" r:id="rId297" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="C351" r:id="rId298" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="C352" r:id="rId299" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="C353" r:id="rId300" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="C354" r:id="rId301" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="C355" r:id="rId302" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="C356" r:id="rId303" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="C357" r:id="rId304" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="C358" r:id="rId305" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="C359" r:id="rId306" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="C360" r:id="rId307" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="C361" r:id="rId308" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="C362" r:id="rId309" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="C363" r:id="rId310" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="C364" r:id="rId311" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="C365" r:id="rId312" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="C366" r:id="rId313" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="C367" r:id="rId314" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="C368" r:id="rId315" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="C369" r:id="rId316" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="C370" r:id="rId317" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="C372" r:id="rId318" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="C371" r:id="rId319" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="C373" r:id="rId320" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="C374" r:id="rId321" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="C375" r:id="rId322" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="C497" r:id="rId323" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="C498" r:id="rId324" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="C499" r:id="rId325" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="C500" r:id="rId326" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="C501" r:id="rId327" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="C502" r:id="rId328" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="C435" r:id="rId329" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="C436" r:id="rId330" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="C437" r:id="rId331" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="C438" r:id="rId332" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="C439" r:id="rId333" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="C440" r:id="rId334" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="C441" r:id="rId335" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="C442" r:id="rId336" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="C443" r:id="rId337" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="C444" r:id="rId338" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="C445" r:id="rId339" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="C446" r:id="rId340" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="C447" r:id="rId341" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="C448" r:id="rId342" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="C449" r:id="rId343" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="C450" r:id="rId344" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="C451" r:id="rId345" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="C452" r:id="rId346" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="C453" r:id="rId347" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="C454" r:id="rId348" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="C455" r:id="rId349" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="C456" r:id="rId350" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="C457" r:id="rId351" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="C458" r:id="rId352" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="C459" r:id="rId353" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="C460" r:id="rId354" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="C461" r:id="rId355" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="C462" r:id="rId356" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="C463" r:id="rId357" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="C464" r:id="rId358" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="C465" r:id="rId359" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="C466" r:id="rId360" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="C467" r:id="rId361" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="C468" r:id="rId362" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="C469" r:id="rId363" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="C470" r:id="rId364" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="C471" r:id="rId365" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="C472" r:id="rId366" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="C473" r:id="rId367" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="C474" r:id="rId368" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="C476" r:id="rId369" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="C475" r:id="rId370" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="C477" r:id="rId371" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="C478" r:id="rId372" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="C479" r:id="rId373" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="C480" r:id="rId374" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="C481" r:id="rId375" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="C482" r:id="rId376" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="C483" r:id="rId377" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="C484" r:id="rId378" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="C485" r:id="rId379" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="C486" r:id="rId380" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="C487" r:id="rId381" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="C494" r:id="rId382" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="C493" r:id="rId383" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="C492" r:id="rId384" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="C491" r:id="rId385" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="C490" r:id="rId386" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="C489" r:id="rId387" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="C488" r:id="rId388" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
     <hyperlink ref="C56" r:id="rId389" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
     <hyperlink ref="C57" r:id="rId390" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
     <hyperlink ref="C58" r:id="rId391" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
@@ -10784,7 +10804,7 @@
     <hyperlink ref="C65" r:id="rId396" display="Power Set" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
     <hyperlink ref="C63" r:id="rId397" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
     <hyperlink ref="C64" r:id="rId398" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="C331" r:id="rId399" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="C332" r:id="rId399" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="C126" r:id="rId400" xr:uid="{F0DDC999-C321-4AB4-BA9D-7538150E84D3}"/>
     <hyperlink ref="C9" r:id="rId401" xr:uid="{310D755F-0FAF-4086-8950-B58917F7CAF8}"/>
     <hyperlink ref="C8" r:id="rId402" xr:uid="{6913685B-862A-49D7-AB28-593B13669931}"/>
@@ -10803,36 +10823,36 @@
     <hyperlink ref="C25" r:id="rId415" xr:uid="{93FD35D8-7CCD-456F-8688-AE16CCDD3523}"/>
     <hyperlink ref="C26" r:id="rId416" xr:uid="{F4AF07B8-F8B8-4F27-8CE4-D2E7B73B36A2}"/>
     <hyperlink ref="C34" r:id="rId417" xr:uid="{1895A946-81DF-437C-A537-65287B4088B6}"/>
-    <hyperlink ref="C166" r:id="rId418" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="C165" r:id="rId419" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="C164" r:id="rId420" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="C163" r:id="rId421" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="C162" r:id="rId422" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="C161" r:id="rId423" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="C160" r:id="rId424" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
-    <hyperlink ref="C159" r:id="rId425" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
-    <hyperlink ref="C158" r:id="rId426" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
-    <hyperlink ref="C157" r:id="rId427" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
-    <hyperlink ref="C156" r:id="rId428" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
-    <hyperlink ref="C155" r:id="rId429" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
-    <hyperlink ref="C154" r:id="rId430" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
-    <hyperlink ref="C153" r:id="rId431" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
-    <hyperlink ref="C152" r:id="rId432" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
-    <hyperlink ref="C151" r:id="rId433" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
-    <hyperlink ref="C150" r:id="rId434" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
-    <hyperlink ref="C149" r:id="rId435" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
-    <hyperlink ref="C148" r:id="rId436" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
-    <hyperlink ref="C147" r:id="rId437" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
-    <hyperlink ref="C146" r:id="rId438" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
-    <hyperlink ref="C145" r:id="rId439" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
-    <hyperlink ref="C144" r:id="rId440" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
-    <hyperlink ref="C143" r:id="rId441" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
-    <hyperlink ref="C142" r:id="rId442" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
-    <hyperlink ref="C141" r:id="rId443" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
-    <hyperlink ref="C140" r:id="rId444" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
-    <hyperlink ref="C139" r:id="rId445" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
-    <hyperlink ref="C138" r:id="rId446" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
-    <hyperlink ref="C137" r:id="rId447" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
+    <hyperlink ref="C167" r:id="rId418" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
+    <hyperlink ref="C166" r:id="rId419" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
+    <hyperlink ref="C165" r:id="rId420" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
+    <hyperlink ref="C164" r:id="rId421" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
+    <hyperlink ref="C163" r:id="rId422" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
+    <hyperlink ref="C162" r:id="rId423" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
+    <hyperlink ref="C161" r:id="rId424" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
+    <hyperlink ref="C160" r:id="rId425" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
+    <hyperlink ref="C159" r:id="rId426" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
+    <hyperlink ref="C158" r:id="rId427" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
+    <hyperlink ref="C157" r:id="rId428" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
+    <hyperlink ref="C156" r:id="rId429" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
+    <hyperlink ref="C155" r:id="rId430" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
+    <hyperlink ref="C154" r:id="rId431" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
+    <hyperlink ref="C153" r:id="rId432" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
+    <hyperlink ref="C152" r:id="rId433" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
+    <hyperlink ref="C151" r:id="rId434" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
+    <hyperlink ref="C150" r:id="rId435" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
+    <hyperlink ref="C149" r:id="rId436" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
+    <hyperlink ref="C148" r:id="rId437" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
+    <hyperlink ref="C147" r:id="rId438" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
+    <hyperlink ref="C146" r:id="rId439" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
+    <hyperlink ref="C145" r:id="rId440" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
+    <hyperlink ref="C144" r:id="rId441" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
+    <hyperlink ref="C143" r:id="rId442" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
+    <hyperlink ref="C142" r:id="rId443" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
+    <hyperlink ref="C141" r:id="rId444" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
+    <hyperlink ref="C140" r:id="rId445" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
+    <hyperlink ref="C139" r:id="rId446" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
+    <hyperlink ref="C138" r:id="rId447" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
     <hyperlink ref="C136" r:id="rId448" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
     <hyperlink ref="C135" r:id="rId449" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
     <hyperlink ref="C134" r:id="rId450" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
@@ -10869,7 +10889,7 @@
     <hyperlink ref="K113" r:id="rId481" xr:uid="{4ABCF4E2-1F23-4DEC-B83E-6F25022FECD7}"/>
     <hyperlink ref="K112" r:id="rId482" xr:uid="{A2E21C54-125D-4835-97AC-B66CAC68024E}"/>
     <hyperlink ref="K133" r:id="rId483" xr:uid="{A2CD53AF-BF86-4A7D-9093-4B270E99140E}"/>
-    <hyperlink ref="K177" r:id="rId484" xr:uid="{1489298F-8F89-45A4-82C2-FF07F9E1E9CD}"/>
+    <hyperlink ref="K178" r:id="rId484" xr:uid="{1489298F-8F89-45A4-82C2-FF07F9E1E9CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId485"/>

</xml_diff>

<commit_message>
Doing Singly Linked List Again
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Java\Java-DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\JavaDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AA9D2B-046C-414E-82A4-77C744880B84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47595748-0C5C-48E8-B8FD-C495C2265ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="579">
   <si>
     <t>Topic:</t>
   </si>
@@ -1759,6 +1759,9 @@
   </si>
   <si>
     <t>ISLL7LL</t>
+  </si>
+  <si>
+    <t>IDLL7LL</t>
   </si>
 </sst>
 </file>
@@ -2324,7 +2327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:M514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
@@ -5916,7 +5919,9 @@
       <c r="A177" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B177" s="26"/>
+      <c r="B177" s="26" t="s">
+        <v>578</v>
+      </c>
       <c r="C177" s="5" t="s">
         <v>575</v>
       </c>

</xml_diff>

<commit_message>
Doubly Linked List Added With deletion,Insertion
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\JavaDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47595748-0C5C-48E8-B8FD-C495C2265ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B9C1CF-2B34-4357-A82B-2838F0B1F167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2328,7 +2328,7 @@
   <dimension ref="A1:M514"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+      <selection activeCell="B178" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>

</xml_diff>